<commit_message>
Get daily reddit data: Tue Apr 15 08:12:44 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_04_20.xlsx
+++ b/data/collected_data/2025_04_20.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C301"/>
+  <dimension ref="A1:C507"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5550,6 +5550,3508 @@
         </is>
       </c>
     </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>1jzm1jv</t>
+        </is>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>Just did my nails. Nearly took 3 hours. Lmk what you think (: *sorry for the mess*</t>
+        </is>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jzm1jv</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>1jzj3pe</t>
+        </is>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>Sparkly blue nails</t>
+        </is>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jzj3pe</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>1jzkjxy</t>
+        </is>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>how much would you pay for these?</t>
+        </is>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vxngbb9zuxue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>1jzjv2h</t>
+        </is>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t>Tragedy</t>
+        </is>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rcpcbs6umxue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>1jzicfh</t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>My hyponychium got ripped away</t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jzicfh/my_hyponychium_got_ripped_away/</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>1jzh043</t>
+        </is>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>Ive been using gel nail polish for quite a while now but stopped recently because my nails are sore to touch and look brittle. What causes this? Is it bc of the gel polish?</t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zt5ilp4juwue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>1jzf9od</t>
+        </is>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>Questionable salon hygiene</t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jzf9od/questionable_salon_hygiene/</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>1jzjhio</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>Colourful Series</t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lbtlwihiixue1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>1jzjgus</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>obsesssssed 😍</t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/yzuq19vgixue1</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>1jzirz0</t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>Fav nails I've done recently</t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jzirz0</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>1jzio7w</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>I'm working on a candy themed Easter set, but this chocolate bunny was too cute to not share right away!</t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lgzobvk9axue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>1jzi6np</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>New to doing my own nails</t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f6l3j8lj5xue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>1jzi0a5</t>
+        </is>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>Fav nails I've done recently</t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jzi0a5</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>1jzhnaq</t>
+        </is>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>What do you think on the colour?</t>
+        </is>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gj153ing0xue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>1jzh3a7</t>
+        </is>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>I usually get pink nails but today I’m feeling icy blue. 🩵❄️</t>
+        </is>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y0ue48jbvwue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>1jzgttv</t>
+        </is>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>Sculpted overlay mani on myself</t>
+        </is>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jzgttv</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>1jzg8kx</t>
+        </is>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>So in love with my new set &amp; ready for spring!! 🧈💛✨ butter yellow french chrome</t>
+        </is>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jzg8kx</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>1jzg03x</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>Spring cotton candy nails</t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jzg03x</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>1jzfu8t</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>new to diy press ons</t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jzfu8t</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>1jzfiir</t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>Too much Sparkle?</t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jzfiir</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>1jzfcvk</t>
+        </is>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>french tips🫶🏻</t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jzfcvk</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>1jzfb5r</t>
+        </is>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>at the beginning of April 💧</t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jzfb5r</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>1jzfb51</t>
+        </is>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>DIY finish</t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jzfb51/diy_finish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>1jzevq6</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>A little pink, a little whimsigoth 🖤💕✨</t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jd3usandbwue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>1jzetrv</t>
+        </is>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>Are my nails too dark??</t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vkhwdbdxawue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>1jzes5l</t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>How can I treat a chip at the base of my nail?</t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jzes5l</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>1jzdpd9</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t>Ok ladies I think I may have a problem lmao💀</t>
+        </is>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jzdpd9/ok_ladies_i_think_i_may_have_a_problem_lmao/</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>1jzd84h</t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>Nude Pink Mani w/ Glitter Accent</t>
+        </is>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jzd84h</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>1jzct7d</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>Easter Nails 🐇</t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jzct7d</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>1jzcsj2</t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>Nail Day!</t>
+        </is>
+      </c>
+      <c r="C331" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t6kdtmjttvue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>1jzch7r</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>thoughts ??</t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jzch7r</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>1jzcdkp</t>
+        </is>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>My first press on set</t>
+        </is>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rfyswpohqvue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>1jzahyp</t>
+        </is>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>Pink for cherry blossom season!</t>
+        </is>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bpbiu9gkbvue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>1jz9v4r</t>
+        </is>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>what's the best? drying spray, drying top coat or drying drops?</t>
+        </is>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jz9v4r/whats_the_best_drying_spray_drying_top_coat_or/</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>1jzc017</t>
+        </is>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t>I think nail tech shaved to far on the sides of my nail?</t>
+        </is>
+      </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jzc017/i_think_nail_tech_shaved_to_far_on_the_sides_of/</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>1jzcbjo</t>
+        </is>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t>Spring/Easter Nails</t>
+        </is>
+      </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v6pzbhj1qvue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>1jzbv3q</t>
+        </is>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>Spring nails</t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mmjno7udmvue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>1jzb41r</t>
+        </is>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t>Possibly my fav nails I’ve ever had</t>
+        </is>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mpgtn1gfgvue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>1jzb2l6</t>
+        </is>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>Did my friend’s nails for the first time</t>
+        </is>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bqxavom3gvue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
+          <t>1jzas2o</t>
+        </is>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t>Realized the last post was blurry AF</t>
+        </is>
+      </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yotki2sqdvue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>1jza1zd</t>
+        </is>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t>Nails Did 😳😳😳</t>
+        </is>
+      </c>
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jza1zd</t>
+        </is>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>1jz9yuw</t>
+        </is>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t>My Birthday Nails🩵 Hello kitty and milk and this cake took me 13 hours JUST THE CAKE HAHA but it was so worth it🩵</t>
+        </is>
+      </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jz9yuw</t>
+        </is>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>1jz9umo</t>
+        </is>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t>Do you like your natural nails to grow long?</t>
+        </is>
+      </c>
+      <c r="C344" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ytqtc3gl6vue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr">
+        <is>
+          <t>1jz8eyr</t>
+        </is>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t>How can I get thick healthy nails without gel / acrylic?</t>
+        </is>
+      </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jz8eyr/how_can_i_get_thick_healthy_nails_without_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="inlineStr">
+        <is>
+          <t>1jz8psz</t>
+        </is>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t>Wanted something simple and dainty looking 💅</t>
+        </is>
+      </c>
+      <c r="C346" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0mpn0pleyuue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr">
+        <is>
+          <t>1jz8mb3</t>
+        </is>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t>DIY</t>
+        </is>
+      </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qtguqf0qxuue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="inlineStr">
+        <is>
+          <t>1jz8jip</t>
+        </is>
+      </c>
+      <c r="B348" t="inlineStr">
+        <is>
+          <t>Lavender opal nails</t>
+        </is>
+      </c>
+      <c r="C348" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oj4o04x1xuue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="inlineStr">
+        <is>
+          <t>1jz88zh</t>
+        </is>
+      </c>
+      <c r="B349" t="inlineStr">
+        <is>
+          <t>Cherry blossom</t>
+        </is>
+      </c>
+      <c r="C349" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jz88zh</t>
+        </is>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="inlineStr">
+        <is>
+          <t>1jz88jc</t>
+        </is>
+      </c>
+      <c r="B350" t="inlineStr">
+        <is>
+          <t>Latest set 💅🏻</t>
+        </is>
+      </c>
+      <c r="C350" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2q1mi462vuue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="inlineStr">
+        <is>
+          <t>1jz7e5t</t>
+        </is>
+      </c>
+      <c r="B351" t="inlineStr">
+        <is>
+          <t>Milky pink polish</t>
+        </is>
+      </c>
+      <c r="C351" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jz7e5t/milky_pink_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="inlineStr">
+        <is>
+          <t>1jz7zhq</t>
+        </is>
+      </c>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t>Is this a yay or nay? I had asked for stiletto shaped</t>
+        </is>
+      </c>
+      <c r="C352" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/76idjzg8tuue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="inlineStr">
+        <is>
+          <t>1jz7v3j</t>
+        </is>
+      </c>
+      <c r="B353" t="inlineStr">
+        <is>
+          <t>Self taught</t>
+        </is>
+      </c>
+      <c r="C353" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n9swersbsuue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="inlineStr">
+        <is>
+          <t>1jz7o0l</t>
+        </is>
+      </c>
+      <c r="B354" t="inlineStr">
+        <is>
+          <t>How to remove the curve from the nail beds?</t>
+        </is>
+      </c>
+      <c r="C354" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jz7o0l</t>
+        </is>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="inlineStr">
+        <is>
+          <t>1jz7nm5</t>
+        </is>
+      </c>
+      <c r="B355" t="inlineStr">
+        <is>
+          <t>Latest Set</t>
+        </is>
+      </c>
+      <c r="C355" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jz7nm5</t>
+        </is>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="inlineStr">
+        <is>
+          <t>1jz7neb</t>
+        </is>
+      </c>
+      <c r="B356" t="inlineStr">
+        <is>
+          <t>I never get tired of pink 🩷</t>
+        </is>
+      </c>
+      <c r="C356" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q55ey5isquue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="inlineStr">
+        <is>
+          <t>1jz7jsy</t>
+        </is>
+      </c>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t>I just bought a magnet for cat eye nail polish. Is it strong enough?</t>
+        </is>
+      </c>
+      <c r="C357" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/5smw7if1quue1</t>
+        </is>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="inlineStr">
+        <is>
+          <t>1jz7ee7</t>
+        </is>
+      </c>
+      <c r="B358" t="inlineStr">
+        <is>
+          <t>Press on nail glue</t>
+        </is>
+      </c>
+      <c r="C358" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jz7ee7/press_on_nail_glue/</t>
+        </is>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="inlineStr">
+        <is>
+          <t>1jz77f1</t>
+        </is>
+      </c>
+      <c r="B359" t="inlineStr">
+        <is>
+          <t>Does stuff work?</t>
+        </is>
+      </c>
+      <c r="C359" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cv0vtl4lnuue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="inlineStr">
+        <is>
+          <t>1jz6yym</t>
+        </is>
+      </c>
+      <c r="B360" t="inlineStr">
+        <is>
+          <t>Thinking to switch to DIY nails - will I have to trim the cuticles?</t>
+        </is>
+      </c>
+      <c r="C360" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6702y2ayluue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="inlineStr">
+        <is>
+          <t>1jz6xf8</t>
+        </is>
+      </c>
+      <c r="B361" t="inlineStr">
+        <is>
+          <t>Obsessed</t>
+        </is>
+      </c>
+      <c r="C361" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jz6xf8</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="inlineStr">
+        <is>
+          <t>1jz6m28</t>
+        </is>
+      </c>
+      <c r="B362" t="inlineStr">
+        <is>
+          <t>I’ve been going to my tech for nearly 3 years. I’ve had a few I didn’t love recently but this one really bothers me. The glue on the gems seems sloppy. Am I wrong? Should I go back when I have time later this week and ask her to fix it, or find someone new?</t>
+        </is>
+      </c>
+      <c r="C362" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7y91whpfjuue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="inlineStr">
+        <is>
+          <t>1jz6km5</t>
+        </is>
+      </c>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t>Easter egg nails</t>
+        </is>
+      </c>
+      <c r="C363" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/omwl8rr5juue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="inlineStr">
+        <is>
+          <t>1jz6iis</t>
+        </is>
+      </c>
+      <c r="B364" t="inlineStr">
+        <is>
+          <t>How about the color contrast and my skin?</t>
+        </is>
+      </c>
+      <c r="C364" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bdxxjq2siuue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="inlineStr">
+        <is>
+          <t>1jz6808</t>
+        </is>
+      </c>
+      <c r="B365" t="inlineStr">
+        <is>
+          <t>Blue Gingham Nails!</t>
+        </is>
+      </c>
+      <c r="C365" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v7kfsdosguue1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="inlineStr">
+        <is>
+          <t>1jz5z79</t>
+        </is>
+      </c>
+      <c r="B366" t="inlineStr">
+        <is>
+          <t>First time trying ombre and i’m in love!</t>
+        </is>
+      </c>
+      <c r="C366" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/md3ka2ryeuue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="inlineStr">
+        <is>
+          <t>1jz5j44</t>
+        </is>
+      </c>
+      <c r="B367" t="inlineStr">
+        <is>
+          <t>Will my nails ever go back to normal?</t>
+        </is>
+      </c>
+      <c r="C367" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/epqazxqubuue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="inlineStr">
+        <is>
+          <t>1jz5jst</t>
+        </is>
+      </c>
+      <c r="B368" t="inlineStr">
+        <is>
+          <t>What are some good gel polish brands?</t>
+        </is>
+      </c>
+      <c r="C368" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jz5jst/what_are_some_good_gel_polish_brands/</t>
+        </is>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="inlineStr">
+        <is>
+          <t>1jz3vdv</t>
+        </is>
+      </c>
+      <c r="B369" t="inlineStr">
+        <is>
+          <t>I’ve been filing my sidewalls for years - looking for advice on how to grow them out!</t>
+        </is>
+      </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jz3vdv/ive_been_filing_my_sidewalls_for_years_looking/</t>
+        </is>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="inlineStr">
+        <is>
+          <t>1jz56i3</t>
+        </is>
+      </c>
+      <c r="B370" t="inlineStr">
+        <is>
+          <t>Got a lil experimental...</t>
+        </is>
+      </c>
+      <c r="C370" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wrx3wfzd9uue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="inlineStr">
+        <is>
+          <t>1jz4ld6</t>
+        </is>
+      </c>
+      <c r="B371" t="inlineStr">
+        <is>
+          <t>I am once again showing you my basic nails that i get done the same way too often</t>
+        </is>
+      </c>
+      <c r="C371" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jz4ld6</t>
+        </is>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="inlineStr">
+        <is>
+          <t>1jz4ka6</t>
+        </is>
+      </c>
+      <c r="B372" t="inlineStr">
+        <is>
+          <t>Okay I think I love these 🥰</t>
+        </is>
+      </c>
+      <c r="C372" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jz4ka6</t>
+        </is>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="inlineStr">
+        <is>
+          <t>1jz4c7r</t>
+        </is>
+      </c>
+      <c r="B373" t="inlineStr">
+        <is>
+          <t>Just got my nails done for the holidays</t>
+        </is>
+      </c>
+      <c r="C373" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jz4c7r</t>
+        </is>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="inlineStr">
+        <is>
+          <t>1jz4bs4</t>
+        </is>
+      </c>
+      <c r="B374" t="inlineStr">
+        <is>
+          <t>fresh hard gel shorties 😍</t>
+        </is>
+      </c>
+      <c r="C374" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jz4bs4</t>
+        </is>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="inlineStr">
+        <is>
+          <t>1jz44ob</t>
+        </is>
+      </c>
+      <c r="B375" t="inlineStr">
+        <is>
+          <t>Beginner doing my own nails</t>
+        </is>
+      </c>
+      <c r="C375" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/az5v4eip1uue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="inlineStr">
+        <is>
+          <t>1jz3xwb</t>
+        </is>
+      </c>
+      <c r="B376" t="inlineStr">
+        <is>
+          <t>I'd like to make a model of the same type</t>
+        </is>
+      </c>
+      <c r="C376" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dqqli9550uue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="inlineStr">
+        <is>
+          <t>1jz3xvt</t>
+        </is>
+      </c>
+      <c r="B377" t="inlineStr">
+        <is>
+          <t>Are my nails ok?</t>
+        </is>
+      </c>
+      <c r="C377" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jz3xvt</t>
+        </is>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="inlineStr">
+        <is>
+          <t>1jz3cu2</t>
+        </is>
+      </c>
+      <c r="B378" t="inlineStr">
+        <is>
+          <t>Blue and grey.</t>
+        </is>
+      </c>
+      <c r="C378" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gf660uuzvtue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="inlineStr">
+        <is>
+          <t>1jz3bsx</t>
+        </is>
+      </c>
+      <c r="B379" t="inlineStr">
+        <is>
+          <t>This weeks set 💅</t>
+        </is>
+      </c>
+      <c r="C379" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i6gf1uyuvtue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="inlineStr">
+        <is>
+          <t>1jz3a78</t>
+        </is>
+      </c>
+      <c r="B380" t="inlineStr">
+        <is>
+          <t>Love this color 🦋💙</t>
+        </is>
+      </c>
+      <c r="C380" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ns70ckmivtue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="inlineStr">
+        <is>
+          <t>1jz2ygo</t>
+        </is>
+      </c>
+      <c r="B381" t="inlineStr">
+        <is>
+          <t>Spring has finally arrived</t>
+        </is>
+      </c>
+      <c r="C381" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/40te3me5ttue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="inlineStr">
+        <is>
+          <t>1jz25vz</t>
+        </is>
+      </c>
+      <c r="B382" t="inlineStr">
+        <is>
+          <t>Fat bunny's</t>
+        </is>
+      </c>
+      <c r="C382" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kjfy5x6entue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="inlineStr">
+        <is>
+          <t>1jz287l</t>
+        </is>
+      </c>
+      <c r="B383" t="inlineStr">
+        <is>
+          <t>What should I be expecting for nail salon hygiene and cleanliness?</t>
+        </is>
+      </c>
+      <c r="C383" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jz287l/what_should_i_be_expecting_for_nail_salon_hygiene/</t>
+        </is>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="inlineStr">
+        <is>
+          <t>1jz277a</t>
+        </is>
+      </c>
+      <c r="B384" t="inlineStr">
+        <is>
+          <t>mini and red</t>
+        </is>
+      </c>
+      <c r="C384" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c0qxv7mnntue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="inlineStr">
+        <is>
+          <t>1jz21j7</t>
+        </is>
+      </c>
+      <c r="B385" t="inlineStr">
+        <is>
+          <t>Made my first press on set 🩷</t>
+        </is>
+      </c>
+      <c r="C385" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jz21j7</t>
+        </is>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="inlineStr">
+        <is>
+          <t>1jz1nc3</t>
+        </is>
+      </c>
+      <c r="B386" t="inlineStr">
+        <is>
+          <t>I’m a boy but obsessed with getting my nails done too. Thought I’d share these!</t>
+        </is>
+      </c>
+      <c r="C386" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jz1nc3</t>
+        </is>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="inlineStr">
+        <is>
+          <t>1jz1l5e</t>
+        </is>
+      </c>
+      <c r="B387" t="inlineStr">
+        <is>
+          <t>Gloomy bear set!</t>
+        </is>
+      </c>
+      <c r="C387" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jz1l5e</t>
+        </is>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="inlineStr">
+        <is>
+          <t>1jz1foc</t>
+        </is>
+      </c>
+      <c r="B388" t="inlineStr">
+        <is>
+          <t>Hard to beat the classic black stiletto.</t>
+        </is>
+      </c>
+      <c r="C388" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/41z0vxt2itue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="inlineStr">
+        <is>
+          <t>1jz14bp</t>
+        </is>
+      </c>
+      <c r="B389" t="inlineStr">
+        <is>
+          <t>Cuticle/non-polish Manicure Expectations</t>
+        </is>
+      </c>
+      <c r="C389" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nny2j45rftue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="inlineStr">
+        <is>
+          <t>1jz171v</t>
+        </is>
+      </c>
+      <c r="B390" t="inlineStr">
+        <is>
+          <t>The reference vs the results 💖</t>
+        </is>
+      </c>
+      <c r="C390" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jz171v</t>
+        </is>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="inlineStr">
+        <is>
+          <t>1jz0g05</t>
+        </is>
+      </c>
+      <c r="B391" t="inlineStr">
+        <is>
+          <t>Is this bad?</t>
+        </is>
+      </c>
+      <c r="C391" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jz0g05</t>
+        </is>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="inlineStr">
+        <is>
+          <t>1jz0rvv</t>
+        </is>
+      </c>
+      <c r="B392" t="inlineStr">
+        <is>
+          <t>An unusual color for me but fell in love with the result. 🩶</t>
+        </is>
+      </c>
+      <c r="C392" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jz0rvv</t>
+        </is>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="inlineStr">
+        <is>
+          <t>1jz0i3t</t>
+        </is>
+      </c>
+      <c r="B393" t="inlineStr">
+        <is>
+          <t>Advice Needed - Applying &amp; Removing Press Ons</t>
+        </is>
+      </c>
+      <c r="C393" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jz0i3t/advice_needed_applying_removing_press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="inlineStr">
+        <is>
+          <t>1jz0dxc</t>
+        </is>
+      </c>
+      <c r="B394" t="inlineStr">
+        <is>
+          <t>Can I get jelly nails done on my natural nails?</t>
+        </is>
+      </c>
+      <c r="C394" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jz0dxc/can_i_get_jelly_nails_done_on_my_natural_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="inlineStr">
+        <is>
+          <t>1jyqosv</t>
+        </is>
+      </c>
+      <c r="B395" t="inlineStr">
+        <is>
+          <t>literally why does this happen</t>
+        </is>
+      </c>
+      <c r="C395" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jyqosv</t>
+        </is>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="inlineStr">
+        <is>
+          <t>1jyzhh9</t>
+        </is>
+      </c>
+      <c r="B396" t="inlineStr">
+        <is>
+          <t>Did them myself 🍒🍷</t>
+        </is>
+      </c>
+      <c r="C396" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jyzhh9</t>
+        </is>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="inlineStr">
+        <is>
+          <t>1jyx425</t>
+        </is>
+      </c>
+      <c r="B397" t="inlineStr">
+        <is>
+          <t>Where do you order your gel? Gems? Colors?</t>
+        </is>
+      </c>
+      <c r="C397" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jyx425/where_do_you_order_your_gel_gems_colors/</t>
+        </is>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="inlineStr">
+        <is>
+          <t>1jywewc</t>
+        </is>
+      </c>
+      <c r="B398" t="inlineStr">
+        <is>
+          <t>What I asked for vs got</t>
+        </is>
+      </c>
+      <c r="C398" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jywewc</t>
+        </is>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="inlineStr">
+        <is>
+          <t>1jywp3b</t>
+        </is>
+      </c>
+      <c r="B399" t="inlineStr">
+        <is>
+          <t>« Anne Boleyn’s revenge » inspired nails</t>
+        </is>
+      </c>
+      <c r="C399" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jywp3b</t>
+        </is>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="inlineStr">
+        <is>
+          <t>1jyy2pt</t>
+        </is>
+      </c>
+      <c r="B400" t="inlineStr">
+        <is>
+          <t>Needed to share my natural growth before filing them down 🩷</t>
+        </is>
+      </c>
+      <c r="C400" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jyy2pt</t>
+        </is>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="inlineStr">
+        <is>
+          <t>1jyzb8s</t>
+        </is>
+      </c>
+      <c r="B401" t="inlineStr">
+        <is>
+          <t>Pink french nails still in?</t>
+        </is>
+      </c>
+      <c r="C401" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c4u6svu02tue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="inlineStr">
+        <is>
+          <t>1jzlmde</t>
+        </is>
+      </c>
+      <c r="B402" t="inlineStr">
+        <is>
+          <t>ISO Holo Taco’s I’m Over Brew and Mooncat’s From the Ashes in the same light</t>
+        </is>
+      </c>
+      <c r="C402" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jzlmde/iso_holo_tacos_im_over_brew_and_mooncats_from_the/</t>
+        </is>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="inlineStr">
+        <is>
+          <t>1jzlhif</t>
+        </is>
+      </c>
+      <c r="B403" t="inlineStr">
+        <is>
+          <t>Cracked ‘murk murk’ from HHC</t>
+        </is>
+      </c>
+      <c r="C403" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/za4a2y476yue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="inlineStr">
+        <is>
+          <t>1jzl5hz</t>
+        </is>
+      </c>
+      <c r="B404" t="inlineStr">
+        <is>
+          <t>Improper use my acetone dried out my nails, how do I recover?</t>
+        </is>
+      </c>
+      <c r="C404" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jzl5hz/improper_use_my_acetone_dried_out_my_nails_how_do/</t>
+        </is>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="inlineStr">
+        <is>
+          <t>1jzirzr</t>
+        </is>
+      </c>
+      <c r="B405" t="inlineStr">
+        <is>
+          <t>help! swapping barbie beads or merkitten</t>
+        </is>
+      </c>
+      <c r="C405" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jzirzr</t>
+        </is>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="inlineStr">
+        <is>
+          <t>1jzioms</t>
+        </is>
+      </c>
+      <c r="B406" t="inlineStr">
+        <is>
+          <t>ISO a polish that looks like this</t>
+        </is>
+      </c>
+      <c r="C406" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p2s2istdaxue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" t="inlineStr">
+        <is>
+          <t>1jzi42u</t>
+        </is>
+      </c>
+      <c r="B407" t="inlineStr">
+        <is>
+          <t>A Few Sub Updates 📫</t>
+        </is>
+      </c>
+      <c r="C407" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jzi42u/a_few_sub_updates/</t>
+        </is>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" t="inlineStr">
+        <is>
+          <t>1jzi2zx</t>
+        </is>
+      </c>
+      <c r="B408" t="inlineStr">
+        <is>
+          <t>{PR} Exxxpose by Sassy Sauce</t>
+        </is>
+      </c>
+      <c r="C408" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jzi2zx</t>
+        </is>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" t="inlineStr">
+        <is>
+          <t>1jzhwyo</t>
+        </is>
+      </c>
+      <c r="B409" t="inlineStr">
+        <is>
+          <t>{PR} Sassy Sauce | HHC - There’s No Place Like Hangin’ with My Homies</t>
+        </is>
+      </c>
+      <c r="C409" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jzhwyo</t>
+        </is>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" t="inlineStr">
+        <is>
+          <t>1jzhu3o</t>
+        </is>
+      </c>
+      <c r="B410" t="inlineStr">
+        <is>
+          <t>{PR} Sassy Sauce | HHC - Pop.yew.lar</t>
+        </is>
+      </c>
+      <c r="C410" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jzhu3o</t>
+        </is>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" t="inlineStr">
+        <is>
+          <t>1jzhen9</t>
+        </is>
+      </c>
+      <c r="B411" t="inlineStr">
+        <is>
+          <t>Seeking out the palest of pale greens</t>
+        </is>
+      </c>
+      <c r="C411" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jzhen9/seeking_out_the_palest_of_pale_greens/</t>
+        </is>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" t="inlineStr">
+        <is>
+          <t>1jzhdo8</t>
+        </is>
+      </c>
+      <c r="B412" t="inlineStr">
+        <is>
+          <t>After the Rain, Sabertooth, or a different brand?</t>
+        </is>
+      </c>
+      <c r="C412" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jzhdo8/after_the_rain_sabertooth_or_a_different_brand/</t>
+        </is>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" t="inlineStr">
+        <is>
+          <t>1jzh5vb</t>
+        </is>
+      </c>
+      <c r="B413" t="inlineStr">
+        <is>
+          <t>🖤💚</t>
+        </is>
+      </c>
+      <c r="C413" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jzh5vb</t>
+        </is>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" t="inlineStr">
+        <is>
+          <t>1jzh1pt</t>
+        </is>
+      </c>
+      <c r="B414" t="inlineStr">
+        <is>
+          <t>My first *successful* “nail art” attempt!🐠🦋🍏</t>
+        </is>
+      </c>
+      <c r="C414" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jzh1pt</t>
+        </is>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" t="inlineStr">
+        <is>
+          <t>1jzgz6c</t>
+        </is>
+      </c>
+      <c r="B415" t="inlineStr">
+        <is>
+          <t>World Champion curlers wear nail polish</t>
+        </is>
+      </c>
+      <c r="C415" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jzgz6c/world_champion_curlers_wear_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" t="inlineStr">
+        <is>
+          <t>1jzg9v6</t>
+        </is>
+      </c>
+      <c r="B416" t="inlineStr">
+        <is>
+          <t>Can y’all help me find a polish similar to Revlon’s “Facets of Fuchsia” but with purple glitter?</t>
+        </is>
+      </c>
+      <c r="C416" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zchc2gyxnwue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" t="inlineStr">
+        <is>
+          <t>1jzfuk9</t>
+        </is>
+      </c>
+      <c r="B417" t="inlineStr">
+        <is>
+          <t>Tariffs to Canada from US</t>
+        </is>
+      </c>
+      <c r="C417" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jzfuk9/tariffs_to_canada_from_us/</t>
+        </is>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" t="inlineStr">
+        <is>
+          <t>1jzfrl3</t>
+        </is>
+      </c>
+      <c r="B418" t="inlineStr">
+        <is>
+          <t>First Mooncat cart help!</t>
+        </is>
+      </c>
+      <c r="C418" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jzfrl3</t>
+        </is>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" t="inlineStr">
+        <is>
+          <t>1jzfhfu</t>
+        </is>
+      </c>
+      <c r="B419" t="inlineStr">
+        <is>
+          <t>You Have Grown So Vast and Boundless</t>
+        </is>
+      </c>
+      <c r="C419" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mohcbygpgwue1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" t="inlineStr">
+        <is>
+          <t>1jzfdza</t>
+        </is>
+      </c>
+      <c r="B420" t="inlineStr">
+        <is>
+          <t>OPI Scorpio Seduction - essential for a blue polish lover 💅</t>
+        </is>
+      </c>
+      <c r="C420" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jzfdza</t>
+        </is>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" t="inlineStr">
+        <is>
+          <t>1jzfdug</t>
+        </is>
+      </c>
+      <c r="B421" t="inlineStr">
+        <is>
+          <t>Went for a night sky themed this week</t>
+        </is>
+      </c>
+      <c r="C421" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jzfdug</t>
+        </is>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" t="inlineStr">
+        <is>
+          <t>1jzf6n2</t>
+        </is>
+      </c>
+      <c r="B422" t="inlineStr">
+        <is>
+          <t>Aussie Autumn Easter Pastel</t>
+        </is>
+      </c>
+      <c r="C422" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/moadke2wdwue1</t>
+        </is>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" t="inlineStr">
+        <is>
+          <t>1jzf5qt</t>
+        </is>
+      </c>
+      <c r="B423" t="inlineStr">
+        <is>
+          <t>Dry drops from dollar tree</t>
+        </is>
+      </c>
+      <c r="C423" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jzf5qt/dry_drops_from_dollar_tree/</t>
+        </is>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" t="inlineStr">
+        <is>
+          <t>1jzf5eq</t>
+        </is>
+      </c>
+      <c r="B424" t="inlineStr">
+        <is>
+          <t>Sassy Sauce Trifecta</t>
+        </is>
+      </c>
+      <c r="C424" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b40uk57sdwue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" t="inlineStr">
+        <is>
+          <t>1jzdfjc</t>
+        </is>
+      </c>
+      <c r="B425" t="inlineStr">
+        <is>
+          <t>Recent LynBDesigns Manis</t>
+        </is>
+      </c>
+      <c r="C425" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jzdfjc</t>
+        </is>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" t="inlineStr">
+        <is>
+          <t>1jzcem6</t>
+        </is>
+      </c>
+      <c r="B426" t="inlineStr">
+        <is>
+          <t>Stunner! 😍💙</t>
+        </is>
+      </c>
+      <c r="C426" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jzcem6</t>
+        </is>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" t="inlineStr">
+        <is>
+          <t>1jzc260</t>
+        </is>
+      </c>
+      <c r="B427" t="inlineStr">
+        <is>
+          <t>ILNP cannonball is sooo sparkly</t>
+        </is>
+      </c>
+      <c r="C427" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7ijejgvxnvue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" t="inlineStr">
+        <is>
+          <t>1jzbquw</t>
+        </is>
+      </c>
+      <c r="B428" t="inlineStr">
+        <is>
+          <t>Chicago Fire or You, of Unshakable Conviction?</t>
+        </is>
+      </c>
+      <c r="C428" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jzbquw</t>
+        </is>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" t="inlineStr">
+        <is>
+          <t>1jzba8j</t>
+        </is>
+      </c>
+      <c r="B429" t="inlineStr">
+        <is>
+          <t>Update: Such A Farce vs Am I Everything You Fear</t>
+        </is>
+      </c>
+      <c r="C429" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jzba8j</t>
+        </is>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" t="inlineStr">
+        <is>
+          <t>1jzavh5</t>
+        </is>
+      </c>
+      <c r="B430" t="inlineStr">
+        <is>
+          <t>Tips for not smearing nail art with top coat?</t>
+        </is>
+      </c>
+      <c r="C430" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jzavh5/tips_for_not_smearing_nail_art_with_top_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" t="inlineStr">
+        <is>
+          <t>1jzatpi</t>
+        </is>
+      </c>
+      <c r="B431" t="inlineStr">
+        <is>
+          <t>Successful magnetic and builder gel!</t>
+        </is>
+      </c>
+      <c r="C431" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jzatpi</t>
+        </is>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" t="inlineStr">
+        <is>
+          <t>1jzaesb</t>
+        </is>
+      </c>
+      <c r="B432" t="inlineStr">
+        <is>
+          <t>First post…. I don’t know what to do with my hands!!!</t>
+        </is>
+      </c>
+      <c r="C432" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/l0h8lwi0avue1</t>
+        </is>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" t="inlineStr">
+        <is>
+          <t>1jzalb4</t>
+        </is>
+      </c>
+      <c r="B433" t="inlineStr">
+        <is>
+          <t>toe beans feat. toe beans 🐈‍⬛</t>
+        </is>
+      </c>
+      <c r="C433" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jza92x</t>
+        </is>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" t="inlineStr">
+        <is>
+          <t>1jzak0w</t>
+        </is>
+      </c>
+      <c r="B434" t="inlineStr">
+        <is>
+          <t>She’s a classic for good reason!</t>
+        </is>
+      </c>
+      <c r="C434" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cok8zblzbvue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" t="inlineStr">
+        <is>
+          <t>1jzagsq</t>
+        </is>
+      </c>
+      <c r="B435" t="inlineStr">
+        <is>
+          <t>Spring Skittle</t>
+        </is>
+      </c>
+      <c r="C435" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9hpv6ndbbvue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" t="inlineStr">
+        <is>
+          <t>1jzagn7</t>
+        </is>
+      </c>
+      <c r="B436" t="inlineStr">
+        <is>
+          <t>Quite Frankly You're My Hero (LynB) vs All The Rage (EdM)?</t>
+        </is>
+      </c>
+      <c r="C436" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jzagn7/quite_frankly_youre_my_hero_lynb_vs_all_the_rage/</t>
+        </is>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" t="inlineStr">
+        <is>
+          <t>1jz9zro</t>
+        </is>
+      </c>
+      <c r="B437" t="inlineStr">
+        <is>
+          <t>Gel overlay 🤍🎀 I was looking for a beautiful nude builder gel and I am absolutely in love with how this one looks on my skin</t>
+        </is>
+      </c>
+      <c r="C437" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jz9zro</t>
+        </is>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" t="inlineStr">
+        <is>
+          <t>1jz9jhw</t>
+        </is>
+      </c>
+      <c r="B438" t="inlineStr">
+        <is>
+          <t>Haven't really seen many UK nails on here, so here's mine!</t>
+        </is>
+      </c>
+      <c r="C438" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jz9jhw</t>
+        </is>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" t="inlineStr">
+        <is>
+          <t>1jz9fb5</t>
+        </is>
+      </c>
+      <c r="B439" t="inlineStr">
+        <is>
+          <t>I can't get over how shiny they are! ❤️</t>
+        </is>
+      </c>
+      <c r="C439" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g78mvnhh3vue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" t="inlineStr">
+        <is>
+          <t>1jz926y</t>
+        </is>
+      </c>
+      <c r="B440" t="inlineStr">
+        <is>
+          <t>My attempt at “soap nails”</t>
+        </is>
+      </c>
+      <c r="C440" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m4i1m8yv0vue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" t="inlineStr">
+        <is>
+          <t>1jz8yno</t>
+        </is>
+      </c>
+      <c r="B441" t="inlineStr">
+        <is>
+          <t>Stocking up😢</t>
+        </is>
+      </c>
+      <c r="C441" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sgsvhiu60vue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" t="inlineStr">
+        <is>
+          <t>1jz8wyh</t>
+        </is>
+      </c>
+      <c r="B442" t="inlineStr">
+        <is>
+          <t>Blueberry Stamp Nails</t>
+        </is>
+      </c>
+      <c r="C442" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jz8wyh</t>
+        </is>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" t="inlineStr">
+        <is>
+          <t>1jz8p6w</t>
+        </is>
+      </c>
+      <c r="B443" t="inlineStr">
+        <is>
+          <t>I've been poisoned🧡😍❤️</t>
+        </is>
+      </c>
+      <c r="C443" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jz8p6w</t>
+        </is>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" t="inlineStr">
+        <is>
+          <t>1jz8fv4</t>
+        </is>
+      </c>
+      <c r="B444" t="inlineStr">
+        <is>
+          <t>New flair for tariffs?</t>
+        </is>
+      </c>
+      <c r="C444" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jz8fv4/new_flair_for_tariffs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" t="inlineStr">
+        <is>
+          <t>1jz6s72</t>
+        </is>
+      </c>
+      <c r="B445" t="inlineStr">
+        <is>
+          <t>finally feels like spring 🩵</t>
+        </is>
+      </c>
+      <c r="C445" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7nmdqoemkuue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" t="inlineStr">
+        <is>
+          <t>1jz6rut</t>
+        </is>
+      </c>
+      <c r="B446" t="inlineStr">
+        <is>
+          <t>Serious staying power.</t>
+        </is>
+      </c>
+      <c r="C446" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t27v9bsjkuue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" t="inlineStr">
+        <is>
+          <t>1jz6oqd</t>
+        </is>
+      </c>
+      <c r="B447" t="inlineStr">
+        <is>
+          <t>Thought I would share my press on nails (on week 2, going strong)!</t>
+        </is>
+      </c>
+      <c r="C447" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jz6oqd</t>
+        </is>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" t="inlineStr">
+        <is>
+          <t>1jz5znf</t>
+        </is>
+      </c>
+      <c r="B448" t="inlineStr">
+        <is>
+          <t>Help with my last ever Mooncat order</t>
+        </is>
+      </c>
+      <c r="C448" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jz5r6i</t>
+        </is>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" t="inlineStr">
+        <is>
+          <t>1jz5aaz</t>
+        </is>
+      </c>
+      <c r="B449" t="inlineStr">
+        <is>
+          <t>I Wanna Dance (A Tragedy)</t>
+        </is>
+      </c>
+      <c r="C449" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jz5aaz</t>
+        </is>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" t="inlineStr">
+        <is>
+          <t>1jz565q</t>
+        </is>
+      </c>
+      <c r="B450" t="inlineStr">
+        <is>
+          <t>Help! I can not keep polish on my nails</t>
+        </is>
+      </c>
+      <c r="C450" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h15hegib9uue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" t="inlineStr">
+        <is>
+          <t>1jz4rdf</t>
+        </is>
+      </c>
+      <c r="B451" t="inlineStr">
+        <is>
+          <t>Smoky lavender with sparkly tips 🪻</t>
+        </is>
+      </c>
+      <c r="C451" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/csna63w35uue1</t>
+        </is>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" t="inlineStr">
+        <is>
+          <t>1jz4pcc</t>
+        </is>
+      </c>
+      <c r="B452" t="inlineStr">
+        <is>
+          <t>Anyone used LynB QDTC &amp; Base Coat?</t>
+        </is>
+      </c>
+      <c r="C452" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jz4pcc/anyone_used_lynb_qdtc_base_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" t="inlineStr">
+        <is>
+          <t>1jz4anw</t>
+        </is>
+      </c>
+      <c r="B453" t="inlineStr">
+        <is>
+          <t>talk me into/out of anything in my cart!</t>
+        </is>
+      </c>
+      <c r="C453" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jz4anw</t>
+        </is>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" t="inlineStr">
+        <is>
+          <t>1jz3tha</t>
+        </is>
+      </c>
+      <c r="B454" t="inlineStr">
+        <is>
+          <t>Looking for a polish I saw on here in the past couple of months…</t>
+        </is>
+      </c>
+      <c r="C454" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jz3tha/looking_for_a_polish_i_saw_on_here_in_the_past/</t>
+        </is>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" t="inlineStr">
+        <is>
+          <t>1jz3q32</t>
+        </is>
+      </c>
+      <c r="B455" t="inlineStr">
+        <is>
+          <t>Sassy Sauce Chicago Fire</t>
+        </is>
+      </c>
+      <c r="C455" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nd1sym1sytue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" t="inlineStr">
+        <is>
+          <t>1jz0f9j</t>
+        </is>
+      </c>
+      <c r="B456" t="inlineStr">
+        <is>
+          <t>Nails are the thinness and texture of those plastic school folders</t>
+        </is>
+      </c>
+      <c r="C456" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jz0f9j/nails_are_the_thinness_and_texture_of_those/</t>
+        </is>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" t="inlineStr">
+        <is>
+          <t>1jz2z7v</t>
+        </is>
+      </c>
+      <c r="B457" t="inlineStr">
+        <is>
+          <t>Color advice? Dazzle Dry</t>
+        </is>
+      </c>
+      <c r="C457" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jz2z7v</t>
+        </is>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" t="inlineStr">
+        <is>
+          <t>1jz2yse</t>
+        </is>
+      </c>
+      <c r="B458" t="inlineStr">
+        <is>
+          <t>When you gotta redo your nail cause cat</t>
+        </is>
+      </c>
+      <c r="C458" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jz2yse</t>
+        </is>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" t="inlineStr">
+        <is>
+          <t>1jz2qyp</t>
+        </is>
+      </c>
+      <c r="B459" t="inlineStr">
+        <is>
+          <t>Surprisingly shifty</t>
+        </is>
+      </c>
+      <c r="C459" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jz2qyp</t>
+        </is>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" t="inlineStr">
+        <is>
+          <t>1jz2pae</t>
+        </is>
+      </c>
+      <c r="B460" t="inlineStr">
+        <is>
+          <t>Essie Aruba Blue is that girl</t>
+        </is>
+      </c>
+      <c r="C460" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0w7st549rtue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" t="inlineStr">
+        <is>
+          <t>1jz29tl</t>
+        </is>
+      </c>
+      <c r="B461" t="inlineStr">
+        <is>
+          <t>Is this too unnoticeable on my skin (Essie Mademoiselle) I was going for milky nails but think I’ve failed</t>
+        </is>
+      </c>
+      <c r="C461" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1s6wxpd6otue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" t="inlineStr">
+        <is>
+          <t>1jz1smy</t>
+        </is>
+      </c>
+      <c r="B462" t="inlineStr">
+        <is>
+          <t>Culture Shock🦠🔬💚🩵💙</t>
+        </is>
+      </c>
+      <c r="C462" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jz1smy</t>
+        </is>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" t="inlineStr">
+        <is>
+          <t>1jz1qhc</t>
+        </is>
+      </c>
+      <c r="B463" t="inlineStr">
+        <is>
+          <t>Fairy water 🧚🏾💧🫧</t>
+        </is>
+      </c>
+      <c r="C463" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jz1qhc</t>
+        </is>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" t="inlineStr">
+        <is>
+          <t>1jz0s5j</t>
+        </is>
+      </c>
+      <c r="B464" t="inlineStr">
+        <is>
+          <t>Oh Mooncats Heavenmetal is STUNNINGGG</t>
+        </is>
+      </c>
+      <c r="C464" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jz0s5j</t>
+        </is>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" t="inlineStr">
+        <is>
+          <t>1jyvp5n</t>
+        </is>
+      </c>
+      <c r="B465" t="inlineStr">
+        <is>
+          <t>To gel or not to gel?</t>
+        </is>
+      </c>
+      <c r="C465" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jyvp5n/to_gel_or_not_to_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" t="inlineStr">
+        <is>
+          <t>1jz0dc6</t>
+        </is>
+      </c>
+      <c r="B466" t="inlineStr">
+        <is>
+          <t>Chrome and Regular Polish</t>
+        </is>
+      </c>
+      <c r="C466" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jz0dc6</t>
+        </is>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" t="inlineStr">
+        <is>
+          <t>1jz0052</t>
+        </is>
+      </c>
+      <c r="B467" t="inlineStr">
+        <is>
+          <t>Mooncat - Alien Invasion 👾</t>
+        </is>
+      </c>
+      <c r="C467" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jz0052</t>
+        </is>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" t="inlineStr">
+        <is>
+          <t>1jyzgxw</t>
+        </is>
+      </c>
+      <c r="B468" t="inlineStr">
+        <is>
+          <t>Mooncat Moving Up Lunar Sale</t>
+        </is>
+      </c>
+      <c r="C468" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jyzgxw</t>
+        </is>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" t="inlineStr">
+        <is>
+          <t>1jyz2e1</t>
+        </is>
+      </c>
+      <c r="B469" t="inlineStr">
+        <is>
+          <t>I call this my Velaris Mani 💅🏼 - ACOTAR inspired</t>
+        </is>
+      </c>
+      <c r="C469" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jyz2e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" t="inlineStr">
+        <is>
+          <t>1jyym06</t>
+        </is>
+      </c>
+      <c r="B470" t="inlineStr">
+        <is>
+          <t>Simplest way to get clear, shiny nails? (I don’t know a thing about nails.)</t>
+        </is>
+      </c>
+      <c r="C470" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jyym06/simplest_way_to_get_clear_shiny_nails_i_dont_know/</t>
+        </is>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" t="inlineStr">
+        <is>
+          <t>1jyyagc</t>
+        </is>
+      </c>
+      <c r="B471" t="inlineStr">
+        <is>
+          <t>💜🌸Wisteria🌸💜</t>
+        </is>
+      </c>
+      <c r="C471" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jyyagc</t>
+        </is>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" t="inlineStr">
+        <is>
+          <t>1jyxdo3</t>
+        </is>
+      </c>
+      <c r="B472" t="inlineStr">
+        <is>
+          <t>Soot Sprites ⭐️</t>
+        </is>
+      </c>
+      <c r="C472" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jyxdo3</t>
+        </is>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" t="inlineStr">
+        <is>
+          <t>1jywyl7</t>
+        </is>
+      </c>
+      <c r="B473" t="inlineStr">
+        <is>
+          <t>Oceanic jelly layering! 🪸</t>
+        </is>
+      </c>
+      <c r="C473" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jywyl7</t>
+        </is>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" t="inlineStr">
+        <is>
+          <t>1jywt5b</t>
+        </is>
+      </c>
+      <c r="B474" t="inlineStr">
+        <is>
+          <t>Best top coat for magnetics?</t>
+        </is>
+      </c>
+      <c r="C474" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9a598kjsfsue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" t="inlineStr">
+        <is>
+          <t>1jywfqo</t>
+        </is>
+      </c>
+      <c r="B475" t="inlineStr">
+        <is>
+          <t>Essie Stones N’ Roses dupe?</t>
+        </is>
+      </c>
+      <c r="C475" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jywfqo/essie_stones_n_roses_dupe/</t>
+        </is>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" t="inlineStr">
+        <is>
+          <t>1jyvg9z</t>
+        </is>
+      </c>
+      <c r="B476" t="inlineStr">
+        <is>
+          <t>One and All</t>
+        </is>
+      </c>
+      <c r="C476" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jyvg9z</t>
+        </is>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" t="inlineStr">
+        <is>
+          <t>1jyv7da</t>
+        </is>
+      </c>
+      <c r="B477" t="inlineStr">
+        <is>
+          <t>No Dumb Questions + Casual Talk</t>
+        </is>
+      </c>
+      <c r="C477" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jyv7da/no_dumb_questions_casual_talk/</t>
+        </is>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" t="inlineStr">
+        <is>
+          <t>1jzkwzj</t>
+        </is>
+      </c>
+      <c r="B478" t="inlineStr">
+        <is>
+          <t>Spring aura nails!</t>
+        </is>
+      </c>
+      <c r="C478" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jzkwzj</t>
+        </is>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" t="inlineStr">
+        <is>
+          <t>1jzagdx</t>
+        </is>
+      </c>
+      <c r="B479" t="inlineStr">
+        <is>
+          <t>How to make chrome powder stay in place?</t>
+        </is>
+      </c>
+      <c r="C479" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/11ik0078bvue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" t="inlineStr">
+        <is>
+          <t>1jzhbsh</t>
+        </is>
+      </c>
+      <c r="B480" t="inlineStr">
+        <is>
+          <t>concert nails</t>
+        </is>
+      </c>
+      <c r="C480" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jzhbsh</t>
+        </is>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" t="inlineStr">
+        <is>
+          <t>1jzgt71</t>
+        </is>
+      </c>
+      <c r="B481" t="inlineStr">
+        <is>
+          <t>my first gel nail art!</t>
+        </is>
+      </c>
+      <c r="C481" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i4b3le6qswue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" t="inlineStr">
+        <is>
+          <t>1jzf0jf</t>
+        </is>
+      </c>
+      <c r="B482" t="inlineStr">
+        <is>
+          <t>Late post back from Christmas.</t>
+        </is>
+      </c>
+      <c r="C482" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jzf0jf</t>
+        </is>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" t="inlineStr">
+        <is>
+          <t>1jzew71</t>
+        </is>
+      </c>
+      <c r="B483" t="inlineStr">
+        <is>
+          <t>Here's a set I did today. I'm not sure I like them</t>
+        </is>
+      </c>
+      <c r="C483" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jzew71</t>
+        </is>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" t="inlineStr">
+        <is>
+          <t>1jze5dg</t>
+        </is>
+      </c>
+      <c r="B484" t="inlineStr">
+        <is>
+          <t>Beauty and the Beast +</t>
+        </is>
+      </c>
+      <c r="C484" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jze5dg</t>
+        </is>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" t="inlineStr">
+        <is>
+          <t>1jzdona</t>
+        </is>
+      </c>
+      <c r="B485" t="inlineStr">
+        <is>
+          <t>Easter egg nail art</t>
+        </is>
+      </c>
+      <c r="C485" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j4lnxl191wue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="486">
+      <c r="A486" t="inlineStr">
+        <is>
+          <t>1jzcjxb</t>
+        </is>
+      </c>
+      <c r="B486" t="inlineStr">
+        <is>
+          <t>Warm Ocean Cosmic Vibes</t>
+        </is>
+      </c>
+      <c r="C486" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jzcjxb</t>
+        </is>
+      </c>
+    </row>
+    <row r="487">
+      <c r="A487" t="inlineStr">
+        <is>
+          <t>1jzc1jb</t>
+        </is>
+      </c>
+      <c r="B487" t="inlineStr">
+        <is>
+          <t>Ready for the beaches 🏖️</t>
+        </is>
+      </c>
+      <c r="C487" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ajt9n2mrnvue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" t="inlineStr">
+        <is>
+          <t>1jzaz86</t>
+        </is>
+      </c>
+      <c r="B488" t="inlineStr">
+        <is>
+          <t>How to make chrome stay in place?</t>
+        </is>
+      </c>
+      <c r="C488" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dhrtn2kcfvue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" t="inlineStr">
+        <is>
+          <t>1jzayhd</t>
+        </is>
+      </c>
+      <c r="B489" t="inlineStr">
+        <is>
+          <t>Gel practice</t>
+        </is>
+      </c>
+      <c r="C489" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jzayhd</t>
+        </is>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" t="inlineStr">
+        <is>
+          <t>1jzayef</t>
+        </is>
+      </c>
+      <c r="B490" t="inlineStr">
+        <is>
+          <t>Look how stunning!</t>
+        </is>
+      </c>
+      <c r="C490" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1xbwth26fvue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" t="inlineStr">
+        <is>
+          <t>1jz9hqt</t>
+        </is>
+      </c>
+      <c r="B491" t="inlineStr">
+        <is>
+          <t>Abejita en las uñas</t>
+        </is>
+      </c>
+      <c r="C491" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l0yt0hdz3vue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" t="inlineStr">
+        <is>
+          <t>1jz82rp</t>
+        </is>
+      </c>
+      <c r="B492" t="inlineStr">
+        <is>
+          <t>Cherry blossom set</t>
+        </is>
+      </c>
+      <c r="C492" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jz82rp</t>
+        </is>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" t="inlineStr">
+        <is>
+          <t>1jz77bk</t>
+        </is>
+      </c>
+      <c r="B493" t="inlineStr">
+        <is>
+          <t>My first ever. 1/10? Be brutally honest</t>
+        </is>
+      </c>
+      <c r="C493" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zas9bsaknuue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" t="inlineStr">
+        <is>
+          <t>1jz6ipg</t>
+        </is>
+      </c>
+      <c r="B494" t="inlineStr">
+        <is>
+          <t>My spring/easter vibe nails</t>
+        </is>
+      </c>
+      <c r="C494" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jz6ipg</t>
+        </is>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" t="inlineStr">
+        <is>
+          <t>1jz48q7</t>
+        </is>
+      </c>
+      <c r="B495" t="inlineStr">
+        <is>
+          <t>Making nails for a homework, gosh I love being in a art program at university</t>
+        </is>
+      </c>
+      <c r="C495" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jz48q7</t>
+        </is>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" t="inlineStr">
+        <is>
+          <t>1jyjo98</t>
+        </is>
+      </c>
+      <c r="B496" t="inlineStr">
+        <is>
+          <t>Nails I've done</t>
+        </is>
+      </c>
+      <c r="C496" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jyjo98</t>
+        </is>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" t="inlineStr">
+        <is>
+          <t>1jyna0r</t>
+        </is>
+      </c>
+      <c r="B497" t="inlineStr">
+        <is>
+          <t>Made a post malone press on nail set inspired by his tatoos</t>
+        </is>
+      </c>
+      <c r="C497" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/d3uxzt1jdpue1</t>
+        </is>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" t="inlineStr">
+        <is>
+          <t>1jywtr0</t>
+        </is>
+      </c>
+      <c r="B498" t="inlineStr">
+        <is>
+          <t>Press on set I made</t>
+        </is>
+      </c>
+      <c r="C498" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/9e2omifzfsue1</t>
+        </is>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" t="inlineStr">
+        <is>
+          <t>1jz1hnw</t>
+        </is>
+      </c>
+      <c r="B499" t="inlineStr">
+        <is>
+          <t>Just posted my first nail art tutorial on YouTube!</t>
+        </is>
+      </c>
+      <c r="C499" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7fd3dm3hitue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" t="inlineStr">
+        <is>
+          <t>1jz1xcv</t>
+        </is>
+      </c>
+      <c r="B500" t="inlineStr">
+        <is>
+          <t>Fruit Nails Remake 🍒</t>
+        </is>
+      </c>
+      <c r="C500" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jz1xcv</t>
+        </is>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" t="inlineStr">
+        <is>
+          <t>1jz1t9t</t>
+        </is>
+      </c>
+      <c r="B501" t="inlineStr">
+        <is>
+          <t>Super mario nails!</t>
+        </is>
+      </c>
+      <c r="C501" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/t5fuu4ztktue1</t>
+        </is>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" t="inlineStr">
+        <is>
+          <t>1jz1bil</t>
+        </is>
+      </c>
+      <c r="B502" t="inlineStr">
+        <is>
+          <t>The reference vs the results 💖</t>
+        </is>
+      </c>
+      <c r="C502" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jz1bil</t>
+        </is>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" t="inlineStr">
+        <is>
+          <t>1jz06kx</t>
+        </is>
+      </c>
+      <c r="B503" t="inlineStr">
+        <is>
+          <t>Today’s work🌷✨</t>
+        </is>
+      </c>
+      <c r="C503" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wgzswdbu8tue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="504">
+      <c r="A504" t="inlineStr">
+        <is>
+          <t>1jz00pg</t>
+        </is>
+      </c>
+      <c r="B504" t="inlineStr">
+        <is>
+          <t>I’m proud!</t>
+        </is>
+      </c>
+      <c r="C504" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3htwynhk7tue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="505">
+      <c r="A505" t="inlineStr">
+        <is>
+          <t>1jyzqcn</t>
+        </is>
+      </c>
+      <c r="B505" t="inlineStr">
+        <is>
+          <t>Newest set 🐍🌙✨</t>
+        </is>
+      </c>
+      <c r="C505" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jyzqcn</t>
+        </is>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" t="inlineStr">
+        <is>
+          <t>1jyw8yo</t>
+        </is>
+      </c>
+      <c r="B506" t="inlineStr">
+        <is>
+          <t>Inspired by Pinterest!</t>
+        </is>
+      </c>
+      <c r="C506" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rqle7xuw9sue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" t="inlineStr">
+        <is>
+          <t>1jyursj</t>
+        </is>
+      </c>
+      <c r="B507" t="inlineStr">
+        <is>
+          <t>Gel paint recs</t>
+        </is>
+      </c>
+      <c r="C507" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1jyursj/gel_paint_recs/</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Wed Apr 16 08:12:05 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_04_20.xlsx
+++ b/data/collected_data/2025_04_20.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C507"/>
+  <dimension ref="A1:C689"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9052,6 +9052,3100 @@
         </is>
       </c>
     </row>
+    <row r="508">
+      <c r="A508" t="inlineStr">
+        <is>
+          <t>1k0evk9</t>
+        </is>
+      </c>
+      <c r="B508" t="inlineStr">
+        <is>
+          <t>I'd take a bullet for my nail tech</t>
+        </is>
+      </c>
+      <c r="C508" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k0evk9</t>
+        </is>
+      </c>
+    </row>
+    <row r="509">
+      <c r="A509" t="inlineStr">
+        <is>
+          <t>1k0esa2</t>
+        </is>
+      </c>
+      <c r="B509" t="inlineStr">
+        <is>
+          <t>First time in 20 years I had changed nail shape</t>
+        </is>
+      </c>
+      <c r="C509" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k0esa2</t>
+        </is>
+      </c>
+    </row>
+    <row r="510">
+      <c r="A510" t="inlineStr">
+        <is>
+          <t>1k0daqj</t>
+        </is>
+      </c>
+      <c r="B510" t="inlineStr">
+        <is>
+          <t>Ingrown</t>
+        </is>
+      </c>
+      <c r="C510" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k0daqj/ingrown/</t>
+        </is>
+      </c>
+    </row>
+    <row r="511">
+      <c r="A511" t="inlineStr">
+        <is>
+          <t>1k08jq1</t>
+        </is>
+      </c>
+      <c r="B511" t="inlineStr">
+        <is>
+          <t>Terrible manicure/pedicure</t>
+        </is>
+      </c>
+      <c r="C511" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k08jq1</t>
+        </is>
+      </c>
+    </row>
+    <row r="512">
+      <c r="A512" t="inlineStr">
+        <is>
+          <t>1k097wu</t>
+        </is>
+      </c>
+      <c r="B512" t="inlineStr">
+        <is>
+          <t>Nails gone wrong</t>
+        </is>
+      </c>
+      <c r="C512" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p13k4db3t3ve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="513">
+      <c r="A513" t="inlineStr">
+        <is>
+          <t>1k0bqs8</t>
+        </is>
+      </c>
+      <c r="B513" t="inlineStr">
+        <is>
+          <t>What’s the best best coat?</t>
+        </is>
+      </c>
+      <c r="C513" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k0bqs8/whats_the_best_best_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="514">
+      <c r="A514" t="inlineStr">
+        <is>
+          <t>1k0c3v3</t>
+        </is>
+      </c>
+      <c r="B514" t="inlineStr">
+        <is>
+          <t>Am I bring too critical?</t>
+        </is>
+      </c>
+      <c r="C514" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k0c3v3</t>
+        </is>
+      </c>
+    </row>
+    <row r="515">
+      <c r="A515" t="inlineStr">
+        <is>
+          <t>1k0bjse</t>
+        </is>
+      </c>
+      <c r="B515" t="inlineStr">
+        <is>
+          <t>Made Them Myself! Cateye</t>
+        </is>
+      </c>
+      <c r="C515" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hr78v75lf4ve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="516">
+      <c r="A516" t="inlineStr">
+        <is>
+          <t>1k0bd05</t>
+        </is>
+      </c>
+      <c r="B516" t="inlineStr">
+        <is>
+          <t>💅💗</t>
+        </is>
+      </c>
+      <c r="C516" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3eyfzd8od4ve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="517">
+      <c r="A517" t="inlineStr">
+        <is>
+          <t>1k0an12</t>
+        </is>
+      </c>
+      <c r="B517" t="inlineStr">
+        <is>
+          <t>Healthy nails</t>
+        </is>
+      </c>
+      <c r="C517" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k0an12/healthy_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="518">
+      <c r="A518" t="inlineStr">
+        <is>
+          <t>1k0ai91</t>
+        </is>
+      </c>
+      <c r="B518" t="inlineStr">
+        <is>
+          <t>New press ons from Ming Original on Etsy ◡̈</t>
+        </is>
+      </c>
+      <c r="C518" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/910i4mv654ve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="519">
+      <c r="A519" t="inlineStr">
+        <is>
+          <t>1k0abep</t>
+        </is>
+      </c>
+      <c r="B519" t="inlineStr">
+        <is>
+          <t>gel x disaster</t>
+        </is>
+      </c>
+      <c r="C519" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k0abep/gel_x_disaster/</t>
+        </is>
+      </c>
+    </row>
+    <row r="520">
+      <c r="A520" t="inlineStr">
+        <is>
+          <t>1k09tsr</t>
+        </is>
+      </c>
+      <c r="B520" t="inlineStr">
+        <is>
+          <t>favorite set to date</t>
+        </is>
+      </c>
+      <c r="C520" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k09tsr</t>
+        </is>
+      </c>
+    </row>
+    <row r="521">
+      <c r="A521" t="inlineStr">
+        <is>
+          <t>1k09tfw</t>
+        </is>
+      </c>
+      <c r="B521" t="inlineStr">
+        <is>
+          <t>todays project</t>
+        </is>
+      </c>
+      <c r="C521" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iuuh2o9py3ve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="522">
+      <c r="A522" t="inlineStr">
+        <is>
+          <t>1k08ssv</t>
+        </is>
+      </c>
+      <c r="B522" t="inlineStr">
+        <is>
+          <t>Dryness</t>
+        </is>
+      </c>
+      <c r="C522" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/li1yk1t4p3ve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="523">
+      <c r="A523" t="inlineStr">
+        <is>
+          <t>1k08rvy</t>
+        </is>
+      </c>
+      <c r="B523" t="inlineStr">
+        <is>
+          <t>Natural Nails - Square</t>
+        </is>
+      </c>
+      <c r="C523" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k08rvy</t>
+        </is>
+      </c>
+    </row>
+    <row r="524">
+      <c r="A524" t="inlineStr">
+        <is>
+          <t>1k08eo5</t>
+        </is>
+      </c>
+      <c r="B524" t="inlineStr">
+        <is>
+          <t>Spring fever!!??</t>
+        </is>
+      </c>
+      <c r="C524" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/55rf456jl3ve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="525">
+      <c r="A525" t="inlineStr">
+        <is>
+          <t>1k089tp</t>
+        </is>
+      </c>
+      <c r="B525" t="inlineStr">
+        <is>
+          <t>💙💅🏼</t>
+        </is>
+      </c>
+      <c r="C525" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k089tp</t>
+        </is>
+      </c>
+    </row>
+    <row r="526">
+      <c r="A526" t="inlineStr">
+        <is>
+          <t>1k05n68</t>
+        </is>
+      </c>
+      <c r="B526" t="inlineStr">
+        <is>
+          <t>My mom's nails today, how do you rate them?</t>
+        </is>
+      </c>
+      <c r="C526" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v6pfby28x2ve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="527">
+      <c r="A527" t="inlineStr">
+        <is>
+          <t>1k065u1</t>
+        </is>
+      </c>
+      <c r="B527" t="inlineStr">
+        <is>
+          <t>Horror story with fake nails</t>
+        </is>
+      </c>
+      <c r="C527" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k065u1/horror_story_with_fake_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="528">
+      <c r="A528" t="inlineStr">
+        <is>
+          <t>1k06wt2</t>
+        </is>
+      </c>
+      <c r="B528" t="inlineStr">
+        <is>
+          <t>Dublin BIAB courses?</t>
+        </is>
+      </c>
+      <c r="C528" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k06wt2/dublin_biab_courses/</t>
+        </is>
+      </c>
+    </row>
+    <row r="529">
+      <c r="A529" t="inlineStr">
+        <is>
+          <t>1k07cma</t>
+        </is>
+      </c>
+      <c r="B529" t="inlineStr">
+        <is>
+          <t>Post gel x nails… help</t>
+        </is>
+      </c>
+      <c r="C529" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k07cma/post_gel_x_nails_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="530">
+      <c r="A530" t="inlineStr">
+        <is>
+          <t>1k07hwp</t>
+        </is>
+      </c>
+      <c r="B530" t="inlineStr">
+        <is>
+          <t>Gel bubbly over base coat?</t>
+        </is>
+      </c>
+      <c r="C530" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/392rx1l6d3ve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="531">
+      <c r="A531" t="inlineStr">
+        <is>
+          <t>1k07x4h</t>
+        </is>
+      </c>
+      <c r="B531" t="inlineStr">
+        <is>
+          <t>First time doing gel-x extensions!</t>
+        </is>
+      </c>
+      <c r="C531" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k07x4h</t>
+        </is>
+      </c>
+    </row>
+    <row r="532">
+      <c r="A532" t="inlineStr">
+        <is>
+          <t>1k07uz4</t>
+        </is>
+      </c>
+      <c r="B532" t="inlineStr">
+        <is>
+          <t>Spring 💅 🍊</t>
+        </is>
+      </c>
+      <c r="C532" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s41oj2dig3ve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="533">
+      <c r="A533" t="inlineStr">
+        <is>
+          <t>1k07mln</t>
+        </is>
+      </c>
+      <c r="B533" t="inlineStr">
+        <is>
+          <t>my new manicure this red french looks good</t>
+        </is>
+      </c>
+      <c r="C533" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aqq4oefae3ve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="534">
+      <c r="A534" t="inlineStr">
+        <is>
+          <t>1k07hhh</t>
+        </is>
+      </c>
+      <c r="B534" t="inlineStr">
+        <is>
+          <t>I braid hair, will getting gel nails fade away while braiding hair?</t>
+        </is>
+      </c>
+      <c r="C534" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k07hhh/i_braid_hair_will_getting_gel_nails_fade_away/</t>
+        </is>
+      </c>
+    </row>
+    <row r="535">
+      <c r="A535" t="inlineStr">
+        <is>
+          <t>1k07gnu</t>
+        </is>
+      </c>
+      <c r="B535" t="inlineStr">
+        <is>
+          <t>Y/n?</t>
+        </is>
+      </c>
+      <c r="C535" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k07gnu</t>
+        </is>
+      </c>
+    </row>
+    <row r="536">
+      <c r="A536" t="inlineStr">
+        <is>
+          <t>1k07bkf</t>
+        </is>
+      </c>
+      <c r="B536" t="inlineStr">
+        <is>
+          <t>5 months strong in my natural nail journey🫶🏼</t>
+        </is>
+      </c>
+      <c r="C536" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eojk4bokb3ve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="537">
+      <c r="A537" t="inlineStr">
+        <is>
+          <t>1k07ask</t>
+        </is>
+      </c>
+      <c r="B537" t="inlineStr">
+        <is>
+          <t>Winter nails</t>
+        </is>
+      </c>
+      <c r="C537" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k07ask</t>
+        </is>
+      </c>
+    </row>
+    <row r="538">
+      <c r="A538" t="inlineStr">
+        <is>
+          <t>1k079xn</t>
+        </is>
+      </c>
+      <c r="B538" t="inlineStr">
+        <is>
+          <t>Nail art stickers</t>
+        </is>
+      </c>
+      <c r="C538" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k079xn</t>
+        </is>
+      </c>
+    </row>
+    <row r="539">
+      <c r="A539" t="inlineStr">
+        <is>
+          <t>1k071y2</t>
+        </is>
+      </c>
+      <c r="B539" t="inlineStr">
+        <is>
+          <t>Getting a bit better at the prep part.</t>
+        </is>
+      </c>
+      <c r="C539" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b247pf8693ve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="540">
+      <c r="A540" t="inlineStr">
+        <is>
+          <t>1k06m55</t>
+        </is>
+      </c>
+      <c r="B540" t="inlineStr">
+        <is>
+          <t>My 3rd set EVER and I’m 68 yrs. old.</t>
+        </is>
+      </c>
+      <c r="C540" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5y3dulff53ve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="541">
+      <c r="A541" t="inlineStr">
+        <is>
+          <t>1k06l24</t>
+        </is>
+      </c>
+      <c r="B541" t="inlineStr">
+        <is>
+          <t>please help 😭</t>
+        </is>
+      </c>
+      <c r="C541" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g4wsd1d653ve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="542">
+      <c r="A542" t="inlineStr">
+        <is>
+          <t>1k06d6r</t>
+        </is>
+      </c>
+      <c r="B542" t="inlineStr">
+        <is>
+          <t>teaching myself how to do gel x</t>
+        </is>
+      </c>
+      <c r="C542" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/msz4lf8a33ve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="543">
+      <c r="A543" t="inlineStr">
+        <is>
+          <t>1k063oq</t>
+        </is>
+      </c>
+      <c r="B543" t="inlineStr">
+        <is>
+          <t>My new nails raised my mood☺️💅🏻</t>
+        </is>
+      </c>
+      <c r="C543" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k063oq</t>
+        </is>
+      </c>
+    </row>
+    <row r="544">
+      <c r="A544" t="inlineStr">
+        <is>
+          <t>1k05xhh</t>
+        </is>
+      </c>
+      <c r="B544" t="inlineStr">
+        <is>
+          <t>Summertime chrome</t>
+        </is>
+      </c>
+      <c r="C544" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k05xhh</t>
+        </is>
+      </c>
+    </row>
+    <row r="545">
+      <c r="A545" t="inlineStr">
+        <is>
+          <t>1k05kcj</t>
+        </is>
+      </c>
+      <c r="B545" t="inlineStr">
+        <is>
+          <t>🍋💙</t>
+        </is>
+      </c>
+      <c r="C545" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vwicwzrjw2ve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="546">
+      <c r="A546" t="inlineStr">
+        <is>
+          <t>1k058jl</t>
+        </is>
+      </c>
+      <c r="B546" t="inlineStr">
+        <is>
+          <t>How to fix my not so great toenails?</t>
+        </is>
+      </c>
+      <c r="C546" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k058jl</t>
+        </is>
+      </c>
+    </row>
+    <row r="547">
+      <c r="A547" t="inlineStr">
+        <is>
+          <t>1k054e2</t>
+        </is>
+      </c>
+      <c r="B547" t="inlineStr">
+        <is>
+          <t>what do we think?</t>
+        </is>
+      </c>
+      <c r="C547" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p39l2u2xs2ve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="548">
+      <c r="A548" t="inlineStr">
+        <is>
+          <t>1k050hq</t>
+        </is>
+      </c>
+      <c r="B548" t="inlineStr">
+        <is>
+          <t>Went with a fire &amp; ice theme for this set</t>
+        </is>
+      </c>
+      <c r="C548" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vzz8qde0s2ve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="549">
+      <c r="A549" t="inlineStr">
+        <is>
+          <t>1k04i9z</t>
+        </is>
+      </c>
+      <c r="B549" t="inlineStr">
+        <is>
+          <t>Color inspo was the toe beans</t>
+        </is>
+      </c>
+      <c r="C549" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bajqnl8yn2ve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="550">
+      <c r="A550" t="inlineStr">
+        <is>
+          <t>1k04rjz</t>
+        </is>
+      </c>
+      <c r="B550" t="inlineStr">
+        <is>
+          <t>First post!  Love my nail girl🌟🌺</t>
+        </is>
+      </c>
+      <c r="C550" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k04rjz</t>
+        </is>
+      </c>
+    </row>
+    <row r="551">
+      <c r="A551" t="inlineStr">
+        <is>
+          <t>1k04qbf</t>
+        </is>
+      </c>
+      <c r="B551" t="inlineStr">
+        <is>
+          <t>Bf paid for these 💅</t>
+        </is>
+      </c>
+      <c r="C551" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lze47kjpp2ve1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="552">
+      <c r="A552" t="inlineStr">
+        <is>
+          <t>1k04jxd</t>
+        </is>
+      </c>
+      <c r="B552" t="inlineStr">
+        <is>
+          <t>Help :(</t>
+        </is>
+      </c>
+      <c r="C552" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k04jxd</t>
+        </is>
+      </c>
+    </row>
+    <row r="553">
+      <c r="A553" t="inlineStr">
+        <is>
+          <t>1k04e1c</t>
+        </is>
+      </c>
+      <c r="B553" t="inlineStr">
+        <is>
+          <t>Client come back 3 times to complain</t>
+        </is>
+      </c>
+      <c r="C553" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k04e1c/client_come_back_3_times_to_complain/</t>
+        </is>
+      </c>
+    </row>
+    <row r="554">
+      <c r="A554" t="inlineStr">
+        <is>
+          <t>1k049n0</t>
+        </is>
+      </c>
+      <c r="B554" t="inlineStr">
+        <is>
+          <t>Confirm if we have all at some point in our lives become pink fans 💓</t>
+        </is>
+      </c>
+      <c r="C554" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k049n0</t>
+        </is>
+      </c>
+    </row>
+    <row r="555">
+      <c r="A555" t="inlineStr">
+        <is>
+          <t>1k03zom</t>
+        </is>
+      </c>
+      <c r="B555" t="inlineStr">
+        <is>
+          <t>This isn’t almond, is it?</t>
+        </is>
+      </c>
+      <c r="C555" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k03zom</t>
+        </is>
+      </c>
+    </row>
+    <row r="556">
+      <c r="A556" t="inlineStr">
+        <is>
+          <t>1k03etc</t>
+        </is>
+      </c>
+      <c r="B556" t="inlineStr">
+        <is>
+          <t>Pretty little spring set🌸</t>
+        </is>
+      </c>
+      <c r="C556" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/77o6vdmdf2ve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="557">
+      <c r="A557" t="inlineStr">
+        <is>
+          <t>1k03awv</t>
+        </is>
+      </c>
+      <c r="B557" t="inlineStr">
+        <is>
+          <t>Spring Fruit</t>
+        </is>
+      </c>
+      <c r="C557" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k03awv</t>
+        </is>
+      </c>
+    </row>
+    <row r="558">
+      <c r="A558" t="inlineStr">
+        <is>
+          <t>1k036zx</t>
+        </is>
+      </c>
+      <c r="B558" t="inlineStr">
+        <is>
+          <t>Birthday nails 💜🦋</t>
+        </is>
+      </c>
+      <c r="C558" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6o0m120qd2ve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="559">
+      <c r="A559" t="inlineStr">
+        <is>
+          <t>1k030em</t>
+        </is>
+      </c>
+      <c r="B559" t="inlineStr">
+        <is>
+          <t>First time getting my nails done!</t>
+        </is>
+      </c>
+      <c r="C559" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bwxvdxbbc2ve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="560">
+      <c r="A560" t="inlineStr">
+        <is>
+          <t>1k02gsq</t>
+        </is>
+      </c>
+      <c r="B560" t="inlineStr">
+        <is>
+          <t>Long time lurker but First time poster :</t>
+        </is>
+      </c>
+      <c r="C560" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k02gsq</t>
+        </is>
+      </c>
+    </row>
+    <row r="561">
+      <c r="A561" t="inlineStr">
+        <is>
+          <t>1k01v6x</t>
+        </is>
+      </c>
+      <c r="B561" t="inlineStr">
+        <is>
+          <t>Polygel set</t>
+        </is>
+      </c>
+      <c r="C561" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k01v6x</t>
+        </is>
+      </c>
+    </row>
+    <row r="562">
+      <c r="A562" t="inlineStr">
+        <is>
+          <t>1k01c68</t>
+        </is>
+      </c>
+      <c r="B562" t="inlineStr">
+        <is>
+          <t>First time trying builder gel - I’m OBSESSED!</t>
+        </is>
+      </c>
+      <c r="C562" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k01c68</t>
+        </is>
+      </c>
+    </row>
+    <row r="563">
+      <c r="A563" t="inlineStr">
+        <is>
+          <t>1k00xzk</t>
+        </is>
+      </c>
+      <c r="B563" t="inlineStr">
+        <is>
+          <t>My nail tech always absolutely kills it on every set she does on me, but I think this set that she did on me today is my new favorite!!</t>
+        </is>
+      </c>
+      <c r="C563" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rs4lvvd1x1ve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="564">
+      <c r="A564" t="inlineStr">
+        <is>
+          <t>1k00xkc</t>
+        </is>
+      </c>
+      <c r="B564" t="inlineStr">
+        <is>
+          <t>🤎</t>
+        </is>
+      </c>
+      <c r="C564" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cy6fcagyw1ve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="565">
+      <c r="A565" t="inlineStr">
+        <is>
+          <t>1k00tkp</t>
+        </is>
+      </c>
+      <c r="B565" t="inlineStr">
+        <is>
+          <t>Did I fucked up with choosing this vintage pink colour for my french tips?</t>
+        </is>
+      </c>
+      <c r="C565" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k00tkp</t>
+        </is>
+      </c>
+    </row>
+    <row r="566">
+      <c r="A566" t="inlineStr">
+        <is>
+          <t>1k00gsy</t>
+        </is>
+      </c>
+      <c r="B566" t="inlineStr">
+        <is>
+          <t>First Time with an Independent Tech</t>
+        </is>
+      </c>
+      <c r="C566" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k00gsy</t>
+        </is>
+      </c>
+    </row>
+    <row r="567">
+      <c r="A567" t="inlineStr">
+        <is>
+          <t>1k00gbe</t>
+        </is>
+      </c>
+      <c r="B567" t="inlineStr">
+        <is>
+          <t>Men nail art</t>
+        </is>
+      </c>
+      <c r="C567" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k00gbe</t>
+        </is>
+      </c>
+    </row>
+    <row r="568">
+      <c r="A568" t="inlineStr">
+        <is>
+          <t>1k00h5l</t>
+        </is>
+      </c>
+      <c r="B568" t="inlineStr">
+        <is>
+          <t>My natural nails</t>
+        </is>
+      </c>
+      <c r="C568" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/16vmo97mt1ve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="569">
+      <c r="A569" t="inlineStr">
+        <is>
+          <t>1jzy5hr</t>
+        </is>
+      </c>
+      <c r="B569" t="inlineStr">
+        <is>
+          <t>Update on the regrowth fix at home 🥹🫶🏻</t>
+        </is>
+      </c>
+      <c r="C569" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jzy5hr</t>
+        </is>
+      </c>
+    </row>
+    <row r="570">
+      <c r="A570" t="inlineStr">
+        <is>
+          <t>1jzvaex</t>
+        </is>
+      </c>
+      <c r="B570" t="inlineStr">
+        <is>
+          <t>Getting my nails done for the very first time!</t>
+        </is>
+      </c>
+      <c r="C570" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jzvaex/getting_my_nails_done_for_the_very_first_time/</t>
+        </is>
+      </c>
+    </row>
+    <row r="571">
+      <c r="A571" t="inlineStr">
+        <is>
+          <t>1k00378</t>
+        </is>
+      </c>
+      <c r="B571" t="inlineStr">
+        <is>
+          <t>best amazon gel polish??</t>
+        </is>
+      </c>
+      <c r="C571" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k00378/best_amazon_gel_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="572">
+      <c r="A572" t="inlineStr">
+        <is>
+          <t>1jzuy28</t>
+        </is>
+      </c>
+      <c r="B572" t="inlineStr">
+        <is>
+          <t>Nail help</t>
+        </is>
+      </c>
+      <c r="C572" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jzuy28/nail_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="573">
+      <c r="A573" t="inlineStr">
+        <is>
+          <t>1jzwjh8</t>
+        </is>
+      </c>
+      <c r="B573" t="inlineStr">
+        <is>
+          <t>Why does the glue at nail salon work better?</t>
+        </is>
+      </c>
+      <c r="C573" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jzwjh8/why_does_the_glue_at_nail_salon_work_better/</t>
+        </is>
+      </c>
+    </row>
+    <row r="574">
+      <c r="A574" t="inlineStr">
+        <is>
+          <t>1jzyoai</t>
+        </is>
+      </c>
+      <c r="B574" t="inlineStr">
+        <is>
+          <t>Inspired by a fellow male poster!</t>
+        </is>
+      </c>
+      <c r="C574" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mv78rw0pg1ve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="575">
+      <c r="A575" t="inlineStr">
+        <is>
+          <t>1jzzv1o</t>
+        </is>
+      </c>
+      <c r="B575" t="inlineStr">
+        <is>
+          <t>I SHOULDN'T HAVE CHANGED THE LONG ALMONDS nooo I feel so idk n@ked lol 😭😭😭😭😭</t>
+        </is>
+      </c>
+      <c r="C575" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aqhgmh08p1ve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="576">
+      <c r="A576" t="inlineStr">
+        <is>
+          <t>1jzzpy0</t>
+        </is>
+      </c>
+      <c r="B576" t="inlineStr">
+        <is>
+          <t>Easter egg French tips! 🐣🩷</t>
+        </is>
+      </c>
+      <c r="C576" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jzzpy0</t>
+        </is>
+      </c>
+    </row>
+    <row r="577">
+      <c r="A577" t="inlineStr">
+        <is>
+          <t>1jzzio8</t>
+        </is>
+      </c>
+      <c r="B577" t="inlineStr">
+        <is>
+          <t>Venalisa gel</t>
+        </is>
+      </c>
+      <c r="C577" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2ar39j4sm1ve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="578">
+      <c r="A578" t="inlineStr">
+        <is>
+          <t>1jzzehc</t>
+        </is>
+      </c>
+      <c r="B578" t="inlineStr">
+        <is>
+          <t>When to get new acrylics put on?</t>
+        </is>
+      </c>
+      <c r="C578" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jzzehc/when_to_get_new_acrylics_put_on/</t>
+        </is>
+      </c>
+    </row>
+    <row r="579">
+      <c r="A579" t="inlineStr">
+        <is>
+          <t>1jzzd88</t>
+        </is>
+      </c>
+      <c r="B579" t="inlineStr">
+        <is>
+          <t>Update on my teethy builder nails.</t>
+        </is>
+      </c>
+      <c r="C579" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jzzd88</t>
+        </is>
+      </c>
+    </row>
+    <row r="580">
+      <c r="A580" t="inlineStr">
+        <is>
+          <t>1jzz7wq</t>
+        </is>
+      </c>
+      <c r="B580" t="inlineStr">
+        <is>
+          <t>Galaxy nails 🌌</t>
+        </is>
+      </c>
+      <c r="C580" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v3mlz25mk1ve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="581">
+      <c r="A581" t="inlineStr">
+        <is>
+          <t>1jzz3ew</t>
+        </is>
+      </c>
+      <c r="B581" t="inlineStr">
+        <is>
+          <t>Natural nails vs Extensions</t>
+        </is>
+      </c>
+      <c r="C581" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jzz3ew/natural_nails_vs_extensions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="582">
+      <c r="A582" t="inlineStr">
+        <is>
+          <t>1jzz23s</t>
+        </is>
+      </c>
+      <c r="B582" t="inlineStr">
+        <is>
+          <t>Could anybody recommend a polish that matches Mac’s lady danger ls exactly or almost exactly? Tia!</t>
+        </is>
+      </c>
+      <c r="C582" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fqbfwnyfj1ve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="583">
+      <c r="A583" t="inlineStr">
+        <is>
+          <t>1jzz0dm</t>
+        </is>
+      </c>
+      <c r="B583" t="inlineStr">
+        <is>
+          <t>For those who like using dip polish, why do you like them?</t>
+        </is>
+      </c>
+      <c r="C583" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jzz0dm/for_those_who_like_using_dip_polish_why_do_you/</t>
+        </is>
+      </c>
+    </row>
+    <row r="584">
+      <c r="A584" t="inlineStr">
+        <is>
+          <t>1jzyzpm</t>
+        </is>
+      </c>
+      <c r="B584" t="inlineStr">
+        <is>
+          <t>what’s wrong with my nail shape?</t>
+        </is>
+      </c>
+      <c r="C584" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jzyzpm</t>
+        </is>
+      </c>
+    </row>
+    <row r="585">
+      <c r="A585" t="inlineStr">
+        <is>
+          <t>1jzyow7</t>
+        </is>
+      </c>
+      <c r="B585" t="inlineStr">
+        <is>
+          <t>Insane clown posse nails I did!</t>
+        </is>
+      </c>
+      <c r="C585" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x4dkl8ktg1ve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="586">
+      <c r="A586" t="inlineStr">
+        <is>
+          <t>1jzyo38</t>
+        </is>
+      </c>
+      <c r="B586" t="inlineStr">
+        <is>
+          <t>Black is my favorite color always.</t>
+        </is>
+      </c>
+      <c r="C586" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6xwjudkng1ve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="587">
+      <c r="A587" t="inlineStr">
+        <is>
+          <t>1jzygc6</t>
+        </is>
+      </c>
+      <c r="B587" t="inlineStr">
+        <is>
+          <t>I promised my son that one day I would make a design that he likes, here it is!</t>
+        </is>
+      </c>
+      <c r="C587" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e5ky4qg6f1ve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="588">
+      <c r="A588" t="inlineStr">
+        <is>
+          <t>1jzydc4</t>
+        </is>
+      </c>
+      <c r="B588" t="inlineStr">
+        <is>
+          <t>New nails 😍</t>
+        </is>
+      </c>
+      <c r="C588" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jzydc4</t>
+        </is>
+      </c>
+    </row>
+    <row r="589">
+      <c r="A589" t="inlineStr">
+        <is>
+          <t>1jzy8kt</t>
+        </is>
+      </c>
+      <c r="B589" t="inlineStr">
+        <is>
+          <t>Need opinions!!!</t>
+        </is>
+      </c>
+      <c r="C589" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jzy8kt</t>
+        </is>
+      </c>
+    </row>
+    <row r="590">
+      <c r="A590" t="inlineStr">
+        <is>
+          <t>1jzy1ql</t>
+        </is>
+      </c>
+      <c r="B590" t="inlineStr">
+        <is>
+          <t>🎀💅🏻</t>
+        </is>
+      </c>
+      <c r="C590" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jtxvi2k9c1ve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="591">
+      <c r="A591" t="inlineStr">
+        <is>
+          <t>1jzxu0g</t>
+        </is>
+      </c>
+      <c r="B591" t="inlineStr">
+        <is>
+          <t>Tips for getting better at nail art?</t>
+        </is>
+      </c>
+      <c r="C591" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o3xn2trpa1ve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="592">
+      <c r="A592" t="inlineStr">
+        <is>
+          <t>1jzxnaj</t>
+        </is>
+      </c>
+      <c r="B592" t="inlineStr">
+        <is>
+          <t>I asked for ‘my nails but better’ 💕</t>
+        </is>
+      </c>
+      <c r="C592" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jzxnaj</t>
+        </is>
+      </c>
+    </row>
+    <row r="593">
+      <c r="A593" t="inlineStr">
+        <is>
+          <t>1jzwwtl</t>
+        </is>
+      </c>
+      <c r="B593" t="inlineStr">
+        <is>
+          <t>DIY french nails</t>
+        </is>
+      </c>
+      <c r="C593" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jzwwtl</t>
+        </is>
+      </c>
+    </row>
+    <row r="594">
+      <c r="A594" t="inlineStr">
+        <is>
+          <t>1jzwwfr</t>
+        </is>
+      </c>
+      <c r="B594" t="inlineStr">
+        <is>
+          <t>Pink pearly club 💅🏻 (done by Jocelyn of course)</t>
+        </is>
+      </c>
+      <c r="C594" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jzwwfr</t>
+        </is>
+      </c>
+    </row>
+    <row r="595">
+      <c r="A595" t="inlineStr">
+        <is>
+          <t>1jzwd6k</t>
+        </is>
+      </c>
+      <c r="B595" t="inlineStr">
+        <is>
+          <t>Daily look</t>
+        </is>
+      </c>
+      <c r="C595" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a3uaiit601ve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="596">
+      <c r="A596" t="inlineStr">
+        <is>
+          <t>1jzw52y</t>
+        </is>
+      </c>
+      <c r="B596" t="inlineStr">
+        <is>
+          <t>Nude claws this time!</t>
+        </is>
+      </c>
+      <c r="C596" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jzw52y</t>
+        </is>
+      </c>
+    </row>
+    <row r="597">
+      <c r="A597" t="inlineStr">
+        <is>
+          <t>1jzvtmk</t>
+        </is>
+      </c>
+      <c r="B597" t="inlineStr">
+        <is>
+          <t>💜💜</t>
+        </is>
+      </c>
+      <c r="C597" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lgx2apgbw0ve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="598">
+      <c r="A598" t="inlineStr">
+        <is>
+          <t>1jzvfns</t>
+        </is>
+      </c>
+      <c r="B598" t="inlineStr">
+        <is>
+          <t>First time Bio Gel Soft Pink Cat Eye Nails for My Wedding</t>
+        </is>
+      </c>
+      <c r="C598" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jzvfns</t>
+        </is>
+      </c>
+    </row>
+    <row r="599">
+      <c r="A599" t="inlineStr">
+        <is>
+          <t>1jzuxkg</t>
+        </is>
+      </c>
+      <c r="B599" t="inlineStr">
+        <is>
+          <t>Something simple 💜</t>
+        </is>
+      </c>
+      <c r="C599" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5vokn3exp0ve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="600">
+      <c r="A600" t="inlineStr">
+        <is>
+          <t>1jzur07</t>
+        </is>
+      </c>
+      <c r="B600" t="inlineStr">
+        <is>
+          <t>Almond aura nails</t>
+        </is>
+      </c>
+      <c r="C600" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4490gytio0ve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="601">
+      <c r="A601" t="inlineStr">
+        <is>
+          <t>1jzum6z</t>
+        </is>
+      </c>
+      <c r="B601" t="inlineStr">
+        <is>
+          <t>Lost a nail at the last moment</t>
+        </is>
+      </c>
+      <c r="C601" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/864e1abon0ve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="602">
+      <c r="A602" t="inlineStr">
+        <is>
+          <t>1jznpp9</t>
+        </is>
+      </c>
+      <c r="B602" t="inlineStr">
+        <is>
+          <t>Been regularly polishing my nails since I was 13 and I still suck at it at age 30.</t>
+        </is>
+      </c>
+      <c r="C602" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3cch8pp5yyue1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="603">
+      <c r="A603" t="inlineStr">
+        <is>
+          <t>1jzqzhg</t>
+        </is>
+      </c>
+      <c r="B603" t="inlineStr">
+        <is>
+          <t>Former nail biter</t>
+        </is>
+      </c>
+      <c r="C603" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jzqzhg</t>
+        </is>
+      </c>
+    </row>
+    <row r="604">
+      <c r="A604" t="inlineStr">
+        <is>
+          <t>1jztxs8</t>
+        </is>
+      </c>
+      <c r="B604" t="inlineStr">
+        <is>
+          <t>Ive been using gel nail polish for quite a while now but stopped recently because my nails are sore to touch and look brittle. What causes this? Is it bc of the gel polish?</t>
+        </is>
+      </c>
+      <c r="C604" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3d8vo2dwi0ve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="605">
+      <c r="A605" t="inlineStr">
+        <is>
+          <t>1jztta8</t>
+        </is>
+      </c>
+      <c r="B605" t="inlineStr">
+        <is>
+          <t>Recreated a set i saw on pinterest!</t>
+        </is>
+      </c>
+      <c r="C605" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jztta8</t>
+        </is>
+      </c>
+    </row>
+    <row r="606">
+      <c r="A606" t="inlineStr">
+        <is>
+          <t>1jztx0v</t>
+        </is>
+      </c>
+      <c r="B606" t="inlineStr">
+        <is>
+          <t>calico cat/orange cat nails</t>
+        </is>
+      </c>
+      <c r="C606" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/a19u0cxqi0ve1</t>
+        </is>
+      </c>
+    </row>
+    <row r="607">
+      <c r="A607" t="inlineStr">
+        <is>
+          <t>1jztswf</t>
+        </is>
+      </c>
+      <c r="B607" t="inlineStr">
+        <is>
+          <t>Gel paint chipping</t>
+        </is>
+      </c>
+      <c r="C607" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jztswf</t>
+        </is>
+      </c>
+    </row>
+    <row r="608">
+      <c r="A608" t="inlineStr">
+        <is>
+          <t>1k0eu0r</t>
+        </is>
+      </c>
+      <c r="B608" t="inlineStr">
+        <is>
+          <t>Red Glass Nails Attempt!</t>
+        </is>
+      </c>
+      <c r="C608" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k0eu0r/red_glass_nails_attempt/</t>
+        </is>
+      </c>
+    </row>
+    <row r="609">
+      <c r="A609" t="inlineStr">
+        <is>
+          <t>1k0eix6</t>
+        </is>
+      </c>
+      <c r="B609" t="inlineStr">
+        <is>
+          <t>Birthday nails!</t>
+        </is>
+      </c>
+      <c r="C609" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k0eix6</t>
+        </is>
+      </c>
+    </row>
+    <row r="610">
+      <c r="A610" t="inlineStr">
+        <is>
+          <t>1k0duxf</t>
+        </is>
+      </c>
+      <c r="B610" t="inlineStr">
+        <is>
+          <t>Emma Frost inspired nails (I love using my cats as background)</t>
+        </is>
+      </c>
+      <c r="C610" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k0duxf</t>
+        </is>
+      </c>
+    </row>
+    <row r="611">
+      <c r="A611" t="inlineStr">
+        <is>
+          <t>1k0d7zy</t>
+        </is>
+      </c>
+      <c r="B611" t="inlineStr">
+        <is>
+          <t>If you’re doing 2 layers of QDTC, how long should you wait between the 2 layers?</t>
+        </is>
+      </c>
+      <c r="C611" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k0d7zy/if_youre_doing_2_layers_of_qdtc_how_long_should/</t>
+        </is>
+      </c>
+    </row>
+    <row r="612">
+      <c r="A612" t="inlineStr">
+        <is>
+          <t>1k0d1ms</t>
+        </is>
+      </c>
+      <c r="B612" t="inlineStr">
+        <is>
+          <t>Clionadh Radiance in four different lightings 🤯</t>
+        </is>
+      </c>
+      <c r="C612" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k0d1ms</t>
+        </is>
+      </c>
+    </row>
+    <row r="613">
+      <c r="A613" t="inlineStr">
+        <is>
+          <t>1k0cg9j</t>
+        </is>
+      </c>
+      <c r="B613" t="inlineStr">
+        <is>
+          <t>So happy with these !🌀💙🩵</t>
+        </is>
+      </c>
+      <c r="C613" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l4xpcobkp4ve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="614">
+      <c r="A614" t="inlineStr">
+        <is>
+          <t>1k0b39j</t>
+        </is>
+      </c>
+      <c r="B614" t="inlineStr">
+        <is>
+          <t>Cookies &amp; Cream 🍪</t>
+        </is>
+      </c>
+      <c r="C614" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8ddsxh7va4ve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="615">
+      <c r="A615" t="inlineStr">
+        <is>
+          <t>1k0ai0w</t>
+        </is>
+      </c>
+      <c r="B615" t="inlineStr">
+        <is>
+          <t>🌸 totoro x spring 🌸</t>
+        </is>
+      </c>
+      <c r="C615" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w3fy1op454ve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="616">
+      <c r="A616" t="inlineStr">
+        <is>
+          <t>1k0agay</t>
+        </is>
+      </c>
+      <c r="B616" t="inlineStr">
+        <is>
+          <t>Anyone know of a dupe for this lumen polish?</t>
+        </is>
+      </c>
+      <c r="C616" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4nz3eieo44ve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="617">
+      <c r="A617" t="inlineStr">
+        <is>
+          <t>1k0a4md</t>
+        </is>
+      </c>
+      <c r="B617" t="inlineStr">
+        <is>
+          <t>Best type of polish for reckless people?</t>
+        </is>
+      </c>
+      <c r="C617" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k0a4md/best_type_of_polish_for_reckless_people/</t>
+        </is>
+      </c>
+    </row>
+    <row r="618">
+      <c r="A618" t="inlineStr">
+        <is>
+          <t>1k09tv7</t>
+        </is>
+      </c>
+      <c r="B618" t="inlineStr">
+        <is>
+          <t>Easter egg skittle</t>
+        </is>
+      </c>
+      <c r="C618" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k09tv7</t>
+        </is>
+      </c>
+    </row>
+    <row r="619">
+      <c r="A619" t="inlineStr">
+        <is>
+          <t>1k09jxc</t>
+        </is>
+      </c>
+      <c r="B619" t="inlineStr">
+        <is>
+          <t>Indomitable vs Riding Sleeping Bags Down the Stairs?</t>
+        </is>
+      </c>
+      <c r="C619" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k09jxc/indomitable_vs_riding_sleeping_bags_down_the/</t>
+        </is>
+      </c>
+    </row>
+    <row r="620">
+      <c r="A620" t="inlineStr">
+        <is>
+          <t>1k097aw</t>
+        </is>
+      </c>
+      <c r="B620" t="inlineStr">
+        <is>
+          <t>Color request for this pink and green pleaseeeeee!!</t>
+        </is>
+      </c>
+      <c r="C620" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iztg2rgxs3ve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="621">
+      <c r="A621" t="inlineStr">
+        <is>
+          <t>1k08jkz</t>
+        </is>
+      </c>
+      <c r="B621" t="inlineStr">
+        <is>
+          <t>Did tequila nails for Mexico trip (swipe for inspo)</t>
+        </is>
+      </c>
+      <c r="C621" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k08jkz</t>
+        </is>
+      </c>
+    </row>
+    <row r="622">
+      <c r="A622" t="inlineStr">
+        <is>
+          <t>1k08ba3</t>
+        </is>
+      </c>
+      <c r="B622" t="inlineStr">
+        <is>
+          <t>LOOK AT WHAT’S IN THE ULTA CATALOG I GOT TODAY!! 👀 (finally an update to our rumored CG rebrand!!)</t>
+        </is>
+      </c>
+      <c r="C622" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uj99qcfnk3ve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="623">
+      <c r="A623" t="inlineStr">
+        <is>
+          <t>1k087wv</t>
+        </is>
+      </c>
+      <c r="B623" t="inlineStr">
+        <is>
+          <t>Clionadh Skittle</t>
+        </is>
+      </c>
+      <c r="C623" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/etg8grwsj3ve1</t>
+        </is>
+      </c>
+    </row>
+    <row r="624">
+      <c r="A624" t="inlineStr">
+        <is>
+          <t>1k07gqr</t>
+        </is>
+      </c>
+      <c r="B624" t="inlineStr">
+        <is>
+          <t>Lurid Lacquer saying what we’re all thinking…. Through pink polish of course</t>
+        </is>
+      </c>
+      <c r="C624" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m7awouzvc3ve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="625">
+      <c r="A625" t="inlineStr">
+        <is>
+          <t>1k074fv</t>
+        </is>
+      </c>
+      <c r="B625" t="inlineStr">
+        <is>
+          <t>Zoya Earth Day Sale?</t>
+        </is>
+      </c>
+      <c r="C625" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k074fv/zoya_earth_day_sale/</t>
+        </is>
+      </c>
+    </row>
+    <row r="626">
+      <c r="A626" t="inlineStr">
+        <is>
+          <t>1k06sy4</t>
+        </is>
+      </c>
+      <c r="B626" t="inlineStr">
+        <is>
+          <t>Kisses to my X’s</t>
+        </is>
+      </c>
+      <c r="C626" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/fx81dye173ve1</t>
+        </is>
+      </c>
+    </row>
+    <row r="627">
+      <c r="A627" t="inlineStr">
+        <is>
+          <t>1k06ls1</t>
+        </is>
+      </c>
+      <c r="B627" t="inlineStr">
+        <is>
+          <t>Starrily’s Serpent’s Lair</t>
+        </is>
+      </c>
+      <c r="C627" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k06ls1</t>
+        </is>
+      </c>
+    </row>
+    <row r="628">
+      <c r="A628" t="inlineStr">
+        <is>
+          <t>1k06ki1</t>
+        </is>
+      </c>
+      <c r="B628" t="inlineStr">
+        <is>
+          <t>It’s giving Spring 🌸</t>
+        </is>
+      </c>
+      <c r="C628" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/faq5hmf153ve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="629">
+      <c r="A629" t="inlineStr">
+        <is>
+          <t>1k06c9l</t>
+        </is>
+      </c>
+      <c r="B629" t="inlineStr">
+        <is>
+          <t>Dupe for sally Hansen haute stone</t>
+        </is>
+      </c>
+      <c r="C629" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tqxlz4e233ve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="630">
+      <c r="A630" t="inlineStr">
+        <is>
+          <t>1k06btd</t>
+        </is>
+      </c>
+      <c r="B630" t="inlineStr">
+        <is>
+          <t>Dust to Dust Spirulina</t>
+        </is>
+      </c>
+      <c r="C630" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k06btd/dust_to_dust_spirulina/</t>
+        </is>
+      </c>
+    </row>
+    <row r="631">
+      <c r="A631" t="inlineStr">
+        <is>
+          <t>1k06192</t>
+        </is>
+      </c>
+      <c r="B631" t="inlineStr">
+        <is>
+          <t>New favorite black polish -ILNP Cityscapes</t>
+        </is>
+      </c>
+      <c r="C631" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/3ksnibog03ve1</t>
+        </is>
+      </c>
+    </row>
+    <row r="632">
+      <c r="A632" t="inlineStr">
+        <is>
+          <t>1k05n8l</t>
+        </is>
+      </c>
+      <c r="B632" t="inlineStr">
+        <is>
+          <t>I just realized what ilnp stands for</t>
+        </is>
+      </c>
+      <c r="C632" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k05n8l/i_just_realized_what_ilnp_stands_for/</t>
+        </is>
+      </c>
+    </row>
+    <row r="633">
+      <c r="A633" t="inlineStr">
+        <is>
+          <t>1k04oa6</t>
+        </is>
+      </c>
+      <c r="B633" t="inlineStr">
+        <is>
+          <t>Teal nails 💙💚</t>
+        </is>
+      </c>
+      <c r="C633" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/o2yxp319p2ve1</t>
+        </is>
+      </c>
+    </row>
+    <row r="634">
+      <c r="A634" t="inlineStr">
+        <is>
+          <t>1k04kqa</t>
+        </is>
+      </c>
+      <c r="B634" t="inlineStr">
+        <is>
+          <t>Smitten With Spyglass</t>
+        </is>
+      </c>
+      <c r="C634" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k04kqa</t>
+        </is>
+      </c>
+    </row>
+    <row r="635">
+      <c r="A635" t="inlineStr">
+        <is>
+          <t>1k04kag</t>
+        </is>
+      </c>
+      <c r="B635" t="inlineStr">
+        <is>
+          <t>Mixing top coats (toluene + non)</t>
+        </is>
+      </c>
+      <c r="C635" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k04kag/mixing_top_coats_toluene_non/</t>
+        </is>
+      </c>
+    </row>
+    <row r="636">
+      <c r="A636" t="inlineStr">
+        <is>
+          <t>1k03ysm</t>
+        </is>
+      </c>
+      <c r="B636" t="inlineStr">
+        <is>
+          <t>Space nails!</t>
+        </is>
+      </c>
+      <c r="C636" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zki9rfpnj2ve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="637">
+      <c r="A637" t="inlineStr">
+        <is>
+          <t>1k03y73</t>
+        </is>
+      </c>
+      <c r="B637" t="inlineStr">
+        <is>
+          <t>Mooncat’s Serpents of Eden sucks.  Agreed?</t>
+        </is>
+      </c>
+      <c r="C637" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k03y73/mooncats_serpents_of_eden_sucks_agreed/</t>
+        </is>
+      </c>
+    </row>
+    <row r="638">
+      <c r="A638" t="inlineStr">
+        <is>
+          <t>1k03p3y</t>
+        </is>
+      </c>
+      <c r="B638" t="inlineStr">
+        <is>
+          <t>“Siblings not Twins”</t>
+        </is>
+      </c>
+      <c r="C638" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k03p3y</t>
+        </is>
+      </c>
+    </row>
+    <row r="639">
+      <c r="A639" t="inlineStr">
+        <is>
+          <t>1k03hey</t>
+        </is>
+      </c>
+      <c r="B639" t="inlineStr">
+        <is>
+          <t>Orly Shine</t>
+        </is>
+      </c>
+      <c r="C639" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rue0f3jxf2ve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="640">
+      <c r="A640" t="inlineStr">
+        <is>
+          <t>1k033dn</t>
+        </is>
+      </c>
+      <c r="B640" t="inlineStr">
+        <is>
+          <t>"Fauna" from Shleee Polish (HHC March 2025)</t>
+        </is>
+      </c>
+      <c r="C640" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/xkfzz8nvc2ve1</t>
+        </is>
+      </c>
+    </row>
+    <row r="641">
+      <c r="A641" t="inlineStr">
+        <is>
+          <t>1k02l7j</t>
+        </is>
+      </c>
+      <c r="B641" t="inlineStr">
+        <is>
+          <t>I seriously can’t say enough good things about Apocalypse Polish! This jelly is to die for!! 😩“Flayer of Minds” 💜✨</t>
+        </is>
+      </c>
+      <c r="C641" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k02l7j</t>
+        </is>
+      </c>
+    </row>
+    <row r="642">
+      <c r="A642" t="inlineStr">
+        <is>
+          <t>1k01yeu</t>
+        </is>
+      </c>
+      <c r="B642" t="inlineStr">
+        <is>
+          <t>What am i doing WRONG with jellies?</t>
+        </is>
+      </c>
+      <c r="C642" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k01yeu/what_am_i_doing_wrong_with_jellies/</t>
+        </is>
+      </c>
+    </row>
+    <row r="643">
+      <c r="A643" t="inlineStr">
+        <is>
+          <t>1k00f5k</t>
+        </is>
+      </c>
+      <c r="B643" t="inlineStr">
+        <is>
+          <t>Top Coat Help</t>
+        </is>
+      </c>
+      <c r="C643" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/04ay23f7t1ve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="644">
+      <c r="A644" t="inlineStr">
+        <is>
+          <t>1jzzkqk</t>
+        </is>
+      </c>
+      <c r="B644" t="inlineStr">
+        <is>
+          <t>I cabochon'd over 70 nail polishes this week: here's what I learned</t>
+        </is>
+      </c>
+      <c r="C644" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jzzkqk</t>
+        </is>
+      </c>
+    </row>
+    <row r="645">
+      <c r="A645" t="inlineStr">
+        <is>
+          <t>1jzzdar</t>
+        </is>
+      </c>
+      <c r="B645" t="inlineStr">
+        <is>
+          <t>Mooncat Reccomendations</t>
+        </is>
+      </c>
+      <c r="C645" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jzzdar/mooncat_reccomendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="646">
+      <c r="A646" t="inlineStr">
+        <is>
+          <t>1jzyozd</t>
+        </is>
+      </c>
+      <c r="B646" t="inlineStr">
+        <is>
+          <t>Got compliments on my skittle at work today!</t>
+        </is>
+      </c>
+      <c r="C646" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jzyozd</t>
+        </is>
+      </c>
+    </row>
+    <row r="647">
+      <c r="A647" t="inlineStr">
+        <is>
+          <t>1jzymmn</t>
+        </is>
+      </c>
+      <c r="B647" t="inlineStr">
+        <is>
+          <t>Help me decide between similar shades!</t>
+        </is>
+      </c>
+      <c r="C647" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jzymmn</t>
+        </is>
+      </c>
+    </row>
+    <row r="648">
+      <c r="A648" t="inlineStr">
+        <is>
+          <t>1jzyd2o</t>
+        </is>
+      </c>
+      <c r="B648" t="inlineStr">
+        <is>
+          <t>Let's talk about Lechat</t>
+        </is>
+      </c>
+      <c r="C648" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jzyd2o/lets_talk_about_lechat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="649">
+      <c r="A649" t="inlineStr">
+        <is>
+          <t>1jzy49d</t>
+        </is>
+      </c>
+      <c r="B649" t="inlineStr">
+        <is>
+          <t>Recommendations for creme polishes (Canada edition)</t>
+        </is>
+      </c>
+      <c r="C649" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jzy49d/recommendations_for_creme_polishes_canada_edition/</t>
+        </is>
+      </c>
+    </row>
+    <row r="650">
+      <c r="A650" t="inlineStr">
+        <is>
+          <t>1jzwwi2</t>
+        </is>
+      </c>
+      <c r="B650" t="inlineStr">
+        <is>
+          <t>Shiny Flowers</t>
+        </is>
+      </c>
+      <c r="C650" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jzwwi2</t>
+        </is>
+      </c>
+    </row>
+    <row r="651">
+      <c r="A651" t="inlineStr">
+        <is>
+          <t>1jzw8n7</t>
+        </is>
+      </c>
+      <c r="B651" t="inlineStr">
+        <is>
+          <t>Holo taco matte topcoat worth it?</t>
+        </is>
+      </c>
+      <c r="C651" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jzw8n7/holo_taco_matte_topcoat_worth_it/</t>
+        </is>
+      </c>
+    </row>
+    <row r="652">
+      <c r="A652" t="inlineStr">
+        <is>
+          <t>1jzw6ti</t>
+        </is>
+      </c>
+      <c r="B652" t="inlineStr">
+        <is>
+          <t>Sparkly polish, me? No, just a demure neutral, I swear... 🌈💕</t>
+        </is>
+      </c>
+      <c r="C652" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jzw6ti</t>
+        </is>
+      </c>
+    </row>
+    <row r="653">
+      <c r="A653" t="inlineStr">
+        <is>
+          <t>1jzw1g0</t>
+        </is>
+      </c>
+      <c r="B653" t="inlineStr">
+        <is>
+          <t>I always go back to neutrals</t>
+        </is>
+      </c>
+      <c r="C653" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8xyu0pxvx0ve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="654">
+      <c r="A654" t="inlineStr">
+        <is>
+          <t>1jzw0kh</t>
+        </is>
+      </c>
+      <c r="B654" t="inlineStr">
+        <is>
+          <t>Mooncat Moonicorn vs LynB Eidolism?</t>
+        </is>
+      </c>
+      <c r="C654" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jzw0kh/mooncat_moonicorn_vs_lynb_eidolism/</t>
+        </is>
+      </c>
+    </row>
+    <row r="655">
+      <c r="A655" t="inlineStr">
+        <is>
+          <t>1jzvboa</t>
+        </is>
+      </c>
+      <c r="B655" t="inlineStr">
+        <is>
+          <t>Sparkly lavender for spring</t>
+        </is>
+      </c>
+      <c r="C655" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/gg66vqgrs0ve1</t>
+        </is>
+      </c>
+    </row>
+    <row r="656">
+      <c r="A656" t="inlineStr">
+        <is>
+          <t>1jzuvrm</t>
+        </is>
+      </c>
+      <c r="B656" t="inlineStr">
+        <is>
+          <t>What magnetic technique is used to get these three lines?</t>
+        </is>
+      </c>
+      <c r="C656" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f1f4be6kp0ve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="657">
+      <c r="A657" t="inlineStr">
+        <is>
+          <t>1jzurcx</t>
+        </is>
+      </c>
+      <c r="B657" t="inlineStr">
+        <is>
+          <t>Mmm, chocolate mini eggs</t>
+        </is>
+      </c>
+      <c r="C657" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jzurcx</t>
+        </is>
+      </c>
+    </row>
+    <row r="658">
+      <c r="A658" t="inlineStr">
+        <is>
+          <t>1jzu8qt</t>
+        </is>
+      </c>
+      <c r="B658" t="inlineStr">
+        <is>
+          <t>Purple and Green Magnetic</t>
+        </is>
+      </c>
+      <c r="C658" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jzu8qt/purple_and_green_magnetic/</t>
+        </is>
+      </c>
+    </row>
+    <row r="659">
+      <c r="A659" t="inlineStr">
+        <is>
+          <t>1jzu5gu</t>
+        </is>
+      </c>
+      <c r="B659" t="inlineStr">
+        <is>
+          <t>KB Shimmer newbie advice</t>
+        </is>
+      </c>
+      <c r="C659" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jzu5gu/kb_shimmer_newbie_advice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="660">
+      <c r="A660" t="inlineStr">
+        <is>
+          <t>1jztprn</t>
+        </is>
+      </c>
+      <c r="B660" t="inlineStr">
+        <is>
+          <t>For my next magic trick, I will be switching the polish on my nails around!</t>
+        </is>
+      </c>
+      <c r="C660" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/6yg8rv09h0ve1</t>
+        </is>
+      </c>
+    </row>
+    <row r="661">
+      <c r="A661" t="inlineStr">
+        <is>
+          <t>1jztluv</t>
+        </is>
+      </c>
+      <c r="B661" t="inlineStr">
+        <is>
+          <t>they’re french, oui oui</t>
+        </is>
+      </c>
+      <c r="C661" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jztluv</t>
+        </is>
+      </c>
+    </row>
+    <row r="662">
+      <c r="A662" t="inlineStr">
+        <is>
+          <t>1jztjg6</t>
+        </is>
+      </c>
+      <c r="B662" t="inlineStr">
+        <is>
+          <t>Lord of the Holo Mountain</t>
+        </is>
+      </c>
+      <c r="C662" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jztjg6</t>
+        </is>
+      </c>
+    </row>
+    <row r="663">
+      <c r="A663" t="inlineStr">
+        <is>
+          <t>1jztgt2</t>
+        </is>
+      </c>
+      <c r="B663" t="inlineStr">
+        <is>
+          <t>My OPI collection after a few months</t>
+        </is>
+      </c>
+      <c r="C663" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qolgsqrff0ve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="664">
+      <c r="A664" t="inlineStr">
+        <is>
+          <t>1jzt5u9</t>
+        </is>
+      </c>
+      <c r="B664" t="inlineStr">
+        <is>
+          <t>This one became a quick fav</t>
+        </is>
+      </c>
+      <c r="C664" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/alduhpw6d0ve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="665">
+      <c r="A665" t="inlineStr">
+        <is>
+          <t>1jzsqmi</t>
+        </is>
+      </c>
+      <c r="B665" t="inlineStr">
+        <is>
+          <t>I need more of Canmake nail polish!</t>
+        </is>
+      </c>
+      <c r="C665" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jzsqmi</t>
+        </is>
+      </c>
+    </row>
+    <row r="666">
+      <c r="A666" t="inlineStr">
+        <is>
+          <t>1jzsiqn</t>
+        </is>
+      </c>
+      <c r="B666" t="inlineStr">
+        <is>
+          <t>Day 3 Magnetic</t>
+        </is>
+      </c>
+      <c r="C666" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/36ck34ue80ve1</t>
+        </is>
+      </c>
+    </row>
+    <row r="667">
+      <c r="A667" t="inlineStr">
+        <is>
+          <t>1jzsd9p</t>
+        </is>
+      </c>
+      <c r="B667" t="inlineStr">
+        <is>
+          <t>MOONCAT SALE; which polishes to avoid? (Even if they're not in the list below) I want to avoid hoarding/panic buying</t>
+        </is>
+      </c>
+      <c r="C667" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jzsd9p</t>
+        </is>
+      </c>
+    </row>
+    <row r="668">
+      <c r="A668" t="inlineStr">
+        <is>
+          <t>1jzrt4m</t>
+        </is>
+      </c>
+      <c r="B668" t="inlineStr">
+        <is>
+          <t>BKL - I Invoke Thee</t>
+        </is>
+      </c>
+      <c r="C668" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jzrt4m</t>
+        </is>
+      </c>
+    </row>
+    <row r="669">
+      <c r="A669" t="inlineStr">
+        <is>
+          <t>1jzrj0g</t>
+        </is>
+      </c>
+      <c r="B669" t="inlineStr">
+        <is>
+          <t>What's in your Mooncat cart for the sale</t>
+        </is>
+      </c>
+      <c r="C669" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jzrj0g/whats_in_your_mooncat_cart_for_the_sale/</t>
+        </is>
+      </c>
+    </row>
+    <row r="670">
+      <c r="A670" t="inlineStr">
+        <is>
+          <t>1jzqb15</t>
+        </is>
+      </c>
+      <c r="B670" t="inlineStr">
+        <is>
+          <t>New H&amp;M jellies</t>
+        </is>
+      </c>
+      <c r="C670" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jzqb15</t>
+        </is>
+      </c>
+    </row>
+    <row r="671">
+      <c r="A671" t="inlineStr">
+        <is>
+          <t>1jzpxay</t>
+        </is>
+      </c>
+      <c r="B671" t="inlineStr">
+        <is>
+          <t>Which finishes/pigments are at risk due to tarrifs?</t>
+        </is>
+      </c>
+      <c r="C671" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6dtobaedmzue1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="672">
+      <c r="A672" t="inlineStr">
+        <is>
+          <t>1jzp84p</t>
+        </is>
+      </c>
+      <c r="B672" t="inlineStr">
+        <is>
+          <t>Polish me silly</t>
+        </is>
+      </c>
+      <c r="C672" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jzp84p</t>
+        </is>
+      </c>
+    </row>
+    <row r="673">
+      <c r="A673" t="inlineStr">
+        <is>
+          <t>1jzn6s9</t>
+        </is>
+      </c>
+      <c r="B673" t="inlineStr">
+        <is>
+          <t>Comparisons: Monarch Culprit’s Charm and Rogue It Glows?</t>
+        </is>
+      </c>
+      <c r="C673" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jzn6s9/comparisons_monarch_culprits_charm_and_rogue_it/</t>
+        </is>
+      </c>
+    </row>
+    <row r="674">
+      <c r="A674" t="inlineStr">
+        <is>
+          <t>1k0cpa9</t>
+        </is>
+      </c>
+      <c r="B674" t="inlineStr">
+        <is>
+          <t>Happy with my progress, making 3D effect</t>
+        </is>
+      </c>
+      <c r="C674" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f3030pids4ve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="675">
+      <c r="A675" t="inlineStr">
+        <is>
+          <t>1k095zn</t>
+        </is>
+      </c>
+      <c r="B675" t="inlineStr">
+        <is>
+          <t>Comic book nails</t>
+        </is>
+      </c>
+      <c r="C675" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/twdz3c7ls3ve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="676">
+      <c r="A676" t="inlineStr">
+        <is>
+          <t>1k081vp</t>
+        </is>
+      </c>
+      <c r="B676" t="inlineStr">
+        <is>
+          <t>Pretty proud of this set 💕 took 4hrs per hand</t>
+        </is>
+      </c>
+      <c r="C676" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k081vp</t>
+        </is>
+      </c>
+    </row>
+    <row r="677">
+      <c r="A677" t="inlineStr">
+        <is>
+          <t>1k08157</t>
+        </is>
+      </c>
+      <c r="B677" t="inlineStr">
+        <is>
+          <t>The different kinds of stickers that could come in a press on nail package, the silicone molds I have to make charms and the charms I have currently</t>
+        </is>
+      </c>
+      <c r="C677" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/mb44ynz0i3ve1</t>
+        </is>
+      </c>
+    </row>
+    <row r="678">
+      <c r="A678" t="inlineStr">
+        <is>
+          <t>1k06m60</t>
+        </is>
+      </c>
+      <c r="B678" t="inlineStr">
+        <is>
+          <t>Hearts for the week 🩷❤️🤍</t>
+        </is>
+      </c>
+      <c r="C678" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w1hvsm5f53ve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="679">
+      <c r="A679" t="inlineStr">
+        <is>
+          <t>1k05c7m</t>
+        </is>
+      </c>
+      <c r="B679" t="inlineStr">
+        <is>
+          <t>Spring fever!!!</t>
+        </is>
+      </c>
+      <c r="C679" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sd7o1zpou2ve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="680">
+      <c r="A680" t="inlineStr">
+        <is>
+          <t>1k050wq</t>
+        </is>
+      </c>
+      <c r="B680" t="inlineStr">
+        <is>
+          <t>Carnival/Circus themed nails for our spring nail art competition at school! 🎪🎡</t>
+        </is>
+      </c>
+      <c r="C680" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tdc8hfw3s2ve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="681">
+      <c r="A681" t="inlineStr">
+        <is>
+          <t>1k04gep</t>
+        </is>
+      </c>
+      <c r="B681" t="inlineStr">
+        <is>
+          <t>Have been playing around with 3D textured nail art and flowers! 🌺</t>
+        </is>
+      </c>
+      <c r="C681" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k04gep</t>
+        </is>
+      </c>
+    </row>
+    <row r="682">
+      <c r="A682" t="inlineStr">
+        <is>
+          <t>1k03rvl</t>
+        </is>
+      </c>
+      <c r="B682" t="inlineStr">
+        <is>
+          <t>Some kind of dark nails? Goth? Bdsm? :)</t>
+        </is>
+      </c>
+      <c r="C682" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k03rvl</t>
+        </is>
+      </c>
+    </row>
+    <row r="683">
+      <c r="A683" t="inlineStr">
+        <is>
+          <t>1k00zee</t>
+        </is>
+      </c>
+      <c r="B683" t="inlineStr">
+        <is>
+          <t>4 months in</t>
+        </is>
+      </c>
+      <c r="C683" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zym0dcicx1ve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="684">
+      <c r="A684" t="inlineStr">
+        <is>
+          <t>1jzzw4z</t>
+        </is>
+      </c>
+      <c r="B684" t="inlineStr">
+        <is>
+          <t>Recent Sets I've Made</t>
+        </is>
+      </c>
+      <c r="C684" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jzzw4z</t>
+        </is>
+      </c>
+    </row>
+    <row r="685">
+      <c r="A685" t="inlineStr">
+        <is>
+          <t>1jzzecd</t>
+        </is>
+      </c>
+      <c r="B685" t="inlineStr">
+        <is>
+          <t>Baby's first chrome</t>
+        </is>
+      </c>
+      <c r="C685" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jzzecd</t>
+        </is>
+      </c>
+    </row>
+    <row r="686">
+      <c r="A686" t="inlineStr">
+        <is>
+          <t>1jzwxm8</t>
+        </is>
+      </c>
+      <c r="B686" t="inlineStr">
+        <is>
+          <t>Recent practice</t>
+        </is>
+      </c>
+      <c r="C686" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jzwxm8</t>
+        </is>
+      </c>
+    </row>
+    <row r="687">
+      <c r="A687" t="inlineStr">
+        <is>
+          <t>1jztqiu</t>
+        </is>
+      </c>
+      <c r="B687" t="inlineStr">
+        <is>
+          <t>I want to eat these</t>
+        </is>
+      </c>
+      <c r="C687" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jztqiu</t>
+        </is>
+      </c>
+    </row>
+    <row r="688">
+      <c r="A688" t="inlineStr">
+        <is>
+          <t>1jzpdqj</t>
+        </is>
+      </c>
+      <c r="B688" t="inlineStr">
+        <is>
+          <t>Help! Top coat is smoothing out my 3d texture gel nails</t>
+        </is>
+      </c>
+      <c r="C688" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jzpdqj</t>
+        </is>
+      </c>
+    </row>
+    <row r="689">
+      <c r="A689" t="inlineStr">
+        <is>
+          <t>1jznwfn</t>
+        </is>
+      </c>
+      <c r="B689" t="inlineStr">
+        <is>
+          <t>Небесная Спираль</t>
+        </is>
+      </c>
+      <c r="C689" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1aygstei0zue1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Thu Apr 17 08:12:29 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_04_20.xlsx
+++ b/data/collected_data/2025_04_20.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C689"/>
+  <dimension ref="A1:C875"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12146,6 +12146,3168 @@
         </is>
       </c>
     </row>
+    <row r="690">
+      <c r="A690" t="inlineStr">
+        <is>
+          <t>1k175mq</t>
+        </is>
+      </c>
+      <c r="B690" t="inlineStr">
+        <is>
+          <t>What do we think?</t>
+        </is>
+      </c>
+      <c r="C690" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u7h56tdnmcve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="691">
+      <c r="A691" t="inlineStr">
+        <is>
+          <t>1k17cw5</t>
+        </is>
+      </c>
+      <c r="B691" t="inlineStr">
+        <is>
+          <t>Work gloves for long nails?</t>
+        </is>
+      </c>
+      <c r="C691" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k17cw5/work_gloves_for_long_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="692">
+      <c r="A692" t="inlineStr">
+        <is>
+          <t>1k16i2y</t>
+        </is>
+      </c>
+      <c r="B692" t="inlineStr">
+        <is>
+          <t>Lifting</t>
+        </is>
+      </c>
+      <c r="C692" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8dw7n63aecve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="693">
+      <c r="A693" t="inlineStr">
+        <is>
+          <t>1k14u9a</t>
+        </is>
+      </c>
+      <c r="B693" t="inlineStr">
+        <is>
+          <t>French Cheat finally!!!</t>
+        </is>
+      </c>
+      <c r="C693" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u8fsyrd9ubve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="694">
+      <c r="A694" t="inlineStr">
+        <is>
+          <t>1k15vlt</t>
+        </is>
+      </c>
+      <c r="B694" t="inlineStr">
+        <is>
+          <t>Last pic of these nails before doing a new set for Coachella weekend 2</t>
+        </is>
+      </c>
+      <c r="C694" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mwqjz6mj6cve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="695">
+      <c r="A695" t="inlineStr">
+        <is>
+          <t>1k14d0r</t>
+        </is>
+      </c>
+      <c r="B695" t="inlineStr">
+        <is>
+          <t>obsessed is an understatement 😭🤩</t>
+        </is>
+      </c>
+      <c r="C695" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k14d0r</t>
+        </is>
+      </c>
+    </row>
+    <row r="696">
+      <c r="A696" t="inlineStr">
+        <is>
+          <t>1k14aj5</t>
+        </is>
+      </c>
+      <c r="B696" t="inlineStr">
+        <is>
+          <t>birthday aura nails 🌈</t>
+        </is>
+      </c>
+      <c r="C696" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k14aj5</t>
+        </is>
+      </c>
+    </row>
+    <row r="697">
+      <c r="A697" t="inlineStr">
+        <is>
+          <t>1k13nfj</t>
+        </is>
+      </c>
+      <c r="B697" t="inlineStr">
+        <is>
+          <t>my nail tips are naturally white</t>
+        </is>
+      </c>
+      <c r="C697" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k13nfj</t>
+        </is>
+      </c>
+    </row>
+    <row r="698">
+      <c r="A698" t="inlineStr">
+        <is>
+          <t>1k169ge</t>
+        </is>
+      </c>
+      <c r="B698" t="inlineStr">
+        <is>
+          <t>Press on</t>
+        </is>
+      </c>
+      <c r="C698" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k169ge</t>
+        </is>
+      </c>
+    </row>
+    <row r="699">
+      <c r="A699" t="inlineStr">
+        <is>
+          <t>1k166e7</t>
+        </is>
+      </c>
+      <c r="B699" t="inlineStr">
+        <is>
+          <t>Gothic spider nails 🕷️</t>
+        </is>
+      </c>
+      <c r="C699" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/baccmsn8acve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="700">
+      <c r="A700" t="inlineStr">
+        <is>
+          <t>1k15k5r</t>
+        </is>
+      </c>
+      <c r="B700" t="inlineStr">
+        <is>
+          <t>does anyone on here do press ons?</t>
+        </is>
+      </c>
+      <c r="C700" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k15k5r/does_anyone_on_here_do_press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="701">
+      <c r="A701" t="inlineStr">
+        <is>
+          <t>1k15emc</t>
+        </is>
+      </c>
+      <c r="B701" t="inlineStr">
+        <is>
+          <t>Best advice for beginner nail artists/aspiring nail artist who wants to go to nail school?</t>
+        </is>
+      </c>
+      <c r="C701" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k15emc/best_advice_for_beginner_nail_artistsaspiring/</t>
+        </is>
+      </c>
+    </row>
+    <row r="702">
+      <c r="A702" t="inlineStr">
+        <is>
+          <t>1k14qsu</t>
+        </is>
+      </c>
+      <c r="B702" t="inlineStr">
+        <is>
+          <t>Gel polish</t>
+        </is>
+      </c>
+      <c r="C702" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kxtfwen4tbve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="703">
+      <c r="A703" t="inlineStr">
+        <is>
+          <t>1k14f57</t>
+        </is>
+      </c>
+      <c r="B703" t="inlineStr">
+        <is>
+          <t>Starting get more creative with nails. Looking forward to working with my new nail tech more and see what we come up with.</t>
+        </is>
+      </c>
+      <c r="C703" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y8q9i2ejpbve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="704">
+      <c r="A704" t="inlineStr">
+        <is>
+          <t>1k14avv</t>
+        </is>
+      </c>
+      <c r="B704" t="inlineStr">
+        <is>
+          <t>My first two attempts at making press on nails!</t>
+        </is>
+      </c>
+      <c r="C704" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k14avv</t>
+        </is>
+      </c>
+    </row>
+    <row r="705">
+      <c r="A705" t="inlineStr">
+        <is>
+          <t>1k140wa</t>
+        </is>
+      </c>
+      <c r="B705" t="inlineStr">
+        <is>
+          <t>Long nails and bras???</t>
+        </is>
+      </c>
+      <c r="C705" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k140wa/long_nails_and_bras/</t>
+        </is>
+      </c>
+    </row>
+    <row r="706">
+      <c r="A706" t="inlineStr">
+        <is>
+          <t>1k13zpy</t>
+        </is>
+      </c>
+      <c r="B706" t="inlineStr">
+        <is>
+          <t>Think this is my best set so far!!</t>
+        </is>
+      </c>
+      <c r="C706" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k13zpy</t>
+        </is>
+      </c>
+    </row>
+    <row r="707">
+      <c r="A707" t="inlineStr">
+        <is>
+          <t>1k13y31</t>
+        </is>
+      </c>
+      <c r="B707" t="inlineStr">
+        <is>
+          <t>Advice needed</t>
+        </is>
+      </c>
+      <c r="C707" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k13y31/advice_needed/</t>
+        </is>
+      </c>
+    </row>
+    <row r="708">
+      <c r="A708" t="inlineStr">
+        <is>
+          <t>1k13urn</t>
+        </is>
+      </c>
+      <c r="B708" t="inlineStr">
+        <is>
+          <t>I did these myself ☺️</t>
+        </is>
+      </c>
+      <c r="C708" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/qx7uncwgjbve1</t>
+        </is>
+      </c>
+    </row>
+    <row r="709">
+      <c r="A709" t="inlineStr">
+        <is>
+          <t>1k13sfh</t>
+        </is>
+      </c>
+      <c r="B709" t="inlineStr">
+        <is>
+          <t>Got these for spring. Quite random.</t>
+        </is>
+      </c>
+      <c r="C709" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1nbce3iwibve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="710">
+      <c r="A710" t="inlineStr">
+        <is>
+          <t>1k13p1q</t>
+        </is>
+      </c>
+      <c r="B710" t="inlineStr">
+        <is>
+          <t>Free nails my friend did for me</t>
+        </is>
+      </c>
+      <c r="C710" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yutc2pvyhbve1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="711">
+      <c r="A711" t="inlineStr">
+        <is>
+          <t>1k13ka8</t>
+        </is>
+      </c>
+      <c r="B711" t="inlineStr">
+        <is>
+          <t>First diy freestyle extension set!!🎀</t>
+        </is>
+      </c>
+      <c r="C711" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k13ka8</t>
+        </is>
+      </c>
+    </row>
+    <row r="712">
+      <c r="A712" t="inlineStr">
+        <is>
+          <t>1k137d3</t>
+        </is>
+      </c>
+      <c r="B712" t="inlineStr">
+        <is>
+          <t>Absolutely love 💅🏻</t>
+        </is>
+      </c>
+      <c r="C712" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k137d3</t>
+        </is>
+      </c>
+    </row>
+    <row r="713">
+      <c r="A713" t="inlineStr">
+        <is>
+          <t>1k137bd</t>
+        </is>
+      </c>
+      <c r="B713" t="inlineStr">
+        <is>
+          <t>Semi-permanent, natural growth 💙👀</t>
+        </is>
+      </c>
+      <c r="C713" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/387wl322dbve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="714">
+      <c r="A714" t="inlineStr">
+        <is>
+          <t>1k12xic</t>
+        </is>
+      </c>
+      <c r="B714" t="inlineStr">
+        <is>
+          <t>My Coachella Naaaaails</t>
+        </is>
+      </c>
+      <c r="C714" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k12xic</t>
+        </is>
+      </c>
+    </row>
+    <row r="715">
+      <c r="A715" t="inlineStr">
+        <is>
+          <t>1k12n51</t>
+        </is>
+      </c>
+      <c r="B715" t="inlineStr">
+        <is>
+          <t>Silver Cateye with Chrome</t>
+        </is>
+      </c>
+      <c r="C715" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6csb3s7i7bve1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="716">
+      <c r="A716" t="inlineStr">
+        <is>
+          <t>1k125yd</t>
+        </is>
+      </c>
+      <c r="B716" t="inlineStr">
+        <is>
+          <t>got acrylic nails but it doesn’t look like it should underneath? is it gelx?</t>
+        </is>
+      </c>
+      <c r="C716" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2euuhzfz2bve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="717">
+      <c r="A717" t="inlineStr">
+        <is>
+          <t>1k0zkl2</t>
+        </is>
+      </c>
+      <c r="B717" t="inlineStr">
+        <is>
+          <t>Keyboard recommendations?</t>
+        </is>
+      </c>
+      <c r="C717" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cez468s9fave1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="718">
+      <c r="A718" t="inlineStr">
+        <is>
+          <t>1k104k5</t>
+        </is>
+      </c>
+      <c r="B718" t="inlineStr">
+        <is>
+          <t>How long to a decent nail bed recovery?</t>
+        </is>
+      </c>
+      <c r="C718" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k104k5</t>
+        </is>
+      </c>
+    </row>
+    <row r="719">
+      <c r="A719" t="inlineStr">
+        <is>
+          <t>1k10n5l</t>
+        </is>
+      </c>
+      <c r="B719" t="inlineStr">
+        <is>
+          <t>I’ve never had nails this long before 😩</t>
+        </is>
+      </c>
+      <c r="C719" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7x7ek9fvoave1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="720">
+      <c r="A720" t="inlineStr">
+        <is>
+          <t>1k10r3m</t>
+        </is>
+      </c>
+      <c r="B720" t="inlineStr">
+        <is>
+          <t>How to make my nail polish last longer than 2 days?</t>
+        </is>
+      </c>
+      <c r="C720" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k10r3m</t>
+        </is>
+      </c>
+    </row>
+    <row r="721">
+      <c r="A721" t="inlineStr">
+        <is>
+          <t>1k11txa</t>
+        </is>
+      </c>
+      <c r="B721" t="inlineStr">
+        <is>
+          <t>a little over a month ago, i posted my botched salon gel manicure on here. these are my nails now</t>
+        </is>
+      </c>
+      <c r="C721" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k11txa</t>
+        </is>
+      </c>
+    </row>
+    <row r="722">
+      <c r="A722" t="inlineStr">
+        <is>
+          <t>1k11s8m</t>
+        </is>
+      </c>
+      <c r="B722" t="inlineStr">
+        <is>
+          <t>Bless My Nail Tech</t>
+        </is>
+      </c>
+      <c r="C722" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k11s8m</t>
+        </is>
+      </c>
+    </row>
+    <row r="723">
+      <c r="A723" t="inlineStr">
+        <is>
+          <t>1k11ov8</t>
+        </is>
+      </c>
+      <c r="B723" t="inlineStr">
+        <is>
+          <t>does lash glue work for press on nails?</t>
+        </is>
+      </c>
+      <c r="C723" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k11ov8/does_lash_glue_work_for_press_on_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="724">
+      <c r="A724" t="inlineStr">
+        <is>
+          <t>1k11mlo</t>
+        </is>
+      </c>
+      <c r="B724" t="inlineStr">
+        <is>
+          <t>Gel vs Acrylic?</t>
+        </is>
+      </c>
+      <c r="C724" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k11mlo/gel_vs_acrylic/</t>
+        </is>
+      </c>
+    </row>
+    <row r="725">
+      <c r="A725" t="inlineStr">
+        <is>
+          <t>1k11540</t>
+        </is>
+      </c>
+      <c r="B725" t="inlineStr">
+        <is>
+          <t>Tried something different!</t>
+        </is>
+      </c>
+      <c r="C725" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k11540</t>
+        </is>
+      </c>
+    </row>
+    <row r="726">
+      <c r="A726" t="inlineStr">
+        <is>
+          <t>1k11477</t>
+        </is>
+      </c>
+      <c r="B726" t="inlineStr">
+        <is>
+          <t>Did Essie Mademoiselle change?!</t>
+        </is>
+      </c>
+      <c r="C726" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k11477</t>
+        </is>
+      </c>
+    </row>
+    <row r="727">
+      <c r="A727" t="inlineStr">
+        <is>
+          <t>1k110wy</t>
+        </is>
+      </c>
+      <c r="B727" t="inlineStr">
+        <is>
+          <t>🎀🎀🎀</t>
+        </is>
+      </c>
+      <c r="C727" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gxk8zgydsave1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="728">
+      <c r="A728" t="inlineStr">
+        <is>
+          <t>1k10v01</t>
+        </is>
+      </c>
+      <c r="B728" t="inlineStr">
+        <is>
+          <t>Rainbow 🌈</t>
+        </is>
+      </c>
+      <c r="C728" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zrt33x1wqave1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="729">
+      <c r="A729" t="inlineStr">
+        <is>
+          <t>1k10uq6</t>
+        </is>
+      </c>
+      <c r="B729" t="inlineStr">
+        <is>
+          <t>My girl is the best 😍</t>
+        </is>
+      </c>
+      <c r="C729" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2udokgltqave1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="730">
+      <c r="A730" t="inlineStr">
+        <is>
+          <t>1k10qcj</t>
+        </is>
+      </c>
+      <c r="B730" t="inlineStr">
+        <is>
+          <t>currently in nail school</t>
+        </is>
+      </c>
+      <c r="C730" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lre4d60ppave1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="731">
+      <c r="A731" t="inlineStr">
+        <is>
+          <t>1k10pcp</t>
+        </is>
+      </c>
+      <c r="B731" t="inlineStr">
+        <is>
+          <t>My first Nail design attempt</t>
+        </is>
+      </c>
+      <c r="C731" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dwafmtqfpave1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="732">
+      <c r="A732" t="inlineStr">
+        <is>
+          <t>1k10ovt</t>
+        </is>
+      </c>
+      <c r="B732" t="inlineStr">
+        <is>
+          <t>Y’all ever just give up on the nail art before finishing? Anyway enjoy my Easter nails</t>
+        </is>
+      </c>
+      <c r="C732" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k10ovt</t>
+        </is>
+      </c>
+    </row>
+    <row r="733">
+      <c r="A733" t="inlineStr">
+        <is>
+          <t>1k10cwr</t>
+        </is>
+      </c>
+      <c r="B733" t="inlineStr">
+        <is>
+          <t>How long does it take you to paint nails yourself? UV/LED</t>
+        </is>
+      </c>
+      <c r="C733" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k10cwr/how_long_does_it_take_you_to_paint_nails_yourself/</t>
+        </is>
+      </c>
+    </row>
+    <row r="734">
+      <c r="A734" t="inlineStr">
+        <is>
+          <t>1k104fw</t>
+        </is>
+      </c>
+      <c r="B734" t="inlineStr">
+        <is>
+          <t>Sobriety Nails</t>
+        </is>
+      </c>
+      <c r="C734" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9jwkad09kave1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="735">
+      <c r="A735" t="inlineStr">
+        <is>
+          <t>1k0zlp4</t>
+        </is>
+      </c>
+      <c r="B735" t="inlineStr">
+        <is>
+          <t>First tries</t>
+        </is>
+      </c>
+      <c r="C735" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2p6nkxwjfave1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="736">
+      <c r="A736" t="inlineStr">
+        <is>
+          <t>1k0yyae</t>
+        </is>
+      </c>
+      <c r="B736" t="inlineStr">
+        <is>
+          <t>I did some jinx inspired nails on myself, how'd I do? 🗣️💕</t>
+        </is>
+      </c>
+      <c r="C736" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k0yyae</t>
+        </is>
+      </c>
+    </row>
+    <row r="737">
+      <c r="A737" t="inlineStr">
+        <is>
+          <t>1k0zf88</t>
+        </is>
+      </c>
+      <c r="B737" t="inlineStr">
+        <is>
+          <t>Tie dye Easter eggs</t>
+        </is>
+      </c>
+      <c r="C737" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k0zf88</t>
+        </is>
+      </c>
+    </row>
+    <row r="738">
+      <c r="A738" t="inlineStr">
+        <is>
+          <t>1k0z2r5</t>
+        </is>
+      </c>
+      <c r="B738" t="inlineStr">
+        <is>
+          <t>What gel polish brand is best for press on nails?</t>
+        </is>
+      </c>
+      <c r="C738" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k0z2r5/what_gel_polish_brand_is_best_for_press_on_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="739">
+      <c r="A739" t="inlineStr">
+        <is>
+          <t>1k0z225</t>
+        </is>
+      </c>
+      <c r="B739" t="inlineStr">
+        <is>
+          <t>Has anyone seen anything like this?</t>
+        </is>
+      </c>
+      <c r="C739" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/smeqjylsaave1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="740">
+      <c r="A740" t="inlineStr">
+        <is>
+          <t>1k0z0p0</t>
+        </is>
+      </c>
+      <c r="B740" t="inlineStr">
+        <is>
+          <t>Nails of illuminated sky.</t>
+        </is>
+      </c>
+      <c r="C740" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jib793ogaave1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="741">
+      <c r="A741" t="inlineStr">
+        <is>
+          <t>1k0yemy</t>
+        </is>
+      </c>
+      <c r="B741" t="inlineStr">
+        <is>
+          <t>One nail bed smaller than rest</t>
+        </is>
+      </c>
+      <c r="C741" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k0yemy</t>
+        </is>
+      </c>
+    </row>
+    <row r="742">
+      <c r="A742" t="inlineStr">
+        <is>
+          <t>1k0xgwq</t>
+        </is>
+      </c>
+      <c r="B742" t="inlineStr">
+        <is>
+          <t>Help needed from press-on connoisseurs please!</t>
+        </is>
+      </c>
+      <c r="C742" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k0xgwq</t>
+        </is>
+      </c>
+    </row>
+    <row r="743">
+      <c r="A743" t="inlineStr">
+        <is>
+          <t>1k0y2ed</t>
+        </is>
+      </c>
+      <c r="B743" t="inlineStr">
+        <is>
+          <t>Vacation Nails 🌺</t>
+        </is>
+      </c>
+      <c r="C743" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/io7bt93d2ave1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="744">
+      <c r="A744" t="inlineStr">
+        <is>
+          <t>1k0y0uv</t>
+        </is>
+      </c>
+      <c r="B744" t="inlineStr">
+        <is>
+          <t>Quick cat-eye</t>
+        </is>
+      </c>
+      <c r="C744" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k0y0uv/quick_cateye/</t>
+        </is>
+      </c>
+    </row>
+    <row r="745">
+      <c r="A745" t="inlineStr">
+        <is>
+          <t>1k0xwyg</t>
+        </is>
+      </c>
+      <c r="B745" t="inlineStr">
+        <is>
+          <t>Loving my new set 🌙💖</t>
+        </is>
+      </c>
+      <c r="C745" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k0xwyg</t>
+        </is>
+      </c>
+    </row>
+    <row r="746">
+      <c r="A746" t="inlineStr">
+        <is>
+          <t>1k0xt65</t>
+        </is>
+      </c>
+      <c r="B746" t="inlineStr">
+        <is>
+          <t>Update: am I being too critical?</t>
+        </is>
+      </c>
+      <c r="C746" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vgw3j0970ave1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="747">
+      <c r="A747" t="inlineStr">
+        <is>
+          <t>1k0wxlo</t>
+        </is>
+      </c>
+      <c r="B747" t="inlineStr">
+        <is>
+          <t>NYC Nails! DIY at home.</t>
+        </is>
+      </c>
+      <c r="C747" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k0wxlo</t>
+        </is>
+      </c>
+    </row>
+    <row r="748">
+      <c r="A748" t="inlineStr">
+        <is>
+          <t>1k0wsjn</t>
+        </is>
+      </c>
+      <c r="B748" t="inlineStr">
+        <is>
+          <t>How’d I do? Just learning to do my own Gel Nails.</t>
+        </is>
+      </c>
+      <c r="C748" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zbuj3p42s9ve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="749">
+      <c r="A749" t="inlineStr">
+        <is>
+          <t>1k0wfk8</t>
+        </is>
+      </c>
+      <c r="B749" t="inlineStr">
+        <is>
+          <t>Easter egg skittle.</t>
+        </is>
+      </c>
+      <c r="C749" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k0wfk8</t>
+        </is>
+      </c>
+    </row>
+    <row r="750">
+      <c r="A750" t="inlineStr">
+        <is>
+          <t>1k0w6lz</t>
+        </is>
+      </c>
+      <c r="B750" t="inlineStr">
+        <is>
+          <t>Princess realness</t>
+        </is>
+      </c>
+      <c r="C750" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k0w6lz</t>
+        </is>
+      </c>
+    </row>
+    <row r="751">
+      <c r="A751" t="inlineStr">
+        <is>
+          <t>1k0vyyi</t>
+        </is>
+      </c>
+      <c r="B751" t="inlineStr">
+        <is>
+          <t>First time doing nail art – how did I do?</t>
+        </is>
+      </c>
+      <c r="C751" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k0vyyi</t>
+        </is>
+      </c>
+    </row>
+    <row r="752">
+      <c r="A752" t="inlineStr">
+        <is>
+          <t>1k0vser</t>
+        </is>
+      </c>
+      <c r="B752" t="inlineStr">
+        <is>
+          <t>How do I tell my nail tech I don’t like the color I picked?</t>
+        </is>
+      </c>
+      <c r="C752" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k0vser/how_do_i_tell_my_nail_tech_i_dont_like_the_color/</t>
+        </is>
+      </c>
+    </row>
+    <row r="753">
+      <c r="A753" t="inlineStr">
+        <is>
+          <t>1k0voq7</t>
+        </is>
+      </c>
+      <c r="B753" t="inlineStr">
+        <is>
+          <t>Springtime talons 🌷🐝✨</t>
+        </is>
+      </c>
+      <c r="C753" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/xafhidglj9ve1</t>
+        </is>
+      </c>
+    </row>
+    <row r="754">
+      <c r="A754" t="inlineStr">
+        <is>
+          <t>1k0vfaw</t>
+        </is>
+      </c>
+      <c r="B754" t="inlineStr">
+        <is>
+          <t>Has anyone tried Imperial Room Gel extensions at your salon?</t>
+        </is>
+      </c>
+      <c r="C754" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hey19hukh9ve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="755">
+      <c r="A755" t="inlineStr">
+        <is>
+          <t>1k0vew7</t>
+        </is>
+      </c>
+      <c r="B755" t="inlineStr">
+        <is>
+          <t>Green cat eye ✨</t>
+        </is>
+      </c>
+      <c r="C755" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/9f8nm1ngh9ve1</t>
+        </is>
+      </c>
+    </row>
+    <row r="756">
+      <c r="A756" t="inlineStr">
+        <is>
+          <t>1k0v4kb</t>
+        </is>
+      </c>
+      <c r="B756" t="inlineStr">
+        <is>
+          <t>My hands are dry, I have psoriasis, but love these extensions and cute flowers</t>
+        </is>
+      </c>
+      <c r="C756" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1y9h4mxcf9ve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="757">
+      <c r="A757" t="inlineStr">
+        <is>
+          <t>1k0usbi</t>
+        </is>
+      </c>
+      <c r="B757" t="inlineStr">
+        <is>
+          <t>First time getting nails</t>
+        </is>
+      </c>
+      <c r="C757" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k0usbi</t>
+        </is>
+      </c>
+    </row>
+    <row r="758">
+      <c r="A758" t="inlineStr">
+        <is>
+          <t>1k0ub1x</t>
+        </is>
+      </c>
+      <c r="B758" t="inlineStr">
+        <is>
+          <t>The dreaded derm….</t>
+        </is>
+      </c>
+      <c r="C758" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k0ub1x</t>
+        </is>
+      </c>
+    </row>
+    <row r="759">
+      <c r="A759" t="inlineStr">
+        <is>
+          <t>1k0u88w</t>
+        </is>
+      </c>
+      <c r="B759" t="inlineStr">
+        <is>
+          <t>Are SNS nails a good option?</t>
+        </is>
+      </c>
+      <c r="C759" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k0u88w/are_sns_nails_a_good_option/</t>
+        </is>
+      </c>
+    </row>
+    <row r="760">
+      <c r="A760" t="inlineStr">
+        <is>
+          <t>1k0u7xg</t>
+        </is>
+      </c>
+      <c r="B760" t="inlineStr">
+        <is>
+          <t>My tech killed it with this set 💅🏻</t>
+        </is>
+      </c>
+      <c r="C760" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xzzl3isj89ve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="761">
+      <c r="A761" t="inlineStr">
+        <is>
+          <t>1k0u3kg</t>
+        </is>
+      </c>
+      <c r="B761" t="inlineStr">
+        <is>
+          <t>My Easter/spring nails!!</t>
+        </is>
+      </c>
+      <c r="C761" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2mjd5kjq79ve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="762">
+      <c r="A762" t="inlineStr">
+        <is>
+          <t>1k0tlvr</t>
+        </is>
+      </c>
+      <c r="B762" t="inlineStr">
+        <is>
+          <t>Got a tequila mani for Mexico vacation. Swipe for inspo from @nailboss619</t>
+        </is>
+      </c>
+      <c r="C762" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k0tlvr</t>
+        </is>
+      </c>
+    </row>
+    <row r="763">
+      <c r="A763" t="inlineStr">
+        <is>
+          <t>1k0trc2</t>
+        </is>
+      </c>
+      <c r="B763" t="inlineStr">
+        <is>
+          <t>It will never be enough pink</t>
+        </is>
+      </c>
+      <c r="C763" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7uoflnpa59ve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="764">
+      <c r="A764" t="inlineStr">
+        <is>
+          <t>1k0tazo</t>
+        </is>
+      </c>
+      <c r="B764" t="inlineStr">
+        <is>
+          <t>another day another set</t>
+        </is>
+      </c>
+      <c r="C764" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pj3xs5hv19ve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="765">
+      <c r="A765" t="inlineStr">
+        <is>
+          <t>1k0t558</t>
+        </is>
+      </c>
+      <c r="B765" t="inlineStr">
+        <is>
+          <t>How to make gel stick better?</t>
+        </is>
+      </c>
+      <c r="C765" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k0t558/how_to_make_gel_stick_better/</t>
+        </is>
+      </c>
+    </row>
+    <row r="766">
+      <c r="A766" t="inlineStr">
+        <is>
+          <t>1k0szo9</t>
+        </is>
+      </c>
+      <c r="B766" t="inlineStr">
+        <is>
+          <t>How possible is it to DIY a gel manicure in 2 hours?</t>
+        </is>
+      </c>
+      <c r="C766" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k0szo9/how_possible_is_it_to_diy_a_gel_manicure_in_2/</t>
+        </is>
+      </c>
+    </row>
+    <row r="767">
+      <c r="A767" t="inlineStr">
+        <is>
+          <t>1k0sqsi</t>
+        </is>
+      </c>
+      <c r="B767" t="inlineStr">
+        <is>
+          <t>New press on set 🤍</t>
+        </is>
+      </c>
+      <c r="C767" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k0sqsi</t>
+        </is>
+      </c>
+    </row>
+    <row r="768">
+      <c r="A768" t="inlineStr">
+        <is>
+          <t>1k0sp73</t>
+        </is>
+      </c>
+      <c r="B768" t="inlineStr">
+        <is>
+          <t>Really proud of this set 🍊</t>
+        </is>
+      </c>
+      <c r="C768" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/76m7gtsex8ve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="769">
+      <c r="A769" t="inlineStr">
+        <is>
+          <t>1k0sjez</t>
+        </is>
+      </c>
+      <c r="B769" t="inlineStr">
+        <is>
+          <t>Felt like spring</t>
+        </is>
+      </c>
+      <c r="C769" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k0sjez</t>
+        </is>
+      </c>
+    </row>
+    <row r="770">
+      <c r="A770" t="inlineStr">
+        <is>
+          <t>1k0sepj</t>
+        </is>
+      </c>
+      <c r="B770" t="inlineStr">
+        <is>
+          <t>The best art i've ever done 💕🌙</t>
+        </is>
+      </c>
+      <c r="C770" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k0sepj</t>
+        </is>
+      </c>
+    </row>
+    <row r="771">
+      <c r="A771" t="inlineStr">
+        <is>
+          <t>1k0sd2l</t>
+        </is>
+      </c>
+      <c r="B771" t="inlineStr">
+        <is>
+          <t>On Wednesdays we do pink</t>
+        </is>
+      </c>
+      <c r="C771" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lk204d6wu8ve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="772">
+      <c r="A772" t="inlineStr">
+        <is>
+          <t>1k0s7jv</t>
+        </is>
+      </c>
+      <c r="B772" t="inlineStr">
+        <is>
+          <t>Is this what jelly nails are supposed to look like?</t>
+        </is>
+      </c>
+      <c r="C772" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k0s7jv</t>
+        </is>
+      </c>
+    </row>
+    <row r="773">
+      <c r="A773" t="inlineStr">
+        <is>
+          <t>1k0s5rt</t>
+        </is>
+      </c>
+      <c r="B773" t="inlineStr">
+        <is>
+          <t>Natural nail Confusion</t>
+        </is>
+      </c>
+      <c r="C773" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k0s5rt/natural_nail_confusion/</t>
+        </is>
+      </c>
+    </row>
+    <row r="774">
+      <c r="A774" t="inlineStr">
+        <is>
+          <t>1k0rrvz</t>
+        </is>
+      </c>
+      <c r="B774" t="inlineStr">
+        <is>
+          <t>Nail tech over filled my nails. Should I change nail tech or should I just talk to her?</t>
+        </is>
+      </c>
+      <c r="C774" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k0rrvz/nail_tech_over_filled_my_nails_should_i_change/</t>
+        </is>
+      </c>
+    </row>
+    <row r="775">
+      <c r="A775" t="inlineStr">
+        <is>
+          <t>1k0rz0x</t>
+        </is>
+      </c>
+      <c r="B775" t="inlineStr">
+        <is>
+          <t>Dreamy nails ☁️ 🦋</t>
+        </is>
+      </c>
+      <c r="C775" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k0rz0x</t>
+        </is>
+      </c>
+    </row>
+    <row r="776">
+      <c r="A776" t="inlineStr">
+        <is>
+          <t>1k0rsmu</t>
+        </is>
+      </c>
+      <c r="B776" t="inlineStr">
+        <is>
+          <t>Should i have these redone?</t>
+        </is>
+      </c>
+      <c r="C776" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k0rsmu</t>
+        </is>
+      </c>
+    </row>
+    <row r="777">
+      <c r="A777" t="inlineStr">
+        <is>
+          <t>1k0rroa</t>
+        </is>
+      </c>
+      <c r="B777" t="inlineStr">
+        <is>
+          <t>In love with my first spring themed manicure!</t>
+        </is>
+      </c>
+      <c r="C777" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xan217elq8ve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="778">
+      <c r="A778" t="inlineStr">
+        <is>
+          <t>1k0rmii</t>
+        </is>
+      </c>
+      <c r="B778" t="inlineStr">
+        <is>
+          <t>Gave into the butter yellow trend :)</t>
+        </is>
+      </c>
+      <c r="C778" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/js3bvfgjp8ve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="779">
+      <c r="A779" t="inlineStr">
+        <is>
+          <t>1k0rkz7</t>
+        </is>
+      </c>
+      <c r="B779" t="inlineStr">
+        <is>
+          <t>Can anyone tell me what’s happening with my nails?</t>
+        </is>
+      </c>
+      <c r="C779" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/90gr2co8p8ve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="780">
+      <c r="A780" t="inlineStr">
+        <is>
+          <t>1k0r4e2</t>
+        </is>
+      </c>
+      <c r="B780" t="inlineStr">
+        <is>
+          <t>Stand Proud</t>
+        </is>
+      </c>
+      <c r="C780" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t4unuk3nl8ve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="781">
+      <c r="A781" t="inlineStr">
+        <is>
+          <t>1k0r3sd</t>
+        </is>
+      </c>
+      <c r="B781" t="inlineStr">
+        <is>
+          <t>Blueberry nails!</t>
+        </is>
+      </c>
+      <c r="C781" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fxxl3okrl8ve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="782">
+      <c r="A782" t="inlineStr">
+        <is>
+          <t>1k0qpbg</t>
+        </is>
+      </c>
+      <c r="B782" t="inlineStr">
+        <is>
+          <t>Can't get a refund what should I do?</t>
+        </is>
+      </c>
+      <c r="C782" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k0qpbg</t>
+        </is>
+      </c>
+    </row>
+    <row r="783">
+      <c r="A783" t="inlineStr">
+        <is>
+          <t>1k0qgzs</t>
+        </is>
+      </c>
+      <c r="B783" t="inlineStr">
+        <is>
+          <t>Blue Nails</t>
+        </is>
+      </c>
+      <c r="C783" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wrwxb35ah8ve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="784">
+      <c r="A784" t="inlineStr">
+        <is>
+          <t>1k0qfs7</t>
+        </is>
+      </c>
+      <c r="B784" t="inlineStr">
+        <is>
+          <t>First time trying cat eye gel polish! The technician called these mermaid colours 🧜🏼‍♀️</t>
+        </is>
+      </c>
+      <c r="C784" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sgreo481h8ve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="785">
+      <c r="A785" t="inlineStr">
+        <is>
+          <t>1k0q8hq</t>
+        </is>
+      </c>
+      <c r="B785" t="inlineStr">
+        <is>
+          <t>Builder, Glue, Polish, Oh My!</t>
+        </is>
+      </c>
+      <c r="C785" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k0q8hq/builder_glue_polish_oh_my/</t>
+        </is>
+      </c>
+    </row>
+    <row r="786">
+      <c r="A786" t="inlineStr">
+        <is>
+          <t>1k0puu2</t>
+        </is>
+      </c>
+      <c r="B786" t="inlineStr">
+        <is>
+          <t>A little classic, I know. but this is the first time I use nails... what color do you suggest?</t>
+        </is>
+      </c>
+      <c r="C786" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k0puu2</t>
+        </is>
+      </c>
+    </row>
+    <row r="787">
+      <c r="A787" t="inlineStr">
+        <is>
+          <t>1k0pt3j</t>
+        </is>
+      </c>
+      <c r="B787" t="inlineStr">
+        <is>
+          <t>Garden fairy set I did!</t>
+        </is>
+      </c>
+      <c r="C787" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k0pt3j</t>
+        </is>
+      </c>
+    </row>
+    <row r="788">
+      <c r="A788" t="inlineStr">
+        <is>
+          <t>1k0pquy</t>
+        </is>
+      </c>
+      <c r="B788" t="inlineStr">
+        <is>
+          <t>trouble pricing press ons nails please help!</t>
+        </is>
+      </c>
+      <c r="C788" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bxfqrzc5c8ve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="789">
+      <c r="A789" t="inlineStr">
+        <is>
+          <t>1k0obkf</t>
+        </is>
+      </c>
+      <c r="B789" t="inlineStr">
+        <is>
+          <t>How to make regular polish last longer?</t>
+        </is>
+      </c>
+      <c r="C789" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k0obkf/how_to_make_regular_polish_last_longer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="790">
+      <c r="A790" t="inlineStr">
+        <is>
+          <t>1k16t9d</t>
+        </is>
+      </c>
+      <c r="B790" t="inlineStr">
+        <is>
+          <t>Non-gel "jelly" polish recommendations?</t>
+        </is>
+      </c>
+      <c r="C790" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k16t9d</t>
+        </is>
+      </c>
+    </row>
+    <row r="791">
+      <c r="A791" t="inlineStr">
+        <is>
+          <t>1k0yd7j</t>
+        </is>
+      </c>
+      <c r="B791" t="inlineStr">
+        <is>
+          <t>Nail topper</t>
+        </is>
+      </c>
+      <c r="C791" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/98mgfb5t4ave1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="792">
+      <c r="A792" t="inlineStr">
+        <is>
+          <t>1k15eco</t>
+        </is>
+      </c>
+      <c r="B792" t="inlineStr">
+        <is>
+          <t>the skye's the limit</t>
+        </is>
+      </c>
+      <c r="C792" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/p3vdmpgs0cve1</t>
+        </is>
+      </c>
+    </row>
+    <row r="793">
+      <c r="A793" t="inlineStr">
+        <is>
+          <t>1k13s31</t>
+        </is>
+      </c>
+      <c r="B793" t="inlineStr">
+        <is>
+          <t>Mooncat dupes</t>
+        </is>
+      </c>
+      <c r="C793" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k13s31</t>
+        </is>
+      </c>
+    </row>
+    <row r="794">
+      <c r="A794" t="inlineStr">
+        <is>
+          <t>1k13nrn</t>
+        </is>
+      </c>
+      <c r="B794" t="inlineStr">
+        <is>
+          <t>My Lurid Lacquer Cart🥰</t>
+        </is>
+      </c>
+      <c r="C794" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zrto8hzlhbve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="795">
+      <c r="A795" t="inlineStr">
+        <is>
+          <t>1k1324x</t>
+        </is>
+      </c>
+      <c r="B795" t="inlineStr">
+        <is>
+          <t>Different Versions of Malaga Wine?</t>
+        </is>
+      </c>
+      <c r="C795" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l1g70xylbbve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="796">
+      <c r="A796" t="inlineStr">
+        <is>
+          <t>1k12lh3</t>
+        </is>
+      </c>
+      <c r="B796" t="inlineStr">
+        <is>
+          <t>Minimalist / Quick Nailcare?</t>
+        </is>
+      </c>
+      <c r="C796" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k12lh3/minimalist_quick_nailcare/</t>
+        </is>
+      </c>
+    </row>
+    <row r="797">
+      <c r="A797" t="inlineStr">
+        <is>
+          <t>1k12lcf</t>
+        </is>
+      </c>
+      <c r="B797" t="inlineStr">
+        <is>
+          <t>mooncat fields of elysium vs. garden of evil?</t>
+        </is>
+      </c>
+      <c r="C797" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k12lcf/mooncat_fields_of_elysium_vs_garden_of_evil/</t>
+        </is>
+      </c>
+    </row>
+    <row r="798">
+      <c r="A798" t="inlineStr">
+        <is>
+          <t>1k10a85</t>
+        </is>
+      </c>
+      <c r="B798" t="inlineStr">
+        <is>
+          <t>I successfully defended my PhD today 🥹 Dr squelseaa at your service</t>
+        </is>
+      </c>
+      <c r="C798" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k10a85</t>
+        </is>
+      </c>
+    </row>
+    <row r="799">
+      <c r="A799" t="inlineStr">
+        <is>
+          <t>1k0zqi6</t>
+        </is>
+      </c>
+      <c r="B799" t="inlineStr">
+        <is>
+          <t>Your favorite iridescent greige polish?</t>
+        </is>
+      </c>
+      <c r="C799" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k0zqi6/your_favorite_iridescent_greige_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="800">
+      <c r="A800" t="inlineStr">
+        <is>
+          <t>1k0zbg4</t>
+        </is>
+      </c>
+      <c r="B800" t="inlineStr">
+        <is>
+          <t>💚Green Dotted Skittle💚</t>
+        </is>
+      </c>
+      <c r="C800" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k0zbg4</t>
+        </is>
+      </c>
+    </row>
+    <row r="801">
+      <c r="A801" t="inlineStr">
+        <is>
+          <t>1k0z1tb</t>
+        </is>
+      </c>
+      <c r="B801" t="inlineStr">
+        <is>
+          <t>very whimsy very goth🧚‍♂️🖤</t>
+        </is>
+      </c>
+      <c r="C801" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k0z1tb</t>
+        </is>
+      </c>
+    </row>
+    <row r="802">
+      <c r="A802" t="inlineStr">
+        <is>
+          <t>1k0z0ep</t>
+        </is>
+      </c>
+      <c r="B802" t="inlineStr">
+        <is>
+          <t>ILNP Ritual</t>
+        </is>
+      </c>
+      <c r="C802" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/9766km7daave1</t>
+        </is>
+      </c>
+    </row>
+    <row r="803">
+      <c r="A803" t="inlineStr">
+        <is>
+          <t>1k0xl4n</t>
+        </is>
+      </c>
+      <c r="B803" t="inlineStr">
+        <is>
+          <t>Gloomy weather, bright nails</t>
+        </is>
+      </c>
+      <c r="C803" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k0xl4n</t>
+        </is>
+      </c>
+    </row>
+    <row r="804">
+      <c r="A804" t="inlineStr">
+        <is>
+          <t>1k0xf43</t>
+        </is>
+      </c>
+      <c r="B804" t="inlineStr">
+        <is>
+          <t>Best QDTC for durability</t>
+        </is>
+      </c>
+      <c r="C804" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k0xf43/best_qdtc_for_durability/</t>
+        </is>
+      </c>
+    </row>
+    <row r="805">
+      <c r="A805" t="inlineStr">
+        <is>
+          <t>1k0xebj</t>
+        </is>
+      </c>
+      <c r="B805" t="inlineStr">
+        <is>
+          <t>Any idea what color she’s wearing? 🤭</t>
+        </is>
+      </c>
+      <c r="C805" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oriibo4vw9ve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="806">
+      <c r="A806" t="inlineStr">
+        <is>
+          <t>1k0x056</t>
+        </is>
+      </c>
+      <c r="B806" t="inlineStr">
+        <is>
+          <t>Guess the polish</t>
+        </is>
+      </c>
+      <c r="C806" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k0x056</t>
+        </is>
+      </c>
+    </row>
+    <row r="807">
+      <c r="A807" t="inlineStr">
+        <is>
+          <t>1k0wva2</t>
+        </is>
+      </c>
+      <c r="B807" t="inlineStr">
+        <is>
+          <t>Lumen - Aquarius or Capricorn Mystery Sets</t>
+        </is>
+      </c>
+      <c r="C807" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k0wva2/lumen_aquarius_or_capricorn_mystery_sets/</t>
+        </is>
+      </c>
+    </row>
+    <row r="808">
+      <c r="A808" t="inlineStr">
+        <is>
+          <t>1k0wb46</t>
+        </is>
+      </c>
+      <c r="B808" t="inlineStr">
+        <is>
+          <t>Easter egg skittles</t>
+        </is>
+      </c>
+      <c r="C808" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k0wb46</t>
+        </is>
+      </c>
+    </row>
+    <row r="809">
+      <c r="A809" t="inlineStr">
+        <is>
+          <t>1k0wa1p</t>
+        </is>
+      </c>
+      <c r="B809" t="inlineStr">
+        <is>
+          <t>Spring sparkle ✨</t>
+        </is>
+      </c>
+      <c r="C809" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k0wa1p</t>
+        </is>
+      </c>
+    </row>
+    <row r="810">
+      <c r="A810" t="inlineStr">
+        <is>
+          <t>1k0vfhu</t>
+        </is>
+      </c>
+      <c r="B810" t="inlineStr">
+        <is>
+          <t>Does anyone have a swatch of both LBShimmer’s Tricked Out and HoloTaco’s Cat’s Evasion?</t>
+        </is>
+      </c>
+      <c r="C810" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k0vfhu/does_anyone_have_a_swatch_of_both_lbshimmers/</t>
+        </is>
+      </c>
+    </row>
+    <row r="811">
+      <c r="A811" t="inlineStr">
+        <is>
+          <t>1k0pjvi</t>
+        </is>
+      </c>
+      <c r="B811" t="inlineStr">
+        <is>
+          <t>So Fiery ❤️😍🔥 Mooncat Pandemonium</t>
+        </is>
+      </c>
+      <c r="C811" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k0pjvi</t>
+        </is>
+      </c>
+    </row>
+    <row r="812">
+      <c r="A812" t="inlineStr">
+        <is>
+          <t>1k0uo3b</t>
+        </is>
+      </c>
+      <c r="B812" t="inlineStr">
+        <is>
+          <t>My First Sassy Sauce Cart. Missing anything essential? Too much of the same? (I clearly have a type.)</t>
+        </is>
+      </c>
+      <c r="C812" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/886k0mazb9ve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="813">
+      <c r="A813" t="inlineStr">
+        <is>
+          <t>1k0tuhj</t>
+        </is>
+      </c>
+      <c r="B813" t="inlineStr">
+        <is>
+          <t>Sapphires on my nails</t>
+        </is>
+      </c>
+      <c r="C813" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/m17ogs8v59ve1</t>
+        </is>
+      </c>
+    </row>
+    <row r="814">
+      <c r="A814" t="inlineStr">
+        <is>
+          <t>1k0ttf2</t>
+        </is>
+      </c>
+      <c r="B814" t="inlineStr">
+        <is>
+          <t>Need thoughts/suggestions</t>
+        </is>
+      </c>
+      <c r="C814" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/txvu4uiq59ve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="815">
+      <c r="A815" t="inlineStr">
+        <is>
+          <t>1k0t4gc</t>
+        </is>
+      </c>
+      <c r="B815" t="inlineStr">
+        <is>
+          <t>Cirque Colors’ Rose Quartz dupe?</t>
+        </is>
+      </c>
+      <c r="C815" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k23zkprj09ve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="816">
+      <c r="A816" t="inlineStr">
+        <is>
+          <t>1k0snsa</t>
+        </is>
+      </c>
+      <c r="B816" t="inlineStr">
+        <is>
+          <t>China Glaze Coming to Ulta 4/20</t>
+        </is>
+      </c>
+      <c r="C816" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lhi1ygd4x8ve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="817">
+      <c r="A817" t="inlineStr">
+        <is>
+          <t>1k0slhn</t>
+        </is>
+      </c>
+      <c r="B817" t="inlineStr">
+        <is>
+          <t>Nail art first attempt</t>
+        </is>
+      </c>
+      <c r="C817" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k0slhn</t>
+        </is>
+      </c>
+    </row>
+    <row r="818">
+      <c r="A818" t="inlineStr">
+        <is>
+          <t>1k0rkke</t>
+        </is>
+      </c>
+      <c r="B818" t="inlineStr">
+        <is>
+          <t>🎰🎰🎰</t>
+        </is>
+      </c>
+      <c r="C818" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k0rkke</t>
+        </is>
+      </c>
+    </row>
+    <row r="819">
+      <c r="A819" t="inlineStr">
+        <is>
+          <t>1k0riiz</t>
+        </is>
+      </c>
+      <c r="B819" t="inlineStr">
+        <is>
+          <t>Serpents of Eden or Shift in Perception</t>
+        </is>
+      </c>
+      <c r="C819" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k0riiz</t>
+        </is>
+      </c>
+    </row>
+    <row r="820">
+      <c r="A820" t="inlineStr">
+        <is>
+          <t>1k0rgw4</t>
+        </is>
+      </c>
+      <c r="B820" t="inlineStr">
+        <is>
+          <t>Glow big or glow home!! ☢️☢️☢️☢️</t>
+        </is>
+      </c>
+      <c r="C820" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k0rgw4</t>
+        </is>
+      </c>
+    </row>
+    <row r="821">
+      <c r="A821" t="inlineStr">
+        <is>
+          <t>1k0qnvg</t>
+        </is>
+      </c>
+      <c r="B821" t="inlineStr">
+        <is>
+          <t>Before I dupe myself with this new Lurid haul....</t>
+        </is>
+      </c>
+      <c r="C821" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m3kplmnni8ve1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="822">
+      <c r="A822" t="inlineStr">
+        <is>
+          <t>1k0ql9l</t>
+        </is>
+      </c>
+      <c r="B822" t="inlineStr">
+        <is>
+          <t>Clear magnetic topper recommendations?</t>
+        </is>
+      </c>
+      <c r="C822" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x5b8fb44i8ve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="823">
+      <c r="A823" t="inlineStr">
+        <is>
+          <t>1k0qb7y</t>
+        </is>
+      </c>
+      <c r="B823" t="inlineStr">
+        <is>
+          <t>ISO Battle of the black/red multichromes</t>
+        </is>
+      </c>
+      <c r="C823" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k0qb7y/iso_battle_of_the_blackred_multichromes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="824">
+      <c r="A824" t="inlineStr">
+        <is>
+          <t>1k0q35g</t>
+        </is>
+      </c>
+      <c r="B824" t="inlineStr">
+        <is>
+          <t>How do I make my edges cleaner?</t>
+        </is>
+      </c>
+      <c r="C824" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k0q35g</t>
+        </is>
+      </c>
+    </row>
+    <row r="825">
+      <c r="A825" t="inlineStr">
+        <is>
+          <t>1k0orv3</t>
+        </is>
+      </c>
+      <c r="B825" t="inlineStr">
+        <is>
+          <t>Cleaning the brush that is in a bottle of polish you still use?</t>
+        </is>
+      </c>
+      <c r="C825" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k0orv3/cleaning_the_brush_that_is_in_a_bottle_of_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="826">
+      <c r="A826" t="inlineStr">
+        <is>
+          <t>1k0pe21</t>
+        </is>
+      </c>
+      <c r="B826" t="inlineStr">
+        <is>
+          <t>What topper would you use over Twilight Sonata?</t>
+        </is>
+      </c>
+      <c r="C826" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/18wxonaq98ve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="827">
+      <c r="A827" t="inlineStr">
+        <is>
+          <t>1k0pdop</t>
+        </is>
+      </c>
+      <c r="B827" t="inlineStr">
+        <is>
+          <t>In my 🌟glowy🌟era</t>
+        </is>
+      </c>
+      <c r="C827" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1sl8tyln98ve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="828">
+      <c r="A828" t="inlineStr">
+        <is>
+          <t>1k0p8r0</t>
+        </is>
+      </c>
+      <c r="B828" t="inlineStr">
+        <is>
+          <t>Looking for a dupe of sinful colors spring fling</t>
+        </is>
+      </c>
+      <c r="C828" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k0p8r0</t>
+        </is>
+      </c>
+    </row>
+    <row r="829">
+      <c r="A829" t="inlineStr">
+        <is>
+          <t>1k0oxse</t>
+        </is>
+      </c>
+      <c r="B829" t="inlineStr">
+        <is>
+          <t>Bread and butterflies 🍞🧈🦋</t>
+        </is>
+      </c>
+      <c r="C829" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ygcw490g68ve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="830">
+      <c r="A830" t="inlineStr">
+        <is>
+          <t>1k0ondd</t>
+        </is>
+      </c>
+      <c r="B830" t="inlineStr">
+        <is>
+          <t>Will there be other sales in the next few weeks?</t>
+        </is>
+      </c>
+      <c r="C830" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k0ondd/will_there_be_other_sales_in_the_next_few_weeks/</t>
+        </is>
+      </c>
+    </row>
+    <row r="831">
+      <c r="A831" t="inlineStr">
+        <is>
+          <t>1k0on40</t>
+        </is>
+      </c>
+      <c r="B831" t="inlineStr">
+        <is>
+          <t>💜</t>
+        </is>
+      </c>
+      <c r="C831" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k0on40</t>
+        </is>
+      </c>
+    </row>
+    <row r="832">
+      <c r="A832" t="inlineStr">
+        <is>
+          <t>1k0oj6t</t>
+        </is>
+      </c>
+      <c r="B832" t="inlineStr">
+        <is>
+          <t>Bug approved</t>
+        </is>
+      </c>
+      <c r="C832" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yqv25jsf38ve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="833">
+      <c r="A833" t="inlineStr">
+        <is>
+          <t>1k0nx7e</t>
+        </is>
+      </c>
+      <c r="B833" t="inlineStr">
+        <is>
+          <t>PSA: marble nails are easier than they look 😍</t>
+        </is>
+      </c>
+      <c r="C833" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8t051iiyy7ve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="834">
+      <c r="A834" t="inlineStr">
+        <is>
+          <t>1k0nv1t</t>
+        </is>
+      </c>
+      <c r="B834" t="inlineStr">
+        <is>
+          <t>Regular manicure strong base? Thick like builder gel?</t>
+        </is>
+      </c>
+      <c r="C834" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k0nv1t/regular_manicure_strong_base_thick_like_builder/</t>
+        </is>
+      </c>
+    </row>
+    <row r="835">
+      <c r="A835" t="inlineStr">
+        <is>
+          <t>1k0n1a6</t>
+        </is>
+      </c>
+      <c r="B835" t="inlineStr">
+        <is>
+          <t>Clionadh Cosmetics - Dreamscape</t>
+        </is>
+      </c>
+      <c r="C835" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k0n1a6</t>
+        </is>
+      </c>
+    </row>
+    <row r="836">
+      <c r="A836" t="inlineStr">
+        <is>
+          <t>1k0mzs6</t>
+        </is>
+      </c>
+      <c r="B836" t="inlineStr">
+        <is>
+          <t>Butterfly wings and glitter 🦋✨️</t>
+        </is>
+      </c>
+      <c r="C836" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x6ahxdszr7ve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="837">
+      <c r="A837" t="inlineStr">
+        <is>
+          <t>1k0mprh</t>
+        </is>
+      </c>
+      <c r="B837" t="inlineStr">
+        <is>
+          <t>Clionadh is having a sale tomorrow</t>
+        </is>
+      </c>
+      <c r="C837" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t9jd1apwp7ve1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="838">
+      <c r="A838" t="inlineStr">
+        <is>
+          <t>1k0mp3x</t>
+        </is>
+      </c>
+      <c r="B838" t="inlineStr">
+        <is>
+          <t>Incognito magnetics</t>
+        </is>
+      </c>
+      <c r="C838" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k0mp3x/incognito_magnetics/</t>
+        </is>
+      </c>
+    </row>
+    <row r="839">
+      <c r="A839" t="inlineStr">
+        <is>
+          <t>1k0mnp2</t>
+        </is>
+      </c>
+      <c r="B839" t="inlineStr">
+        <is>
+          <t>She glows 💜</t>
+        </is>
+      </c>
+      <c r="C839" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j36p2zwgp7ve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="840">
+      <c r="A840" t="inlineStr">
+        <is>
+          <t>1k0m6nv</t>
+        </is>
+      </c>
+      <c r="B840" t="inlineStr">
+        <is>
+          <t>Has anyone experienced fading with neons?</t>
+        </is>
+      </c>
+      <c r="C840" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k0m6nv/has_anyone_experienced_fading_with_neons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="841">
+      <c r="A841" t="inlineStr">
+        <is>
+          <t>1k0m003</t>
+        </is>
+      </c>
+      <c r="B841" t="inlineStr">
+        <is>
+          <t>Collapsing Clouds☁️🌤️⛈️🌩️</t>
+        </is>
+      </c>
+      <c r="C841" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k0m003</t>
+        </is>
+      </c>
+    </row>
+    <row r="842">
+      <c r="A842" t="inlineStr">
+        <is>
+          <t>1k0lzdn</t>
+        </is>
+      </c>
+      <c r="B842" t="inlineStr">
+        <is>
+          <t>Dany Vianna and KBShimmer clearly on top not playing well together?</t>
+        </is>
+      </c>
+      <c r="C842" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k0lzdn/dany_vianna_and_kbshimmer_clearly_on_top_not/</t>
+        </is>
+      </c>
+    </row>
+    <row r="843">
+      <c r="A843" t="inlineStr">
+        <is>
+          <t>1k0ldng</t>
+        </is>
+      </c>
+      <c r="B843" t="inlineStr">
+        <is>
+          <t>Dupe for sally hansen hue there?</t>
+        </is>
+      </c>
+      <c r="C843" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/195ixnnuf7ve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="844">
+      <c r="A844" t="inlineStr">
+        <is>
+          <t>1k0lc29</t>
+        </is>
+      </c>
+      <c r="B844" t="inlineStr">
+        <is>
+          <t>Fierce mojo</t>
+        </is>
+      </c>
+      <c r="C844" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/37szbrngf7ve1</t>
+        </is>
+      </c>
+    </row>
+    <row r="845">
+      <c r="A845" t="inlineStr">
+        <is>
+          <t>1k0l013</t>
+        </is>
+      </c>
+      <c r="B845" t="inlineStr">
+        <is>
+          <t>Water Lily nails in front of Monet's Water Lilies</t>
+        </is>
+      </c>
+      <c r="C845" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k0l013</t>
+        </is>
+      </c>
+    </row>
+    <row r="846">
+      <c r="A846" t="inlineStr">
+        <is>
+          <t>1k0hqt7</t>
+        </is>
+      </c>
+      <c r="B846" t="inlineStr">
+        <is>
+          <t>L.A. Colors - Mermaid Mist</t>
+        </is>
+      </c>
+      <c r="C846" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k0hqt7</t>
+        </is>
+      </c>
+    </row>
+    <row r="847">
+      <c r="A847" t="inlineStr">
+        <is>
+          <t>1k0iuw0</t>
+        </is>
+      </c>
+      <c r="B847" t="inlineStr">
+        <is>
+          <t>Bridezilla needs your recos</t>
+        </is>
+      </c>
+      <c r="C847" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/npu1g90ju6ve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="848">
+      <c r="A848" t="inlineStr">
+        <is>
+          <t>1k0kgdx</t>
+        </is>
+      </c>
+      <c r="B848" t="inlineStr">
+        <is>
+          <t>What nails for what events</t>
+        </is>
+      </c>
+      <c r="C848" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k0kgdx/what_nails_for_what_events/</t>
+        </is>
+      </c>
+    </row>
+    <row r="849">
+      <c r="A849" t="inlineStr">
+        <is>
+          <t>1k0k97b</t>
+        </is>
+      </c>
+      <c r="B849" t="inlineStr">
+        <is>
+          <t>Mooncat lid/brush replacement?</t>
+        </is>
+      </c>
+      <c r="C849" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k0k97b/mooncat_lidbrush_replacement/</t>
+        </is>
+      </c>
+    </row>
+    <row r="850">
+      <c r="A850" t="inlineStr">
+        <is>
+          <t>1k0it14</t>
+        </is>
+      </c>
+      <c r="B850" t="inlineStr">
+        <is>
+          <t>Cassiopeia ❤️</t>
+        </is>
+      </c>
+      <c r="C850" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/w0b9qtt0u6ve1</t>
+        </is>
+      </c>
+    </row>
+    <row r="851">
+      <c r="A851" t="inlineStr">
+        <is>
+          <t>1k0iqkl</t>
+        </is>
+      </c>
+      <c r="B851" t="inlineStr">
+        <is>
+          <t>OPI Did you see those mussels?</t>
+        </is>
+      </c>
+      <c r="C851" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k0iqkl</t>
+        </is>
+      </c>
+    </row>
+    <row r="852">
+      <c r="A852" t="inlineStr">
+        <is>
+          <t>1k0i90o</t>
+        </is>
+      </c>
+      <c r="B852" t="inlineStr">
+        <is>
+          <t>Nail artists: what are your game-changers?</t>
+        </is>
+      </c>
+      <c r="C852" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pbe7jk7oo6ve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="853">
+      <c r="A853" t="inlineStr">
+        <is>
+          <t>1k0hhic</t>
+        </is>
+      </c>
+      <c r="B853" t="inlineStr">
+        <is>
+          <t>good japanese brands?</t>
+        </is>
+      </c>
+      <c r="C853" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k0hhic/good_japanese_brands/</t>
+        </is>
+      </c>
+    </row>
+    <row r="854">
+      <c r="A854" t="inlineStr">
+        <is>
+          <t>1k0f8u6</t>
+        </is>
+      </c>
+      <c r="B854" t="inlineStr">
+        <is>
+          <t>Commiserate with me for I am a fool: bought before the Mooncat sale 🌙🤦🏻‍♀️</t>
+        </is>
+      </c>
+      <c r="C854" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k0f8u6/commiserate_with_me_for_i_am_a_fool_bought_before/</t>
+        </is>
+      </c>
+    </row>
+    <row r="855">
+      <c r="A855" t="inlineStr">
+        <is>
+          <t>1k14vib</t>
+        </is>
+      </c>
+      <c r="B855" t="inlineStr">
+        <is>
+          <t>French Cheat finally!!!</t>
+        </is>
+      </c>
+      <c r="C855" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vcfmqttmubve1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="856">
+      <c r="A856" t="inlineStr">
+        <is>
+          <t>1k14o95</t>
+        </is>
+      </c>
+      <c r="B856" t="inlineStr">
+        <is>
+          <t>Today I did this beautiful work</t>
+        </is>
+      </c>
+      <c r="C856" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k14o95</t>
+        </is>
+      </c>
+    </row>
+    <row r="857">
+      <c r="A857" t="inlineStr">
+        <is>
+          <t>1k1280w</t>
+        </is>
+      </c>
+      <c r="B857" t="inlineStr">
+        <is>
+          <t>Rave Nails</t>
+        </is>
+      </c>
+      <c r="C857" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k1280w</t>
+        </is>
+      </c>
+    </row>
+    <row r="858">
+      <c r="A858" t="inlineStr">
+        <is>
+          <t>1k11wp6</t>
+        </is>
+      </c>
+      <c r="B858" t="inlineStr">
+        <is>
+          <t>I finished the set!</t>
+        </is>
+      </c>
+      <c r="C858" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k11wp6</t>
+        </is>
+      </c>
+    </row>
+    <row r="859">
+      <c r="A859" t="inlineStr">
+        <is>
+          <t>1k0z5su</t>
+        </is>
+      </c>
+      <c r="B859" t="inlineStr">
+        <is>
+          <t>What is this?</t>
+        </is>
+      </c>
+      <c r="C859" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9w5di4dobave1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="860">
+      <c r="A860" t="inlineStr">
+        <is>
+          <t>1k0xujx</t>
+        </is>
+      </c>
+      <c r="B860" t="inlineStr">
+        <is>
+          <t>INSPO: Across the universe✨</t>
+        </is>
+      </c>
+      <c r="C860" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k0jegr7k0ave1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="861">
+      <c r="A861" t="inlineStr">
+        <is>
+          <t>1k0x2jl</t>
+        </is>
+      </c>
+      <c r="B861" t="inlineStr">
+        <is>
+          <t>Aura stars ✨</t>
+        </is>
+      </c>
+      <c r="C861" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k0x2jl</t>
+        </is>
+      </c>
+    </row>
+    <row r="862">
+      <c r="A862" t="inlineStr">
+        <is>
+          <t>1k0ux3n</t>
+        </is>
+      </c>
+      <c r="B862" t="inlineStr">
+        <is>
+          <t>Set For Myself</t>
+        </is>
+      </c>
+      <c r="C862" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1k0ux3n/set_for_myself/</t>
+        </is>
+      </c>
+    </row>
+    <row r="863">
+      <c r="A863" t="inlineStr">
+        <is>
+          <t>1k0sii5</t>
+        </is>
+      </c>
+      <c r="B863" t="inlineStr">
+        <is>
+          <t>Pink &amp; Pearls</t>
+        </is>
+      </c>
+      <c r="C863" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/21bxrbj0w8ve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="864">
+      <c r="A864" t="inlineStr">
+        <is>
+          <t>1k0q63l</t>
+        </is>
+      </c>
+      <c r="B864" t="inlineStr">
+        <is>
+          <t>Looks like a little galaxy</t>
+        </is>
+      </c>
+      <c r="C864" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k0q63l</t>
+        </is>
+      </c>
+    </row>
+    <row r="865">
+      <c r="A865" t="inlineStr">
+        <is>
+          <t>1k0pdm1</t>
+        </is>
+      </c>
+      <c r="B865" t="inlineStr">
+        <is>
+          <t>Just wanted to show off 🫣</t>
+        </is>
+      </c>
+      <c r="C865" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k0pdm1</t>
+        </is>
+      </c>
+    </row>
+    <row r="866">
+      <c r="A866" t="inlineStr">
+        <is>
+          <t>1k0ok5q</t>
+        </is>
+      </c>
+      <c r="B866" t="inlineStr">
+        <is>
+          <t>Sleek-ish fandom nails? Fairytail Acnologia theme, I could have done better but am still happy about the result</t>
+        </is>
+      </c>
+      <c r="C866" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k0ok5q</t>
+        </is>
+      </c>
+    </row>
+    <row r="867">
+      <c r="A867" t="inlineStr">
+        <is>
+          <t>1k0n0v7</t>
+        </is>
+      </c>
+      <c r="B867" t="inlineStr">
+        <is>
+          <t>Stained Glass</t>
+        </is>
+      </c>
+      <c r="C867" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/3ko0fik7s7ve1</t>
+        </is>
+      </c>
+    </row>
+    <row r="868">
+      <c r="A868" t="inlineStr">
+        <is>
+          <t>1k0kuxr</t>
+        </is>
+      </c>
+      <c r="B868" t="inlineStr">
+        <is>
+          <t>Ok.. what do these look like 😭</t>
+        </is>
+      </c>
+      <c r="C868" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mbk6ce5rb7ve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="869">
+      <c r="A869" t="inlineStr">
+        <is>
+          <t>1k0kehe</t>
+        </is>
+      </c>
+      <c r="B869" t="inlineStr">
+        <is>
+          <t>What nails for what event</t>
+        </is>
+      </c>
+      <c r="C869" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1k0kehe/what_nails_for_what_event/</t>
+        </is>
+      </c>
+    </row>
+    <row r="870">
+      <c r="A870" t="inlineStr">
+        <is>
+          <t>1k0jo2z</t>
+        </is>
+      </c>
+      <c r="B870" t="inlineStr">
+        <is>
+          <t>Help pls...</t>
+        </is>
+      </c>
+      <c r="C870" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1k0jo2z/help_pls/</t>
+        </is>
+      </c>
+    </row>
+    <row r="871">
+      <c r="A871" t="inlineStr">
+        <is>
+          <t>1k0j9qa</t>
+        </is>
+      </c>
+      <c r="B871" t="inlineStr">
+        <is>
+          <t>Press on nail package I made</t>
+        </is>
+      </c>
+      <c r="C871" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/wwaraesay6ve1</t>
+        </is>
+      </c>
+    </row>
+    <row r="872">
+      <c r="A872" t="inlineStr">
+        <is>
+          <t>1k0iq65</t>
+        </is>
+      </c>
+      <c r="B872" t="inlineStr">
+        <is>
+          <t>First Set</t>
+        </is>
+      </c>
+      <c r="C872" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k0iq65</t>
+        </is>
+      </c>
+    </row>
+    <row r="873">
+      <c r="A873" t="inlineStr">
+        <is>
+          <t>1k0hpph</t>
+        </is>
+      </c>
+      <c r="B873" t="inlineStr">
+        <is>
+          <t>Here's My Water Mark...Sooo What Yall Think 🤔</t>
+        </is>
+      </c>
+      <c r="C873" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k0hpph</t>
+        </is>
+      </c>
+    </row>
+    <row r="874">
+      <c r="A874" t="inlineStr">
+        <is>
+          <t>1k0gvze</t>
+        </is>
+      </c>
+      <c r="B874" t="inlineStr">
+        <is>
+          <t>Press ons for my friend</t>
+        </is>
+      </c>
+      <c r="C874" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k0gvze</t>
+        </is>
+      </c>
+    </row>
+    <row r="875">
+      <c r="A875" t="inlineStr">
+        <is>
+          <t>1k0gqiz</t>
+        </is>
+      </c>
+      <c r="B875" t="inlineStr">
+        <is>
+          <t>purple vibes💜💜</t>
+        </is>
+      </c>
+      <c r="C875" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l777syqn76ve1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Fri Apr 18 08:11:25 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_04_20.xlsx
+++ b/data/collected_data/2025_04_20.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C875"/>
+  <dimension ref="A1:C1067"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15308,6 +15308,3270 @@
         </is>
       </c>
     </row>
+    <row r="876">
+      <c r="A876" t="inlineStr">
+        <is>
+          <t>1k1ydv8</t>
+        </is>
+      </c>
+      <c r="B876" t="inlineStr">
+        <is>
+          <t>🌸Pink Stiletto🌸</t>
+        </is>
+      </c>
+      <c r="C876" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k1ydv8</t>
+        </is>
+      </c>
+    </row>
+    <row r="877">
+      <c r="A877" t="inlineStr">
+        <is>
+          <t>1k1xnsj</t>
+        </is>
+      </c>
+      <c r="B877" t="inlineStr">
+        <is>
+          <t>What’s spring without pastels 🌼🌸</t>
+        </is>
+      </c>
+      <c r="C877" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a3gr3dvn7jve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="878">
+      <c r="A878" t="inlineStr">
+        <is>
+          <t>1k1x9zu</t>
+        </is>
+      </c>
+      <c r="B878" t="inlineStr">
+        <is>
+          <t>What do tou think of this color?</t>
+        </is>
+      </c>
+      <c r="C878" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/45z880v53jve1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="879">
+      <c r="A879" t="inlineStr">
+        <is>
+          <t>1k1wopm</t>
+        </is>
+      </c>
+      <c r="B879" t="inlineStr">
+        <is>
+          <t>Question about grow out</t>
+        </is>
+      </c>
+      <c r="C879" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vluhzh0hwive1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="880">
+      <c r="A880" t="inlineStr">
+        <is>
+          <t>1k1wr82</t>
+        </is>
+      </c>
+      <c r="B880" t="inlineStr">
+        <is>
+          <t>DND not curing - troubleshooting</t>
+        </is>
+      </c>
+      <c r="C880" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k1wr82/dnd_not_curing_troubleshooting/</t>
+        </is>
+      </c>
+    </row>
+    <row r="881">
+      <c r="A881" t="inlineStr">
+        <is>
+          <t>1k1wnpl</t>
+        </is>
+      </c>
+      <c r="B881" t="inlineStr">
+        <is>
+          <t>Help 🥲</t>
+        </is>
+      </c>
+      <c r="C881" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k1wnpl/help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="882">
+      <c r="A882" t="inlineStr">
+        <is>
+          <t>1k1q8qt</t>
+        </is>
+      </c>
+      <c r="B882" t="inlineStr">
+        <is>
+          <t>Need advice</t>
+        </is>
+      </c>
+      <c r="C882" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k1q8qt/need_advice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="883">
+      <c r="A883" t="inlineStr">
+        <is>
+          <t>1k1rrxu</t>
+        </is>
+      </c>
+      <c r="B883" t="inlineStr">
+        <is>
+          <t>new nails. who dis? 💅</t>
+        </is>
+      </c>
+      <c r="C883" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k1rrxu</t>
+        </is>
+      </c>
+    </row>
+    <row r="884">
+      <c r="A884" t="inlineStr">
+        <is>
+          <t>1k1s2wa</t>
+        </is>
+      </c>
+      <c r="B884" t="inlineStr">
+        <is>
+          <t>Used gel polish on my boyfriends nails and it keeps popping off what do i do?</t>
+        </is>
+      </c>
+      <c r="C884" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k1s2wa</t>
+        </is>
+      </c>
+    </row>
+    <row r="885">
+      <c r="A885" t="inlineStr">
+        <is>
+          <t>1k1t77s</t>
+        </is>
+      </c>
+      <c r="B885" t="inlineStr">
+        <is>
+          <t>New nails💕 wicked inspired ✨✨</t>
+        </is>
+      </c>
+      <c r="C885" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xpr3sxzmxhve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="886">
+      <c r="A886" t="inlineStr">
+        <is>
+          <t>1k1tpkf</t>
+        </is>
+      </c>
+      <c r="B886" t="inlineStr">
+        <is>
+          <t>Nail damage after taking off acrylic</t>
+        </is>
+      </c>
+      <c r="C886" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k1tpkf</t>
+        </is>
+      </c>
+    </row>
+    <row r="887">
+      <c r="A887" t="inlineStr">
+        <is>
+          <t>1k1n15v</t>
+        </is>
+      </c>
+      <c r="B887" t="inlineStr">
+        <is>
+          <t>HEMA-free builder gel help?</t>
+        </is>
+      </c>
+      <c r="C887" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k1n15v</t>
+        </is>
+      </c>
+    </row>
+    <row r="888">
+      <c r="A888" t="inlineStr">
+        <is>
+          <t>1k1tr98</t>
+        </is>
+      </c>
+      <c r="B888" t="inlineStr">
+        <is>
+          <t>Please help :(</t>
+        </is>
+      </c>
+      <c r="C888" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k1tr98</t>
+        </is>
+      </c>
+    </row>
+    <row r="889">
+      <c r="A889" t="inlineStr">
+        <is>
+          <t>1k1un6q</t>
+        </is>
+      </c>
+      <c r="B889" t="inlineStr">
+        <is>
+          <t>What do I ask for? - INSPO PICS FROM @prettynailboutique</t>
+        </is>
+      </c>
+      <c r="C889" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k1un6q</t>
+        </is>
+      </c>
+    </row>
+    <row r="890">
+      <c r="A890" t="inlineStr">
+        <is>
+          <t>1k1v36z</t>
+        </is>
+      </c>
+      <c r="B890" t="inlineStr">
+        <is>
+          <t>first time getting my nails done in years and I could cry</t>
+        </is>
+      </c>
+      <c r="C890" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k1v36z</t>
+        </is>
+      </c>
+    </row>
+    <row r="891">
+      <c r="A891" t="inlineStr">
+        <is>
+          <t>1k1vyps</t>
+        </is>
+      </c>
+      <c r="B891" t="inlineStr">
+        <is>
+          <t>Gel nails changing color?</t>
+        </is>
+      </c>
+      <c r="C891" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bp7fcy2uoive1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="892">
+      <c r="A892" t="inlineStr">
+        <is>
+          <t>1k1w4dl</t>
+        </is>
+      </c>
+      <c r="B892" t="inlineStr">
+        <is>
+          <t>For a special occasion, something different ✨️</t>
+        </is>
+      </c>
+      <c r="C892" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/auyi5bucqive1</t>
+        </is>
+      </c>
+    </row>
+    <row r="893">
+      <c r="A893" t="inlineStr">
+        <is>
+          <t>1k1w4co</t>
+        </is>
+      </c>
+      <c r="B893" t="inlineStr">
+        <is>
+          <t>What do u think? Natural nails 😍💅🏻</t>
+        </is>
+      </c>
+      <c r="C893" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kqayvyqdqive1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="894">
+      <c r="A894" t="inlineStr">
+        <is>
+          <t>1k1vp8b</t>
+        </is>
+      </c>
+      <c r="B894" t="inlineStr">
+        <is>
+          <t>First time trying 3D art</t>
+        </is>
+      </c>
+      <c r="C894" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/kew3b803mive1</t>
+        </is>
+      </c>
+    </row>
+    <row r="895">
+      <c r="A895" t="inlineStr">
+        <is>
+          <t>1k1vfm7</t>
+        </is>
+      </c>
+      <c r="B895" t="inlineStr">
+        <is>
+          <t>¿Podrían darme consejos?</t>
+        </is>
+      </c>
+      <c r="C895" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4dl63iydjive1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="896">
+      <c r="A896" t="inlineStr">
+        <is>
+          <t>1k1v1p4</t>
+        </is>
+      </c>
+      <c r="B896" t="inlineStr">
+        <is>
+          <t>I’m a press on convert</t>
+        </is>
+      </c>
+      <c r="C896" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fxpxpgfjfive1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="897">
+      <c r="A897" t="inlineStr">
+        <is>
+          <t>1k1urxn</t>
+        </is>
+      </c>
+      <c r="B897" t="inlineStr">
+        <is>
+          <t>im a beginner and my nail polish is lifting</t>
+        </is>
+      </c>
+      <c r="C897" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k1urxn/im_a_beginner_and_my_nail_polish_is_lifting/</t>
+        </is>
+      </c>
+    </row>
+    <row r="898">
+      <c r="A898" t="inlineStr">
+        <is>
+          <t>1k1unfg</t>
+        </is>
+      </c>
+      <c r="B898" t="inlineStr">
+        <is>
+          <t>Very happy with new nail tech!</t>
+        </is>
+      </c>
+      <c r="C898" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rirs643mbive1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="899">
+      <c r="A899" t="inlineStr">
+        <is>
+          <t>1k1u6xi</t>
+        </is>
+      </c>
+      <c r="B899" t="inlineStr">
+        <is>
+          <t>New nails</t>
+        </is>
+      </c>
+      <c r="C899" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0pf6y3c77ive1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="900">
+      <c r="A900" t="inlineStr">
+        <is>
+          <t>1k1u5b6</t>
+        </is>
+      </c>
+      <c r="B900" t="inlineStr">
+        <is>
+          <t>Birthdayyyy nails 💅🏾</t>
+        </is>
+      </c>
+      <c r="C900" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gkpnpuxr6ive1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="901">
+      <c r="A901" t="inlineStr">
+        <is>
+          <t>1k1u1df</t>
+        </is>
+      </c>
+      <c r="B901" t="inlineStr">
+        <is>
+          <t>dO tHeSe lOoK LiKe pReSsOnS?//?/?</t>
+        </is>
+      </c>
+      <c r="C901" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k1u1df</t>
+        </is>
+      </c>
+    </row>
+    <row r="902">
+      <c r="A902" t="inlineStr">
+        <is>
+          <t>1k1tp4d</t>
+        </is>
+      </c>
+      <c r="B902" t="inlineStr">
+        <is>
+          <t>I did my nails today</t>
+        </is>
+      </c>
+      <c r="C902" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k1tp4d</t>
+        </is>
+      </c>
+    </row>
+    <row r="903">
+      <c r="A903" t="inlineStr">
+        <is>
+          <t>1k1thlh</t>
+        </is>
+      </c>
+      <c r="B903" t="inlineStr">
+        <is>
+          <t>got my nails done today!</t>
+        </is>
+      </c>
+      <c r="C903" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k1thlh</t>
+        </is>
+      </c>
+    </row>
+    <row r="904">
+      <c r="A904" t="inlineStr">
+        <is>
+          <t>1k1tg8z</t>
+        </is>
+      </c>
+      <c r="B904" t="inlineStr">
+        <is>
+          <t>been rocking black nails for a while but honestly this is my fave set ever</t>
+        </is>
+      </c>
+      <c r="C904" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k1tg8z</t>
+        </is>
+      </c>
+    </row>
+    <row r="905">
+      <c r="A905" t="inlineStr">
+        <is>
+          <t>1k1sw61</t>
+        </is>
+      </c>
+      <c r="B905" t="inlineStr">
+        <is>
+          <t>A lil something for spring 🌻</t>
+        </is>
+      </c>
+      <c r="C905" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/36davstruhve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="906">
+      <c r="A906" t="inlineStr">
+        <is>
+          <t>1k1ssr8</t>
+        </is>
+      </c>
+      <c r="B906" t="inlineStr">
+        <is>
+          <t>My first gel set</t>
+        </is>
+      </c>
+      <c r="C906" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k1ssr8</t>
+        </is>
+      </c>
+    </row>
+    <row r="907">
+      <c r="A907" t="inlineStr">
+        <is>
+          <t>1k1shzx</t>
+        </is>
+      </c>
+      <c r="B907" t="inlineStr">
+        <is>
+          <t>Been wanting to to try this for a while</t>
+        </is>
+      </c>
+      <c r="C907" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/026tt03wqhve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="908">
+      <c r="A908" t="inlineStr">
+        <is>
+          <t>1k1sf4o</t>
+        </is>
+      </c>
+      <c r="B908" t="inlineStr">
+        <is>
+          <t>Product recs for a beginner in gel nails</t>
+        </is>
+      </c>
+      <c r="C908" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k1sf4o/product_recs_for_a_beginner_in_gel_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="909">
+      <c r="A909" t="inlineStr">
+        <is>
+          <t>1k1s98f</t>
+        </is>
+      </c>
+      <c r="B909" t="inlineStr">
+        <is>
+          <t>Blueberry Milk</t>
+        </is>
+      </c>
+      <c r="C909" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k1s98f</t>
+        </is>
+      </c>
+    </row>
+    <row r="910">
+      <c r="A910" t="inlineStr">
+        <is>
+          <t>1k1s3k9</t>
+        </is>
+      </c>
+      <c r="B910" t="inlineStr">
+        <is>
+          <t>What went wrong with my SNS nails?</t>
+        </is>
+      </c>
+      <c r="C910" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k1s3k9</t>
+        </is>
+      </c>
+    </row>
+    <row r="911">
+      <c r="A911" t="inlineStr">
+        <is>
+          <t>1k1ryhm</t>
+        </is>
+      </c>
+      <c r="B911" t="inlineStr">
+        <is>
+          <t>Saved money, but did I lose the glam?</t>
+        </is>
+      </c>
+      <c r="C911" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k1ryhm</t>
+        </is>
+      </c>
+    </row>
+    <row r="912">
+      <c r="A912" t="inlineStr">
+        <is>
+          <t>1k1rpxl</t>
+        </is>
+      </c>
+      <c r="B912" t="inlineStr">
+        <is>
+          <t>I absolutely love these 💙🩵🩶🤍</t>
+        </is>
+      </c>
+      <c r="C912" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k1rpxl</t>
+        </is>
+      </c>
+    </row>
+    <row r="913">
+      <c r="A913" t="inlineStr">
+        <is>
+          <t>1k1qsp2</t>
+        </is>
+      </c>
+      <c r="B913" t="inlineStr">
+        <is>
+          <t>twas for vacation</t>
+        </is>
+      </c>
+      <c r="C913" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k1qsp2</t>
+        </is>
+      </c>
+    </row>
+    <row r="914">
+      <c r="A914" t="inlineStr">
+        <is>
+          <t>1k1r7mu</t>
+        </is>
+      </c>
+      <c r="B914" t="inlineStr">
+        <is>
+          <t>Gel nails won’t last</t>
+        </is>
+      </c>
+      <c r="C914" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k1r7mu/gel_nails_wont_last/</t>
+        </is>
+      </c>
+    </row>
+    <row r="915">
+      <c r="A915" t="inlineStr">
+        <is>
+          <t>1k1rh1o</t>
+        </is>
+      </c>
+      <c r="B915" t="inlineStr">
+        <is>
+          <t>my favorite set I’ve ever gotten</t>
+        </is>
+      </c>
+      <c r="C915" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k1rh1o</t>
+        </is>
+      </c>
+    </row>
+    <row r="916">
+      <c r="A916" t="inlineStr">
+        <is>
+          <t>1k1rbdl</t>
+        </is>
+      </c>
+      <c r="B916" t="inlineStr">
+        <is>
+          <t>My sister's first time doing nail art.</t>
+        </is>
+      </c>
+      <c r="C916" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k1rbdl</t>
+        </is>
+      </c>
+    </row>
+    <row r="917">
+      <c r="A917" t="inlineStr">
+        <is>
+          <t>1k1qt8f</t>
+        </is>
+      </c>
+      <c r="B917" t="inlineStr">
+        <is>
+          <t>press ons!!</t>
+        </is>
+      </c>
+      <c r="C917" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8amnmscwbhve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="918">
+      <c r="A918" t="inlineStr">
+        <is>
+          <t>1k1qqn2</t>
+        </is>
+      </c>
+      <c r="B918" t="inlineStr">
+        <is>
+          <t>New Easter set</t>
+        </is>
+      </c>
+      <c r="C918" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/51x7xx5bbhve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="919">
+      <c r="A919" t="inlineStr">
+        <is>
+          <t>1k1oows</t>
+        </is>
+      </c>
+      <c r="B919" t="inlineStr">
+        <is>
+          <t>Star Wars: Ready for May The Fourth</t>
+        </is>
+      </c>
+      <c r="C919" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/62wtjvfcugve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="920">
+      <c r="A920" t="inlineStr">
+        <is>
+          <t>1k1paok</t>
+        </is>
+      </c>
+      <c r="B920" t="inlineStr">
+        <is>
+          <t>I am v happy</t>
+        </is>
+      </c>
+      <c r="C920" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k1paok</t>
+        </is>
+      </c>
+    </row>
+    <row r="921">
+      <c r="A921" t="inlineStr">
+        <is>
+          <t>1k1pfu5</t>
+        </is>
+      </c>
+      <c r="B921" t="inlineStr">
+        <is>
+          <t>Xalitla Art inspired nails for my Mexican vacay</t>
+        </is>
+      </c>
+      <c r="C921" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k1pfu5</t>
+        </is>
+      </c>
+    </row>
+    <row r="922">
+      <c r="A922" t="inlineStr">
+        <is>
+          <t>1k1q3if</t>
+        </is>
+      </c>
+      <c r="B922" t="inlineStr">
+        <is>
+          <t>Matte &amp; Chrome</t>
+        </is>
+      </c>
+      <c r="C922" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k1q3if</t>
+        </is>
+      </c>
+    </row>
+    <row r="923">
+      <c r="A923" t="inlineStr">
+        <is>
+          <t>1k1pnxr</t>
+        </is>
+      </c>
+      <c r="B923" t="inlineStr">
+        <is>
+          <t>Moving to gel polish</t>
+        </is>
+      </c>
+      <c r="C923" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k1pnxr</t>
+        </is>
+      </c>
+    </row>
+    <row r="924">
+      <c r="A924" t="inlineStr">
+        <is>
+          <t>1k1pg4o</t>
+        </is>
+      </c>
+      <c r="B924" t="inlineStr">
+        <is>
+          <t>new mani, new me ✨</t>
+        </is>
+      </c>
+      <c r="C924" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ket0zz1f0hve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="925">
+      <c r="A925" t="inlineStr">
+        <is>
+          <t>1k1og8j</t>
+        </is>
+      </c>
+      <c r="B925" t="inlineStr">
+        <is>
+          <t>What do u guys think</t>
+        </is>
+      </c>
+      <c r="C925" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o835crresgve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="926">
+      <c r="A926" t="inlineStr">
+        <is>
+          <t>1k1nzsm</t>
+        </is>
+      </c>
+      <c r="B926" t="inlineStr">
+        <is>
+          <t>Simple blue nails💙</t>
+        </is>
+      </c>
+      <c r="C926" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6j204d2uogve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="927">
+      <c r="A927" t="inlineStr">
+        <is>
+          <t>1k1nmyf</t>
+        </is>
+      </c>
+      <c r="B927" t="inlineStr">
+        <is>
+          <t>Thinking about becoming a nail tech, I like the idea of a creative job, but a few family members said I shouldn't.</t>
+        </is>
+      </c>
+      <c r="C927" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k1nmyf/thinking_about_becoming_a_nail_tech_i_like_the/</t>
+        </is>
+      </c>
+    </row>
+    <row r="928">
+      <c r="A928" t="inlineStr">
+        <is>
+          <t>1k1msup</t>
+        </is>
+      </c>
+      <c r="B928" t="inlineStr">
+        <is>
+          <t>New nails. I love it!</t>
+        </is>
+      </c>
+      <c r="C928" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lqz7xdipfgve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="929">
+      <c r="A929" t="inlineStr">
+        <is>
+          <t>1k1mgng</t>
+        </is>
+      </c>
+      <c r="B929" t="inlineStr">
+        <is>
+          <t>How to make press ons last only a day?</t>
+        </is>
+      </c>
+      <c r="C929" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k1mgng/how_to_make_press_ons_last_only_a_day/</t>
+        </is>
+      </c>
+    </row>
+    <row r="930">
+      <c r="A930" t="inlineStr">
+        <is>
+          <t>1k1m0f4</t>
+        </is>
+      </c>
+      <c r="B930" t="inlineStr">
+        <is>
+          <t>My Easter Nails</t>
+        </is>
+      </c>
+      <c r="C930" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1sfw40cs9gve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="931">
+      <c r="A931" t="inlineStr">
+        <is>
+          <t>1k1ljeq</t>
+        </is>
+      </c>
+      <c r="B931" t="inlineStr">
+        <is>
+          <t>Green and denim</t>
+        </is>
+      </c>
+      <c r="C931" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k1ljeq</t>
+        </is>
+      </c>
+    </row>
+    <row r="932">
+      <c r="A932" t="inlineStr">
+        <is>
+          <t>1k1lfhi</t>
+        </is>
+      </c>
+      <c r="B932" t="inlineStr">
+        <is>
+          <t>Base Coat Recommendations - Butter London or Holo Taco?</t>
+        </is>
+      </c>
+      <c r="C932" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k1lfhi/base_coat_recommendations_butter_london_or_holo/</t>
+        </is>
+      </c>
+    </row>
+    <row r="933">
+      <c r="A933" t="inlineStr">
+        <is>
+          <t>1k1ladv</t>
+        </is>
+      </c>
+      <c r="B933" t="inlineStr">
+        <is>
+          <t>Help! I don’t get my nails done often and I need some advice…</t>
+        </is>
+      </c>
+      <c r="C933" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k1ladv/help_i_dont_get_my_nails_done_often_and_i_need/</t>
+        </is>
+      </c>
+    </row>
+    <row r="934">
+      <c r="A934" t="inlineStr">
+        <is>
+          <t>1k1i23w</t>
+        </is>
+      </c>
+      <c r="B934" t="inlineStr">
+        <is>
+          <t>Just took off gel x, what do we think?</t>
+        </is>
+      </c>
+      <c r="C934" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k1i23w</t>
+        </is>
+      </c>
+    </row>
+    <row r="935">
+      <c r="A935" t="inlineStr">
+        <is>
+          <t>1k1l5jp</t>
+        </is>
+      </c>
+      <c r="B935" t="inlineStr">
+        <is>
+          <t>a simple french</t>
+        </is>
+      </c>
+      <c r="C935" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ehwtt24c3gve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="936">
+      <c r="A936" t="inlineStr">
+        <is>
+          <t>1k1l4w9</t>
+        </is>
+      </c>
+      <c r="B936" t="inlineStr">
+        <is>
+          <t>Lovely Lemons!</t>
+        </is>
+      </c>
+      <c r="C936" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w2vxwrt63gve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="937">
+      <c r="A937" t="inlineStr">
+        <is>
+          <t>1k1jmlx</t>
+        </is>
+      </c>
+      <c r="B937" t="inlineStr">
+        <is>
+          <t>Struggling with my nails big time as a housekeeper 😬 Tips?</t>
+        </is>
+      </c>
+      <c r="C937" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k1jmlx</t>
+        </is>
+      </c>
+    </row>
+    <row r="938">
+      <c r="A938" t="inlineStr">
+        <is>
+          <t>1k1jybb</t>
+        </is>
+      </c>
+      <c r="B938" t="inlineStr">
+        <is>
+          <t>How do i "taper" the ends?..</t>
+        </is>
+      </c>
+      <c r="C938" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ra485rvaufve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="939">
+      <c r="A939" t="inlineStr">
+        <is>
+          <t>1k1jshu</t>
+        </is>
+      </c>
+      <c r="B939" t="inlineStr">
+        <is>
+          <t>Gel remover making skin feel like burning?</t>
+        </is>
+      </c>
+      <c r="C939" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k1jshu/gel_remover_making_skin_feel_like_burning/</t>
+        </is>
+      </c>
+    </row>
+    <row r="940">
+      <c r="A940" t="inlineStr">
+        <is>
+          <t>1k1gztr</t>
+        </is>
+      </c>
+      <c r="B940" t="inlineStr">
+        <is>
+          <t>Where do y'all find nail art inspo?</t>
+        </is>
+      </c>
+      <c r="C940" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k1gztr/where_do_yall_find_nail_art_inspo/</t>
+        </is>
+      </c>
+    </row>
+    <row r="941">
+      <c r="A941" t="inlineStr">
+        <is>
+          <t>1k1khwc</t>
+        </is>
+      </c>
+      <c r="B941" t="inlineStr">
+        <is>
+          <t>Spring vibes</t>
+        </is>
+      </c>
+      <c r="C941" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/muaeuapcyfve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="942">
+      <c r="A942" t="inlineStr">
+        <is>
+          <t>1k1kfo6</t>
+        </is>
+      </c>
+      <c r="B942" t="inlineStr">
+        <is>
+          <t>First time trying frenchies</t>
+        </is>
+      </c>
+      <c r="C942" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b6r5h0fvxfve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="943">
+      <c r="A943" t="inlineStr">
+        <is>
+          <t>1k1k7sp</t>
+        </is>
+      </c>
+      <c r="B943" t="inlineStr">
+        <is>
+          <t>DND 883 Candy kiss sheer gel</t>
+        </is>
+      </c>
+      <c r="C943" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wth2x748wfve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="944">
+      <c r="A944" t="inlineStr">
+        <is>
+          <t>1k1jy2s</t>
+        </is>
+      </c>
+      <c r="B944" t="inlineStr">
+        <is>
+          <t>What do you guys think of my nails I did?(newbie)</t>
+        </is>
+      </c>
+      <c r="C944" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k1jy2s</t>
+        </is>
+      </c>
+    </row>
+    <row r="945">
+      <c r="A945" t="inlineStr">
+        <is>
+          <t>1k1ja58</t>
+        </is>
+      </c>
+      <c r="B945" t="inlineStr">
+        <is>
+          <t>Black &amp; silver combo 💿🖤</t>
+        </is>
+      </c>
+      <c r="C945" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k1ja58</t>
+        </is>
+      </c>
+    </row>
+    <row r="946">
+      <c r="A946" t="inlineStr">
+        <is>
+          <t>1k1iscf</t>
+        </is>
+      </c>
+      <c r="B946" t="inlineStr">
+        <is>
+          <t>First time getting Gel X Nails 💅🏻 and I love them so much ❤️!</t>
+        </is>
+      </c>
+      <c r="C946" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mgzznw6vlfve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="947">
+      <c r="A947" t="inlineStr">
+        <is>
+          <t>1k1iq2p</t>
+        </is>
+      </c>
+      <c r="B947" t="inlineStr">
+        <is>
+          <t>My favorite nails of all time😍</t>
+        </is>
+      </c>
+      <c r="C947" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k1iq2p</t>
+        </is>
+      </c>
+    </row>
+    <row r="948">
+      <c r="A948" t="inlineStr">
+        <is>
+          <t>1k1ip8h</t>
+        </is>
+      </c>
+      <c r="B948" t="inlineStr">
+        <is>
+          <t>Overcharged for color chain, but at least they’re cute!</t>
+        </is>
+      </c>
+      <c r="C948" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ccg6zxt8lfve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="949">
+      <c r="A949" t="inlineStr">
+        <is>
+          <t>1k1i77p</t>
+        </is>
+      </c>
+      <c r="B949" t="inlineStr">
+        <is>
+          <t>Done my own nails with gel for the first time</t>
+        </is>
+      </c>
+      <c r="C949" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ffiy43qlhfve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="950">
+      <c r="A950" t="inlineStr">
+        <is>
+          <t>1k1i0c5</t>
+        </is>
+      </c>
+      <c r="B950" t="inlineStr">
+        <is>
+          <t>This Weeks Nails</t>
+        </is>
+      </c>
+      <c r="C950" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jvvxa6z6gfve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="951">
+      <c r="A951" t="inlineStr">
+        <is>
+          <t>1k1hvb8</t>
+        </is>
+      </c>
+      <c r="B951" t="inlineStr">
+        <is>
+          <t>Easter set ❤️✨</t>
+        </is>
+      </c>
+      <c r="C951" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ria7r7p5ffve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="952">
+      <c r="A952" t="inlineStr">
+        <is>
+          <t>1k1ht47</t>
+        </is>
+      </c>
+      <c r="B952" t="inlineStr">
+        <is>
+          <t>Birthday nails! I went extra fancy and I could not be happier!</t>
+        </is>
+      </c>
+      <c r="C952" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/at9ts0tqefve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="953">
+      <c r="A953" t="inlineStr">
+        <is>
+          <t>1k1hp8i</t>
+        </is>
+      </c>
+      <c r="B953" t="inlineStr">
+        <is>
+          <t>easter twist</t>
+        </is>
+      </c>
+      <c r="C953" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c6scvgsydfve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="954">
+      <c r="A954" t="inlineStr">
+        <is>
+          <t>1k1hi0q</t>
+        </is>
+      </c>
+      <c r="B954" t="inlineStr">
+        <is>
+          <t>First builder gel mani</t>
+        </is>
+      </c>
+      <c r="C954" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6xee0mmfcfve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="955">
+      <c r="A955" t="inlineStr">
+        <is>
+          <t>1k1heab</t>
+        </is>
+      </c>
+      <c r="B955" t="inlineStr">
+        <is>
+          <t>Barbie nails 💅</t>
+        </is>
+      </c>
+      <c r="C955" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/70fq061pbfve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="956">
+      <c r="A956" t="inlineStr">
+        <is>
+          <t>1k1h3bg</t>
+        </is>
+      </c>
+      <c r="B956" t="inlineStr">
+        <is>
+          <t>Springtime moment</t>
+        </is>
+      </c>
+      <c r="C956" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/np1gzdjh9fve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="957">
+      <c r="A957" t="inlineStr">
+        <is>
+          <t>1k1gkrx</t>
+        </is>
+      </c>
+      <c r="B957" t="inlineStr">
+        <is>
+          <t>Nails shape</t>
+        </is>
+      </c>
+      <c r="C957" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z6zhd8jq5fve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="958">
+      <c r="A958" t="inlineStr">
+        <is>
+          <t>1k1gk82</t>
+        </is>
+      </c>
+      <c r="B958" t="inlineStr">
+        <is>
+          <t>Are they worth the price or are they overpriced ?</t>
+        </is>
+      </c>
+      <c r="C958" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k1gk82</t>
+        </is>
+      </c>
+    </row>
+    <row r="959">
+      <c r="A959" t="inlineStr">
+        <is>
+          <t>1k1g8f1</t>
+        </is>
+      </c>
+      <c r="B959" t="inlineStr">
+        <is>
+          <t>Treating damaged nails post-press ons</t>
+        </is>
+      </c>
+      <c r="C959" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k1g8f1/treating_damaged_nails_postpress_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="960">
+      <c r="A960" t="inlineStr">
+        <is>
+          <t>1k1gjip</t>
+        </is>
+      </c>
+      <c r="B960" t="inlineStr">
+        <is>
+          <t>Slowly getting into the world of having my nails decorated!</t>
+        </is>
+      </c>
+      <c r="C960" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k1gjip</t>
+        </is>
+      </c>
+    </row>
+    <row r="961">
+      <c r="A961" t="inlineStr">
+        <is>
+          <t>1k1ggqz</t>
+        </is>
+      </c>
+      <c r="B961" t="inlineStr">
+        <is>
+          <t>Iceland Wedding - Help me decide what to do for my nails!</t>
+        </is>
+      </c>
+      <c r="C961" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k1ggqz/iceland_wedding_help_me_decide_what_to_do_for_my/</t>
+        </is>
+      </c>
+    </row>
+    <row r="962">
+      <c r="A962" t="inlineStr">
+        <is>
+          <t>1k1fa53</t>
+        </is>
+      </c>
+      <c r="B962" t="inlineStr">
+        <is>
+          <t>Simple Easter Nails</t>
+        </is>
+      </c>
+      <c r="C962" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rlwodu37weve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="963">
+      <c r="A963" t="inlineStr">
+        <is>
+          <t>1k1f30b</t>
+        </is>
+      </c>
+      <c r="B963" t="inlineStr">
+        <is>
+          <t>is it time for a fill?</t>
+        </is>
+      </c>
+      <c r="C963" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0qxr7d4pueve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="964">
+      <c r="A964" t="inlineStr">
+        <is>
+          <t>1k1euga</t>
+        </is>
+      </c>
+      <c r="B964" t="inlineStr">
+        <is>
+          <t>Acrylic Nail Shape Suggestions?</t>
+        </is>
+      </c>
+      <c r="C964" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k1euga</t>
+        </is>
+      </c>
+    </row>
+    <row r="965">
+      <c r="A965" t="inlineStr">
+        <is>
+          <t>1k18o6i</t>
+        </is>
+      </c>
+      <c r="B965" t="inlineStr">
+        <is>
+          <t>Biab keeps on lifting</t>
+        </is>
+      </c>
+      <c r="C965" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k18o6i</t>
+        </is>
+      </c>
+    </row>
+    <row r="966">
+      <c r="A966" t="inlineStr">
+        <is>
+          <t>1k1d7wl</t>
+        </is>
+      </c>
+      <c r="B966" t="inlineStr">
+        <is>
+          <t>Tried line work. How I do?</t>
+        </is>
+      </c>
+      <c r="C966" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oz07ut1mgeve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="967">
+      <c r="A967" t="inlineStr">
+        <is>
+          <t>1k1en0w</t>
+        </is>
+      </c>
+      <c r="B967" t="inlineStr">
+        <is>
+          <t>Beginner Gel Nail Tech</t>
+        </is>
+      </c>
+      <c r="C967" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8zn44z2ereve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="968">
+      <c r="A968" t="inlineStr">
+        <is>
+          <t>1k1ejpb</t>
+        </is>
+      </c>
+      <c r="B968" t="inlineStr">
+        <is>
+          <t>New spring mani</t>
+        </is>
+      </c>
+      <c r="C968" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tm0261soqeve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="969">
+      <c r="A969" t="inlineStr">
+        <is>
+          <t>1k1eexv</t>
+        </is>
+      </c>
+      <c r="B969" t="inlineStr">
+        <is>
+          <t>First time!!!</t>
+        </is>
+      </c>
+      <c r="C969" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k1eexv</t>
+        </is>
+      </c>
+    </row>
+    <row r="970">
+      <c r="A970" t="inlineStr">
+        <is>
+          <t>1k1edrb</t>
+        </is>
+      </c>
+      <c r="B970" t="inlineStr">
+        <is>
+          <t>Tried cat eye polish for the first time</t>
+        </is>
+      </c>
+      <c r="C970" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k1edrb</t>
+        </is>
+      </c>
+    </row>
+    <row r="971">
+      <c r="A971" t="inlineStr">
+        <is>
+          <t>1k1dvyc</t>
+        </is>
+      </c>
+      <c r="B971" t="inlineStr">
+        <is>
+          <t>Fixed a broken nail</t>
+        </is>
+      </c>
+      <c r="C971" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mgz5z14nleve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="972">
+      <c r="A972" t="inlineStr">
+        <is>
+          <t>1k1dtfx</t>
+        </is>
+      </c>
+      <c r="B972" t="inlineStr">
+        <is>
+          <t>Long nail havers, please give me tips! Struggling to function</t>
+        </is>
+      </c>
+      <c r="C972" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k1dtfx/long_nail_havers_please_give_me_tips_struggling/</t>
+        </is>
+      </c>
+    </row>
+    <row r="973">
+      <c r="A973" t="inlineStr">
+        <is>
+          <t>1k1dkjo</t>
+        </is>
+      </c>
+      <c r="B973" t="inlineStr">
+        <is>
+          <t>Bubble bath and ballet slippers girlie no longer!</t>
+        </is>
+      </c>
+      <c r="C973" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d44bgl88jeve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="974">
+      <c r="A974" t="inlineStr">
+        <is>
+          <t>1k1d7x4</t>
+        </is>
+      </c>
+      <c r="B974" t="inlineStr">
+        <is>
+          <t>Going simple with gradation nail</t>
+        </is>
+      </c>
+      <c r="C974" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/e6ut0i5lgeve1</t>
+        </is>
+      </c>
+    </row>
+    <row r="975">
+      <c r="A975" t="inlineStr">
+        <is>
+          <t>1k1cwtg</t>
+        </is>
+      </c>
+      <c r="B975" t="inlineStr">
+        <is>
+          <t>First time doing citrus—super proud!</t>
+        </is>
+      </c>
+      <c r="C975" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k1cwtg</t>
+        </is>
+      </c>
+    </row>
+    <row r="976">
+      <c r="A976" t="inlineStr">
+        <is>
+          <t>1k1zl21</t>
+        </is>
+      </c>
+      <c r="B976" t="inlineStr">
+        <is>
+          <t>Recreating nail art with super shorties</t>
+        </is>
+      </c>
+      <c r="C976" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k1zl21</t>
+        </is>
+      </c>
+    </row>
+    <row r="977">
+      <c r="A977" t="inlineStr">
+        <is>
+          <t>1k1yjju</t>
+        </is>
+      </c>
+      <c r="B977" t="inlineStr">
+        <is>
+          <t>Easter nails fail and win (swipe for more)</t>
+        </is>
+      </c>
+      <c r="C977" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k1yjju</t>
+        </is>
+      </c>
+    </row>
+    <row r="978">
+      <c r="A978" t="inlineStr">
+        <is>
+          <t>1k1x4ij</t>
+        </is>
+      </c>
+      <c r="B978" t="inlineStr">
+        <is>
+          <t>OPI Bubble Bath always looks terrible</t>
+        </is>
+      </c>
+      <c r="C978" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k1x4ij/opi_bubble_bath_always_looks_terrible/</t>
+        </is>
+      </c>
+    </row>
+    <row r="979">
+      <c r="A979" t="inlineStr">
+        <is>
+          <t>1k1x2lp</t>
+        </is>
+      </c>
+      <c r="B979" t="inlineStr">
+        <is>
+          <t>Shifty unicorn- polish bought in 🇮🇳</t>
+        </is>
+      </c>
+      <c r="C979" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k1x2lp</t>
+        </is>
+      </c>
+    </row>
+    <row r="980">
+      <c r="A980" t="inlineStr">
+        <is>
+          <t>1k1vcyn</t>
+        </is>
+      </c>
+      <c r="B980" t="inlineStr">
+        <is>
+          <t>I just started doing gel nails.</t>
+        </is>
+      </c>
+      <c r="C980" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/bc97smiliive1</t>
+        </is>
+      </c>
+    </row>
+    <row r="981">
+      <c r="A981" t="inlineStr">
+        <is>
+          <t>1k1v2x6</t>
+        </is>
+      </c>
+      <c r="B981" t="inlineStr">
+        <is>
+          <t>Do I need a UV lamp for this?</t>
+        </is>
+      </c>
+      <c r="C981" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b62sehlufive1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="982">
+      <c r="A982" t="inlineStr">
+        <is>
+          <t>1k1urs6</t>
+        </is>
+      </c>
+      <c r="B982" t="inlineStr">
+        <is>
+          <t>Please help me find a dupe for Blue Duke!</t>
+        </is>
+      </c>
+      <c r="C982" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lxblknmscive1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="983">
+      <c r="A983" t="inlineStr">
+        <is>
+          <t>1k1upts</t>
+        </is>
+      </c>
+      <c r="B983" t="inlineStr">
+        <is>
+          <t>In honor of Clionadh sale... Norpsilocin 🔥</t>
+        </is>
+      </c>
+      <c r="C983" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/0snwht08cive1</t>
+        </is>
+      </c>
+    </row>
+    <row r="984">
+      <c r="A984" t="inlineStr">
+        <is>
+          <t>1k1tfkh</t>
+        </is>
+      </c>
+      <c r="B984" t="inlineStr">
+        <is>
+          <t>Zodiac Collab - Rainbow Flourite v2</t>
+        </is>
+      </c>
+      <c r="C984" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k1tfkh</t>
+        </is>
+      </c>
+    </row>
+    <row r="985">
+      <c r="A985" t="inlineStr">
+        <is>
+          <t>1k1t8yr</t>
+        </is>
+      </c>
+      <c r="B985" t="inlineStr">
+        <is>
+          <t>🌱 Green &amp; Golden Hour</t>
+        </is>
+      </c>
+      <c r="C985" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nyxvf4tixhve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="986">
+      <c r="A986" t="inlineStr">
+        <is>
+          <t>1k1ssj8</t>
+        </is>
+      </c>
+      <c r="B986" t="inlineStr">
+        <is>
+          <t>The sun today was perfect for showing off the holo</t>
+        </is>
+      </c>
+      <c r="C986" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/7yqrab1uthve1</t>
+        </is>
+      </c>
+    </row>
+    <row r="987">
+      <c r="A987" t="inlineStr">
+        <is>
+          <t>1k1s0jx</t>
+        </is>
+      </c>
+      <c r="B987" t="inlineStr">
+        <is>
+          <t>Hummingbird glass</t>
+        </is>
+      </c>
+      <c r="C987" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k1s0jx</t>
+        </is>
+      </c>
+    </row>
+    <row r="988">
+      <c r="A988" t="inlineStr">
+        <is>
+          <t>1k1ryij</t>
+        </is>
+      </c>
+      <c r="B988" t="inlineStr">
+        <is>
+          <t>Swatch request: Mooncat Memento Mori and ILNP Flicker</t>
+        </is>
+      </c>
+      <c r="C988" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k1ryij/swatch_request_mooncat_memento_mori_and_ilnp/</t>
+        </is>
+      </c>
+    </row>
+    <row r="989">
+      <c r="A989" t="inlineStr">
+        <is>
+          <t>1k1rtfn</t>
+        </is>
+      </c>
+      <c r="B989" t="inlineStr">
+        <is>
+          <t>Earl Grey inspired mani ☕️</t>
+        </is>
+      </c>
+      <c r="C989" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k1rtfn</t>
+        </is>
+      </c>
+    </row>
+    <row r="990">
+      <c r="A990" t="inlineStr">
+        <is>
+          <t>1k1oto9</t>
+        </is>
+      </c>
+      <c r="B990" t="inlineStr">
+        <is>
+          <t>Great Lakes Lacquer</t>
+        </is>
+      </c>
+      <c r="C990" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k1oto9/great_lakes_lacquer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="991">
+      <c r="A991" t="inlineStr">
+        <is>
+          <t>1k1r35o</t>
+        </is>
+      </c>
+      <c r="B991" t="inlineStr">
+        <is>
+          <t>Easter chocolate mani</t>
+        </is>
+      </c>
+      <c r="C991" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aqe26hmcehve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="992">
+      <c r="A992" t="inlineStr">
+        <is>
+          <t>1k1qw5w</t>
+        </is>
+      </c>
+      <c r="B992" t="inlineStr">
+        <is>
+          <t>My hygienist complimented my nails today!</t>
+        </is>
+      </c>
+      <c r="C992" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/29xi9k3nchve1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="993">
+      <c r="A993" t="inlineStr">
+        <is>
+          <t>1k1q8vz</t>
+        </is>
+      </c>
+      <c r="B993" t="inlineStr">
+        <is>
+          <t>Soul Mates</t>
+        </is>
+      </c>
+      <c r="C993" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k1q8vz</t>
+        </is>
+      </c>
+    </row>
+    <row r="994">
+      <c r="A994" t="inlineStr">
+        <is>
+          <t>1k1q3h2</t>
+        </is>
+      </c>
+      <c r="B994" t="inlineStr">
+        <is>
+          <t>Super Neon Iridescent Pink mani</t>
+        </is>
+      </c>
+      <c r="C994" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k1q3h2</t>
+        </is>
+      </c>
+    </row>
+    <row r="995">
+      <c r="A995" t="inlineStr">
+        <is>
+          <t>1k1pdkn</t>
+        </is>
+      </c>
+      <c r="B995" t="inlineStr">
+        <is>
+          <t>New brand spotlight: Apocalypse Polish's "Toto I Don't Think We're In Hawkins Anymore"</t>
+        </is>
+      </c>
+      <c r="C995" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k1pdkn</t>
+        </is>
+      </c>
+    </row>
+    <row r="996">
+      <c r="A996" t="inlineStr">
+        <is>
+          <t>1k1pcvh</t>
+        </is>
+      </c>
+      <c r="B996" t="inlineStr">
+        <is>
+          <t>Bluebird Spring Fever Collection - Available on Friday, April 18th at 5pm EST</t>
+        </is>
+      </c>
+      <c r="C996" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k1pcvh/bluebird_spring_fever_collection_available_on/</t>
+        </is>
+      </c>
+    </row>
+    <row r="997">
+      <c r="A997" t="inlineStr">
+        <is>
+          <t>1k1oy5l</t>
+        </is>
+      </c>
+      <c r="B997" t="inlineStr">
+        <is>
+          <t>Clionadh's "Hilt" got me feeling anything but sour 🩵🧡</t>
+        </is>
+      </c>
+      <c r="C997" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t2se9ogdwgve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="998">
+      <c r="A998" t="inlineStr">
+        <is>
+          <t>1k1oek4</t>
+        </is>
+      </c>
+      <c r="B998" t="inlineStr">
+        <is>
+          <t>Are press ons allowed?</t>
+        </is>
+      </c>
+      <c r="C998" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/85iag0g0sgve1</t>
+        </is>
+      </c>
+    </row>
+    <row r="999">
+      <c r="A999" t="inlineStr">
+        <is>
+          <t>1k1o057</t>
+        </is>
+      </c>
+      <c r="B999" t="inlineStr">
+        <is>
+          <t>I don’t even do nail art but I think I *have* to have these</t>
+        </is>
+      </c>
+      <c r="C999" t="inlineStr">
+        <is>
+          <t>https://youtube.com/shorts/qCadJw7RQoo?si=ah99mA00wYHxabwn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1000">
+      <c r="A1000" t="inlineStr">
+        <is>
+          <t>1k1njkn</t>
+        </is>
+      </c>
+      <c r="B1000" t="inlineStr">
+        <is>
+          <t>bees knees overpour?</t>
+        </is>
+      </c>
+      <c r="C1000" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k1njkn/bees_knees_overpour/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1001">
+      <c r="A1001" t="inlineStr">
+        <is>
+          <t>1k1nbho</t>
+        </is>
+      </c>
+      <c r="B1001" t="inlineStr">
+        <is>
+          <t>Would you guess my nails glow in the dark?</t>
+        </is>
+      </c>
+      <c r="C1001" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rahdhpbojgve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1002">
+      <c r="A1002" t="inlineStr">
+        <is>
+          <t>1k1n0rr</t>
+        </is>
+      </c>
+      <c r="B1002" t="inlineStr">
+        <is>
+          <t>inky blue jelly recs?</t>
+        </is>
+      </c>
+      <c r="C1002" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k1n0rr/inky_blue_jelly_recs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1003">
+      <c r="A1003" t="inlineStr">
+        <is>
+          <t>1k1mn91</t>
+        </is>
+      </c>
+      <c r="B1003" t="inlineStr">
+        <is>
+          <t>🐥🍒🐤Peeps N' Cherries🐤🍒🐥</t>
+        </is>
+      </c>
+      <c r="C1003" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k1mn91</t>
+        </is>
+      </c>
+    </row>
+    <row r="1004">
+      <c r="A1004" t="inlineStr">
+        <is>
+          <t>1k1mjwa</t>
+        </is>
+      </c>
+      <c r="B1004" t="inlineStr">
+        <is>
+          <t>Easter Skittle mani!</t>
+        </is>
+      </c>
+      <c r="C1004" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ve9u8b9tdgve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1005">
+      <c r="A1005" t="inlineStr">
+        <is>
+          <t>1k1mcs6</t>
+        </is>
+      </c>
+      <c r="B1005" t="inlineStr">
+        <is>
+          <t>Moonboots by Cracked polish might be my perfect greige</t>
+        </is>
+      </c>
+      <c r="C1005" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k1mcs6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1006">
+      <c r="A1006" t="inlineStr">
+        <is>
+          <t>1k1m7qf</t>
+        </is>
+      </c>
+      <c r="B1006" t="inlineStr">
+        <is>
+          <t>Root of All Evil vs. Fair Isle</t>
+        </is>
+      </c>
+      <c r="C1006" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k1m7qf/root_of_all_evil_vs_fair_isle/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1007">
+      <c r="A1007" t="inlineStr">
+        <is>
+          <t>1k1lzlz</t>
+        </is>
+      </c>
+      <c r="B1007" t="inlineStr">
+        <is>
+          <t>Ruincharmed</t>
+        </is>
+      </c>
+      <c r="C1007" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k1lzlz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1008">
+      <c r="A1008" t="inlineStr">
+        <is>
+          <t>1k1lqac</t>
+        </is>
+      </c>
+      <c r="B1008" t="inlineStr">
+        <is>
+          <t>Alternatives to Zoya naked manicure?</t>
+        </is>
+      </c>
+      <c r="C1008" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k1lqac/alternatives_to_zoya_naked_manicure/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1009">
+      <c r="A1009" t="inlineStr">
+        <is>
+          <t>1k1kukm</t>
+        </is>
+      </c>
+      <c r="B1009" t="inlineStr">
+        <is>
+          <t>Can regular polish be contaminated or pose the same risks as gel polish?</t>
+        </is>
+      </c>
+      <c r="C1009" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k1kukm/can_regular_polish_be_contaminated_or_pose_the/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1010">
+      <c r="A1010" t="inlineStr">
+        <is>
+          <t>1k1kjtg</t>
+        </is>
+      </c>
+      <c r="B1010" t="inlineStr">
+        <is>
+          <t>Born Ugly Dotticure</t>
+        </is>
+      </c>
+      <c r="C1010" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k1kjtg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1011">
+      <c r="A1011" t="inlineStr">
+        <is>
+          <t>1k1jeky</t>
+        </is>
+      </c>
+      <c r="B1011" t="inlineStr">
+        <is>
+          <t>Blueberry Milk</t>
+        </is>
+      </c>
+      <c r="C1011" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k1jeky</t>
+        </is>
+      </c>
+    </row>
+    <row r="1012">
+      <c r="A1012" t="inlineStr">
+        <is>
+          <t>1k1j289</t>
+        </is>
+      </c>
+      <c r="B1012" t="inlineStr">
+        <is>
+          <t>The hype is real</t>
+        </is>
+      </c>
+      <c r="C1012" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k1j289</t>
+        </is>
+      </c>
+    </row>
+    <row r="1013">
+      <c r="A1013" t="inlineStr">
+        <is>
+          <t>1k1i7xv</t>
+        </is>
+      </c>
+      <c r="B1013" t="inlineStr">
+        <is>
+          <t>Alien Invasion in the sun 🌞</t>
+        </is>
+      </c>
+      <c r="C1013" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/na2h2jhphfve1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1014">
+      <c r="A1014" t="inlineStr">
+        <is>
+          <t>1k1i7sf</t>
+        </is>
+      </c>
+      <c r="B1014" t="inlineStr">
+        <is>
+          <t>So I hallucinated ordering a BKL polish and now it’s Archived</t>
+        </is>
+      </c>
+      <c r="C1014" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k1i7sf/so_i_hallucinated_ordering_a_bkl_polish_and_now/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1015">
+      <c r="A1015" t="inlineStr">
+        <is>
+          <t>1k1hsmu</t>
+        </is>
+      </c>
+      <c r="B1015" t="inlineStr">
+        <is>
+          <t>Pink and Orange nails</t>
+        </is>
+      </c>
+      <c r="C1015" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k1hsmu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1016">
+      <c r="A1016" t="inlineStr">
+        <is>
+          <t>1k1hl7k</t>
+        </is>
+      </c>
+      <c r="B1016" t="inlineStr">
+        <is>
+          <t>Spring has sprung</t>
+        </is>
+      </c>
+      <c r="C1016" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k1hl7k</t>
+        </is>
+      </c>
+    </row>
+    <row r="1017">
+      <c r="A1017" t="inlineStr">
+        <is>
+          <t>1k1hcyi</t>
+        </is>
+      </c>
+      <c r="B1017" t="inlineStr">
+        <is>
+          <t>AI stamping plate was removed from PPU, maker is no longer part of PPU</t>
+        </is>
+      </c>
+      <c r="C1017" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k1hcyi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1018">
+      <c r="A1018" t="inlineStr">
+        <is>
+          <t>1k1gg5e</t>
+        </is>
+      </c>
+      <c r="B1018" t="inlineStr">
+        <is>
+          <t>My first magnetic and its a 1.50$ minibottle from the convenience store 😂</t>
+        </is>
+      </c>
+      <c r="C1018" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k1gg5e</t>
+        </is>
+      </c>
+    </row>
+    <row r="1019">
+      <c r="A1019" t="inlineStr">
+        <is>
+          <t>1k1g85r</t>
+        </is>
+      </c>
+      <c r="B1019" t="inlineStr">
+        <is>
+          <t>Human Magpie</t>
+        </is>
+      </c>
+      <c r="C1019" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/c2bymjo83fve1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1020">
+      <c r="A1020" t="inlineStr">
+        <is>
+          <t>1k1g62f</t>
+        </is>
+      </c>
+      <c r="B1020" t="inlineStr">
+        <is>
+          <t>My Spring/Easter nails (first time posting)</t>
+        </is>
+      </c>
+      <c r="C1020" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k1g62f</t>
+        </is>
+      </c>
+    </row>
+    <row r="1021">
+      <c r="A1021" t="inlineStr">
+        <is>
+          <t>1k1g078</t>
+        </is>
+      </c>
+      <c r="B1021" t="inlineStr">
+        <is>
+          <t>Are these too similar?</t>
+        </is>
+      </c>
+      <c r="C1021" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k1g078</t>
+        </is>
+      </c>
+    </row>
+    <row r="1022">
+      <c r="A1022" t="inlineStr">
+        <is>
+          <t>1k1fh6x</t>
+        </is>
+      </c>
+      <c r="B1022" t="inlineStr">
+        <is>
+          <t>what's your most irreplaceable bottle of polish?</t>
+        </is>
+      </c>
+      <c r="C1022" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k1fh6x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1023">
+      <c r="A1023" t="inlineStr">
+        <is>
+          <t>1k1f52x</t>
+        </is>
+      </c>
+      <c r="B1023" t="inlineStr">
+        <is>
+          <t>Fastest shipping in the history of ever?</t>
+        </is>
+      </c>
+      <c r="C1023" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qnktr9r4veve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1024">
+      <c r="A1024" t="inlineStr">
+        <is>
+          <t>1k1f0s9</t>
+        </is>
+      </c>
+      <c r="B1024" t="inlineStr">
+        <is>
+          <t>Can I use regular polish color in between gel base and top coat?</t>
+        </is>
+      </c>
+      <c r="C1024" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k1f0s9/can_i_use_regular_polish_color_in_between_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1025">
+      <c r="A1025" t="inlineStr">
+        <is>
+          <t>1k1eumx</t>
+        </is>
+      </c>
+      <c r="B1025" t="inlineStr">
+        <is>
+          <t>My bunny was sooo cute until I smudged it with top coat 🥴</t>
+        </is>
+      </c>
+      <c r="C1025" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6fck8k30teve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1026">
+      <c r="A1026" t="inlineStr">
+        <is>
+          <t>1k1eoxw</t>
+        </is>
+      </c>
+      <c r="B1026" t="inlineStr">
+        <is>
+          <t>Any dupes for Mooncat’s Curiosity’s Prey?</t>
+        </is>
+      </c>
+      <c r="C1026" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k1eoxw/any_dupes_for_mooncats_curiositys_prey/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1027">
+      <c r="A1027" t="inlineStr">
+        <is>
+          <t>1k1dzsi</t>
+        </is>
+      </c>
+      <c r="B1027" t="inlineStr">
+        <is>
+          <t>Who maintains the manipedia spread sheet?</t>
+        </is>
+      </c>
+      <c r="C1027" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k1dzsi/who_maintains_the_manipedia_spread_sheet/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1028">
+      <c r="A1028" t="inlineStr">
+        <is>
+          <t>1k1dzhc</t>
+        </is>
+      </c>
+      <c r="B1028" t="inlineStr">
+        <is>
+          <t>Good Scare Day in April</t>
+        </is>
+      </c>
+      <c r="C1028" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k1dzhc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1029">
+      <c r="A1029" t="inlineStr">
+        <is>
+          <t>1k1dzb7</t>
+        </is>
+      </c>
+      <c r="B1029" t="inlineStr">
+        <is>
+          <t>Spring vibes 💜🌸🌺🩷</t>
+        </is>
+      </c>
+      <c r="C1029" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qtuiklidmeve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1030">
+      <c r="A1030" t="inlineStr">
+        <is>
+          <t>1k1dvt6</t>
+        </is>
+      </c>
+      <c r="B1030" t="inlineStr">
+        <is>
+          <t>Battle of Holo Taco continues for me</t>
+        </is>
+      </c>
+      <c r="C1030" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k1dvt6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1031">
+      <c r="A1031" t="inlineStr">
+        <is>
+          <t>1k1dufm</t>
+        </is>
+      </c>
+      <c r="B1031" t="inlineStr">
+        <is>
+          <t>Glisten &amp; Glow top coat peeling</t>
+        </is>
+      </c>
+      <c r="C1031" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k1dufm/glisten_glow_top_coat_peeling/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1032">
+      <c r="A1032" t="inlineStr">
+        <is>
+          <t>1k1dmpe</t>
+        </is>
+      </c>
+      <c r="B1032" t="inlineStr">
+        <is>
+          <t>Rosenrot by Herzlack</t>
+        </is>
+      </c>
+      <c r="C1032" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k1dmpe</t>
+        </is>
+      </c>
+    </row>
+    <row r="1033">
+      <c r="A1033" t="inlineStr">
+        <is>
+          <t>1k1d8qk</t>
+        </is>
+      </c>
+      <c r="B1033" t="inlineStr">
+        <is>
+          <t>Pleasantly pleased with just one coat of this polish</t>
+        </is>
+      </c>
+      <c r="C1033" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k1d8qk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1034">
+      <c r="A1034" t="inlineStr">
+        <is>
+          <t>1k1d75g</t>
+        </is>
+      </c>
+      <c r="B1034" t="inlineStr">
+        <is>
+          <t>My new favorite blue</t>
+        </is>
+      </c>
+      <c r="C1034" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/un0vw6vfgeve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1035">
+      <c r="A1035" t="inlineStr">
+        <is>
+          <t>1k1cvjn</t>
+        </is>
+      </c>
+      <c r="B1035" t="inlineStr">
+        <is>
+          <t>Curing "regular" polish</t>
+        </is>
+      </c>
+      <c r="C1035" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k1cvjn/curing_regular_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1036">
+      <c r="A1036" t="inlineStr">
+        <is>
+          <t>1k1ctcz</t>
+        </is>
+      </c>
+      <c r="B1036" t="inlineStr">
+        <is>
+          <t>These came out SO pretty - by accident!</t>
+        </is>
+      </c>
+      <c r="C1036" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k1ctcz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1037">
+      <c r="A1037" t="inlineStr">
+        <is>
+          <t>1k1cmuk</t>
+        </is>
+      </c>
+      <c r="B1037" t="inlineStr">
+        <is>
+          <t>Parrot Polish w/ ILNP Topper</t>
+        </is>
+      </c>
+      <c r="C1037" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k1cmuk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1038">
+      <c r="A1038" t="inlineStr">
+        <is>
+          <t>1k1cdbh</t>
+        </is>
+      </c>
+      <c r="B1038" t="inlineStr">
+        <is>
+          <t>Crabs Is Bugs</t>
+        </is>
+      </c>
+      <c r="C1038" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/1jsqd4sh9eve1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1039">
+      <c r="A1039" t="inlineStr">
+        <is>
+          <t>1k1ca6g</t>
+        </is>
+      </c>
+      <c r="B1039" t="inlineStr">
+        <is>
+          <t>💖🌴Tropic Like It's Hot🌴💖</t>
+        </is>
+      </c>
+      <c r="C1039" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k1ca6g</t>
+        </is>
+      </c>
+    </row>
+    <row r="1040">
+      <c r="A1040" t="inlineStr">
+        <is>
+          <t>1k1c7wo</t>
+        </is>
+      </c>
+      <c r="B1040" t="inlineStr">
+        <is>
+          <t>Top coat help</t>
+        </is>
+      </c>
+      <c r="C1040" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k1c7wo/top_coat_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1041">
+      <c r="A1041" t="inlineStr">
+        <is>
+          <t>1k1c7a7</t>
+        </is>
+      </c>
+      <c r="B1041" t="inlineStr">
+        <is>
+          <t>Tropical skittle for the beach</t>
+        </is>
+      </c>
+      <c r="C1041" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k1c7a7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1042">
+      <c r="A1042" t="inlineStr">
+        <is>
+          <t>1k1c13w</t>
+        </is>
+      </c>
+      <c r="B1042" t="inlineStr">
+        <is>
+          <t>Easter blobs</t>
+        </is>
+      </c>
+      <c r="C1042" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k1c13w</t>
+        </is>
+      </c>
+    </row>
+    <row r="1043">
+      <c r="A1043" t="inlineStr">
+        <is>
+          <t>1k19pmh</t>
+        </is>
+      </c>
+      <c r="B1043" t="inlineStr">
+        <is>
+          <t>Thrifted YSL Nail Polish</t>
+        </is>
+      </c>
+      <c r="C1043" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e56xo16vjdve1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1044">
+      <c r="A1044" t="inlineStr">
+        <is>
+          <t>1k19c9x</t>
+        </is>
+      </c>
+      <c r="B1044" t="inlineStr">
+        <is>
+          <t>Biab keeps on lifting</t>
+        </is>
+      </c>
+      <c r="C1044" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k19c9x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1045">
+      <c r="A1045" t="inlineStr">
+        <is>
+          <t>1k1z66p</t>
+        </is>
+      </c>
+      <c r="B1045" t="inlineStr">
+        <is>
+          <t>Was super inspired by r/Hexfiles13 ✨</t>
+        </is>
+      </c>
+      <c r="C1045" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k1z66p</t>
+        </is>
+      </c>
+    </row>
+    <row r="1046">
+      <c r="A1046" t="inlineStr">
+        <is>
+          <t>1k1wkuo</t>
+        </is>
+      </c>
+      <c r="B1046" t="inlineStr">
+        <is>
+          <t>Gel Hybrid Matte Wild Flowers</t>
+        </is>
+      </c>
+      <c r="C1046" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k1wkuo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1047">
+      <c r="A1047" t="inlineStr">
+        <is>
+          <t>1k1vwiz</t>
+        </is>
+      </c>
+      <c r="B1047" t="inlineStr">
+        <is>
+          <t>Just started my nail art journey</t>
+        </is>
+      </c>
+      <c r="C1047" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k1vwiz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1048">
+      <c r="A1048" t="inlineStr">
+        <is>
+          <t>1k1vq01</t>
+        </is>
+      </c>
+      <c r="B1048" t="inlineStr">
+        <is>
+          <t>Fill over cat eye</t>
+        </is>
+      </c>
+      <c r="C1048" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1k1vq01/fill_over_cat_eye/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1049">
+      <c r="A1049" t="inlineStr">
+        <is>
+          <t>1k1ttd5</t>
+        </is>
+      </c>
+      <c r="B1049" t="inlineStr">
+        <is>
+          <t>"it shouldn't take 4 hours" I said. "keep it simple" I said</t>
+        </is>
+      </c>
+      <c r="C1049" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k1ttd5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1050">
+      <c r="A1050" t="inlineStr">
+        <is>
+          <t>1k1t7eh</t>
+        </is>
+      </c>
+      <c r="B1050" t="inlineStr">
+        <is>
+          <t>Pond! 🐸</t>
+        </is>
+      </c>
+      <c r="C1050" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/az5xp1unxhve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1051">
+      <c r="A1051" t="inlineStr">
+        <is>
+          <t>1k1so9k</t>
+        </is>
+      </c>
+      <c r="B1051" t="inlineStr">
+        <is>
+          <t>All nails I've done this week! (Open to tips and critique!!)</t>
+        </is>
+      </c>
+      <c r="C1051" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k1so9k</t>
+        </is>
+      </c>
+    </row>
+    <row r="1052">
+      <c r="A1052" t="inlineStr">
+        <is>
+          <t>1k1rolr</t>
+        </is>
+      </c>
+      <c r="B1052" t="inlineStr">
+        <is>
+          <t>First time doing nail art!</t>
+        </is>
+      </c>
+      <c r="C1052" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qrf7585njhve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1053">
+      <c r="A1053" t="inlineStr">
+        <is>
+          <t>1k1ph84</t>
+        </is>
+      </c>
+      <c r="B1053" t="inlineStr">
+        <is>
+          <t>Xalitla Art inspired nails for my Mexican vacay 🇲🇽</t>
+        </is>
+      </c>
+      <c r="C1053" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k1ph84</t>
+        </is>
+      </c>
+    </row>
+    <row r="1054">
+      <c r="A1054" t="inlineStr">
+        <is>
+          <t>1k1myzg</t>
+        </is>
+      </c>
+      <c r="B1054" t="inlineStr">
+        <is>
+          <t>Painting</t>
+        </is>
+      </c>
+      <c r="C1054" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eus7h1azggve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1055">
+      <c r="A1055" t="inlineStr">
+        <is>
+          <t>1k1mr9x</t>
+        </is>
+      </c>
+      <c r="B1055" t="inlineStr">
+        <is>
+          <t>Is there anything I can use for 3d nails that doesn’t need uv or resin ?</t>
+        </is>
+      </c>
+      <c r="C1055" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1k1mr9x/is_there_anything_i_can_use_for_3d_nails_that/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1056">
+      <c r="A1056" t="inlineStr">
+        <is>
+          <t>1k1lwyi</t>
+        </is>
+      </c>
+      <c r="B1056" t="inlineStr">
+        <is>
+          <t>My Easter-Spring Nails 🩷</t>
+        </is>
+      </c>
+      <c r="C1056" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k1lwyi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1057">
+      <c r="A1057" t="inlineStr">
+        <is>
+          <t>1k1l9xi</t>
+        </is>
+      </c>
+      <c r="B1057" t="inlineStr">
+        <is>
+          <t>Green and jeans</t>
+        </is>
+      </c>
+      <c r="C1057" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k1l9xi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1058">
+      <c r="A1058" t="inlineStr">
+        <is>
+          <t>1k1iuv9</t>
+        </is>
+      </c>
+      <c r="B1058" t="inlineStr">
+        <is>
+          <t>Favorit</t>
+        </is>
+      </c>
+      <c r="C1058" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uvzcw7gdmfve1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1059">
+      <c r="A1059" t="inlineStr">
+        <is>
+          <t>1k1ise0</t>
+        </is>
+      </c>
+      <c r="B1059" t="inlineStr">
+        <is>
+          <t>Pink nails🩷</t>
+        </is>
+      </c>
+      <c r="C1059" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k1ise0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1060">
+      <c r="A1060" t="inlineStr">
+        <is>
+          <t>1k1f3x6</t>
+        </is>
+      </c>
+      <c r="B1060" t="inlineStr">
+        <is>
+          <t>Practiced lines. How did I do?</t>
+        </is>
+      </c>
+      <c r="C1060" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qvosolwvueve1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1061">
+      <c r="A1061" t="inlineStr">
+        <is>
+          <t>1k1d5sk</t>
+        </is>
+      </c>
+      <c r="B1061" t="inlineStr">
+        <is>
+          <t>Citrus nails! (And a question)</t>
+        </is>
+      </c>
+      <c r="C1061" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k1d5sk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1062">
+      <c r="A1062" t="inlineStr">
+        <is>
+          <t>1k1cw52</t>
+        </is>
+      </c>
+      <c r="B1062" t="inlineStr">
+        <is>
+          <t>This took a lot longer than it should have 😩</t>
+        </is>
+      </c>
+      <c r="C1062" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tu0naux0eeve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1063">
+      <c r="A1063" t="inlineStr">
+        <is>
+          <t>1k1cqo9</t>
+        </is>
+      </c>
+      <c r="B1063" t="inlineStr">
+        <is>
+          <t>Pre-drawn nails for my mom who won't sit still for an hour.</t>
+        </is>
+      </c>
+      <c r="C1063" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4fzbr7gqceve1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1064">
+      <c r="A1064" t="inlineStr">
+        <is>
+          <t>1k1codb</t>
+        </is>
+      </c>
+      <c r="B1064" t="inlineStr">
+        <is>
+          <t>Been loving fruit nails lately 🫐</t>
+        </is>
+      </c>
+      <c r="C1064" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k1codb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1065">
+      <c r="A1065" t="inlineStr">
+        <is>
+          <t>1k196x5</t>
+        </is>
+      </c>
+      <c r="B1065" t="inlineStr">
+        <is>
+          <t>Was feeling the spring sunshine</t>
+        </is>
+      </c>
+      <c r="C1065" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mx6s4p6pddve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1066">
+      <c r="A1066" t="inlineStr">
+        <is>
+          <t>1k187ew</t>
+        </is>
+      </c>
+      <c r="B1066" t="inlineStr">
+        <is>
+          <t>Favorite summer nails</t>
+        </is>
+      </c>
+      <c r="C1066" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k187ew</t>
+        </is>
+      </c>
+    </row>
+    <row r="1067">
+      <c r="A1067" t="inlineStr">
+        <is>
+          <t>1k0q5ae</t>
+        </is>
+      </c>
+      <c r="B1067" t="inlineStr">
+        <is>
+          <t>Blueberries and Strawberries, did you like them?˚˖𓍢🌷✧˚.🎀⋆</t>
+        </is>
+      </c>
+      <c r="C1067" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pihutwjwe8ve1.png</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sat Apr 19 08:10:03 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_04_20.xlsx
+++ b/data/collected_data/2025_04_20.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1067"/>
+  <dimension ref="A1:C1276"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -18572,6 +18572,3559 @@
         </is>
       </c>
     </row>
+    <row r="1068">
+      <c r="A1068" t="inlineStr">
+        <is>
+          <t>1k2rdno</t>
+        </is>
+      </c>
+      <c r="B1068" t="inlineStr">
+        <is>
+          <t>New to getting nails done...natural length question</t>
+        </is>
+      </c>
+      <c r="C1068" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k2rdno</t>
+        </is>
+      </c>
+    </row>
+    <row r="1069">
+      <c r="A1069" t="inlineStr">
+        <is>
+          <t>1k2qnlu</t>
+        </is>
+      </c>
+      <c r="B1069" t="inlineStr">
+        <is>
+          <t>🤍</t>
+        </is>
+      </c>
+      <c r="C1069" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k2qnlu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1070">
+      <c r="A1070" t="inlineStr">
+        <is>
+          <t>1k2qj2v</t>
+        </is>
+      </c>
+      <c r="B1070" t="inlineStr">
+        <is>
+          <t>Do these look good on me? I dunno what I feel about how the “blush” effect went and I have a beach trip tomorrow :((</t>
+        </is>
+      </c>
+      <c r="C1070" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4kvwnw36rqve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1071">
+      <c r="A1071" t="inlineStr">
+        <is>
+          <t>1k2qcls</t>
+        </is>
+      </c>
+      <c r="B1071" t="inlineStr">
+        <is>
+          <t>the same nail keeps popping off</t>
+        </is>
+      </c>
+      <c r="C1071" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k2qcls/the_same_nail_keeps_popping_off/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1072">
+      <c r="A1072" t="inlineStr">
+        <is>
+          <t>1k2q6f0</t>
+        </is>
+      </c>
+      <c r="B1072" t="inlineStr">
+        <is>
+          <t>Builder gel??</t>
+        </is>
+      </c>
+      <c r="C1072" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k2q6f0/builder_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1073">
+      <c r="A1073" t="inlineStr">
+        <is>
+          <t>1k2pg3e</t>
+        </is>
+      </c>
+      <c r="B1073" t="inlineStr">
+        <is>
+          <t>I loved my new nails</t>
+        </is>
+      </c>
+      <c r="C1073" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n3f48mzwdqve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1074">
+      <c r="A1074" t="inlineStr">
+        <is>
+          <t>1k2mcdb</t>
+        </is>
+      </c>
+      <c r="B1074" t="inlineStr">
+        <is>
+          <t>Please help 😭 i just applied glue on nails and i want them OFF</t>
+        </is>
+      </c>
+      <c r="C1074" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k2mcdb/please_help_i_just_applied_glue_on_nails_and_i/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1075">
+      <c r="A1075" t="inlineStr">
+        <is>
+          <t>1k2mirl</t>
+        </is>
+      </c>
+      <c r="B1075" t="inlineStr">
+        <is>
+          <t>Got my nails done for the first time a month or so ago! Inspo posted by baranasarvi on Pinterest!</t>
+        </is>
+      </c>
+      <c r="C1075" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k2mirl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1076">
+      <c r="A1076" t="inlineStr">
+        <is>
+          <t>1k2mmvd</t>
+        </is>
+      </c>
+      <c r="B1076" t="inlineStr">
+        <is>
+          <t>What happened to my nail? It’s splitting?</t>
+        </is>
+      </c>
+      <c r="C1076" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ho01a42sipve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1077">
+      <c r="A1077" t="inlineStr">
+        <is>
+          <t>1k2myk1</t>
+        </is>
+      </c>
+      <c r="B1077" t="inlineStr">
+        <is>
+          <t>very hungry caterpillar for spring :)</t>
+        </is>
+      </c>
+      <c r="C1077" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ur1bty83mpve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1078">
+      <c r="A1078" t="inlineStr">
+        <is>
+          <t>1k2owes</t>
+        </is>
+      </c>
+      <c r="B1078" t="inlineStr">
+        <is>
+          <t>my natural nails w/ clear builder gel on top!</t>
+        </is>
+      </c>
+      <c r="C1078" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k2owes</t>
+        </is>
+      </c>
+    </row>
+    <row r="1079">
+      <c r="A1079" t="inlineStr">
+        <is>
+          <t>1k2ouls</t>
+        </is>
+      </c>
+      <c r="B1079" t="inlineStr">
+        <is>
+          <t>I love this set!</t>
+        </is>
+      </c>
+      <c r="C1079" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gqkdjxlv6qve1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1080">
+      <c r="A1080" t="inlineStr">
+        <is>
+          <t>1k2ojh4</t>
+        </is>
+      </c>
+      <c r="B1080" t="inlineStr">
+        <is>
+          <t>Went to a new new nail tech</t>
+        </is>
+      </c>
+      <c r="C1080" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k2ojh4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1081">
+      <c r="A1081" t="inlineStr">
+        <is>
+          <t>1k2oi5z</t>
+        </is>
+      </c>
+      <c r="B1081" t="inlineStr">
+        <is>
+          <t>Nail biting relapse</t>
+        </is>
+      </c>
+      <c r="C1081" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k2oi5z/nail_biting_relapse/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1082">
+      <c r="A1082" t="inlineStr">
+        <is>
+          <t>1k2o6w2</t>
+        </is>
+      </c>
+      <c r="B1082" t="inlineStr">
+        <is>
+          <t>Obsessed w these</t>
+        </is>
+      </c>
+      <c r="C1082" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pmjb09obzpve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1083">
+      <c r="A1083" t="inlineStr">
+        <is>
+          <t>1k2n8y1</t>
+        </is>
+      </c>
+      <c r="B1083" t="inlineStr">
+        <is>
+          <t>Snowed today, snowflake nails!</t>
+        </is>
+      </c>
+      <c r="C1083" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k2n8y1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1084">
+      <c r="A1084" t="inlineStr">
+        <is>
+          <t>1k2n57m</t>
+        </is>
+      </c>
+      <c r="B1084" t="inlineStr">
+        <is>
+          <t>Spring nails</t>
+        </is>
+      </c>
+      <c r="C1084" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r0lcxpd2opve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1085">
+      <c r="A1085" t="inlineStr">
+        <is>
+          <t>1k2n3ny</t>
+        </is>
+      </c>
+      <c r="B1085" t="inlineStr">
+        <is>
+          <t>The clippers call to me…</t>
+        </is>
+      </c>
+      <c r="C1085" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8brkjfdlnpve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1086">
+      <c r="A1086" t="inlineStr">
+        <is>
+          <t>1k2n2xi</t>
+        </is>
+      </c>
+      <c r="B1086" t="inlineStr">
+        <is>
+          <t>Easter/BDay Nails</t>
+        </is>
+      </c>
+      <c r="C1086" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k2n2xi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1087">
+      <c r="A1087" t="inlineStr">
+        <is>
+          <t>1k2n15j</t>
+        </is>
+      </c>
+      <c r="B1087" t="inlineStr">
+        <is>
+          <t>First time using cat eye gel!</t>
+        </is>
+      </c>
+      <c r="C1087" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k2n15j</t>
+        </is>
+      </c>
+    </row>
+    <row r="1088">
+      <c r="A1088" t="inlineStr">
+        <is>
+          <t>1k2mw5a</t>
+        </is>
+      </c>
+      <c r="B1088" t="inlineStr">
+        <is>
+          <t>Alternating lavender/grass green short almond nails for Spring 🌱</t>
+        </is>
+      </c>
+      <c r="C1088" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k2mw5a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1089">
+      <c r="A1089" t="inlineStr">
+        <is>
+          <t>1k2mjpi</t>
+        </is>
+      </c>
+      <c r="B1089" t="inlineStr">
+        <is>
+          <t>Is this normal?</t>
+        </is>
+      </c>
+      <c r="C1089" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cpmd83wuhpve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1090">
+      <c r="A1090" t="inlineStr">
+        <is>
+          <t>1k2ltye</t>
+        </is>
+      </c>
+      <c r="B1090" t="inlineStr">
+        <is>
+          <t>Some of my favorite sets on my natural nails over the months (from most recent to older)</t>
+        </is>
+      </c>
+      <c r="C1090" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k2ltye</t>
+        </is>
+      </c>
+    </row>
+    <row r="1091">
+      <c r="A1091" t="inlineStr">
+        <is>
+          <t>1k2mcsa</t>
+        </is>
+      </c>
+      <c r="B1091" t="inlineStr">
+        <is>
+          <t>Fresh nails, fresh vibes 🤍</t>
+        </is>
+      </c>
+      <c r="C1091" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z1s66wlvfpve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1092">
+      <c r="A1092" t="inlineStr">
+        <is>
+          <t>1k2m5ek</t>
+        </is>
+      </c>
+      <c r="B1092" t="inlineStr">
+        <is>
+          <t>Throwback to last year when I got my nails done, and she completely messed it up and I even told her to fix it but she goes u have to pay more 💀</t>
+        </is>
+      </c>
+      <c r="C1092" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k2m5ek</t>
+        </is>
+      </c>
+    </row>
+    <row r="1093">
+      <c r="A1093" t="inlineStr">
+        <is>
+          <t>1k2maxq</t>
+        </is>
+      </c>
+      <c r="B1093" t="inlineStr">
+        <is>
+          <t>Finished these today at home. Nail Thoughts builder base.</t>
+        </is>
+      </c>
+      <c r="C1093" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k2maxq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1094">
+      <c r="A1094" t="inlineStr">
+        <is>
+          <t>1k2lzre</t>
+        </is>
+      </c>
+      <c r="B1094" t="inlineStr">
+        <is>
+          <t>I think my artist popped off</t>
+        </is>
+      </c>
+      <c r="C1094" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wydcijo9cpve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1095">
+      <c r="A1095" t="inlineStr">
+        <is>
+          <t>1k2lycv</t>
+        </is>
+      </c>
+      <c r="B1095" t="inlineStr">
+        <is>
+          <t>pastel celestial obsession 😍</t>
+        </is>
+      </c>
+      <c r="C1095" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k2lycv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1096">
+      <c r="A1096" t="inlineStr">
+        <is>
+          <t>1k2lcpa</t>
+        </is>
+      </c>
+      <c r="B1096" t="inlineStr">
+        <is>
+          <t>I have an important meeting and I would like you to help me choose which of these options would be the most delicate</t>
+        </is>
+      </c>
+      <c r="C1096" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k2lcpa</t>
+        </is>
+      </c>
+    </row>
+    <row r="1097">
+      <c r="A1097" t="inlineStr">
+        <is>
+          <t>1k2ldun</t>
+        </is>
+      </c>
+      <c r="B1097" t="inlineStr">
+        <is>
+          <t>Gel allergy</t>
+        </is>
+      </c>
+      <c r="C1097" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k2ldun/gel_allergy/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1098">
+      <c r="A1098" t="inlineStr">
+        <is>
+          <t>1k2li3s</t>
+        </is>
+      </c>
+      <c r="B1098" t="inlineStr">
+        <is>
+          <t>Light to cure Japanese gel?</t>
+        </is>
+      </c>
+      <c r="C1098" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k2li3s/light_to_cure_japanese_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1099">
+      <c r="A1099" t="inlineStr">
+        <is>
+          <t>1k2kmql</t>
+        </is>
+      </c>
+      <c r="B1099" t="inlineStr">
+        <is>
+          <t>Told my nail lady I wanted soft pink</t>
+        </is>
+      </c>
+      <c r="C1099" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/03836aw0zove1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1100">
+      <c r="A1100" t="inlineStr">
+        <is>
+          <t>1k2k8ak</t>
+        </is>
+      </c>
+      <c r="B1100" t="inlineStr">
+        <is>
+          <t>First time doing chrome</t>
+        </is>
+      </c>
+      <c r="C1100" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/6le655j8vove1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1101">
+      <c r="A1101" t="inlineStr">
+        <is>
+          <t>1k2k3fh</t>
+        </is>
+      </c>
+      <c r="B1101" t="inlineStr">
+        <is>
+          <t>420 💚😶‍🌫️🍃</t>
+        </is>
+      </c>
+      <c r="C1101" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/81gj6c6ytove1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1102">
+      <c r="A1102" t="inlineStr">
+        <is>
+          <t>1k2k2ir</t>
+        </is>
+      </c>
+      <c r="B1102" t="inlineStr">
+        <is>
+          <t>Showing Appreciation For The Wifeys Russian Manicure 💅🏾</t>
+        </is>
+      </c>
+      <c r="C1102" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5w58fiyotove1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1103">
+      <c r="A1103" t="inlineStr">
+        <is>
+          <t>1k2hekr</t>
+        </is>
+      </c>
+      <c r="B1103" t="inlineStr">
+        <is>
+          <t>My Easter Nails</t>
+        </is>
+      </c>
+      <c r="C1103" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gklyqb9w5ove1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1104">
+      <c r="A1104" t="inlineStr">
+        <is>
+          <t>1k2izo5</t>
+        </is>
+      </c>
+      <c r="B1104" t="inlineStr">
+        <is>
+          <t>Unsure if I'm liking these or not</t>
+        </is>
+      </c>
+      <c r="C1104" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k2izo5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1105">
+      <c r="A1105" t="inlineStr">
+        <is>
+          <t>1k2jc6y</t>
+        </is>
+      </c>
+      <c r="B1105" t="inlineStr">
+        <is>
+          <t>My request was blue cow and I got blue camo but I still love it!</t>
+        </is>
+      </c>
+      <c r="C1105" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mgg3u39wmove1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1106">
+      <c r="A1106" t="inlineStr">
+        <is>
+          <t>1k2j2n1</t>
+        </is>
+      </c>
+      <c r="B1106" t="inlineStr">
+        <is>
+          <t>are these decent?</t>
+        </is>
+      </c>
+      <c r="C1106" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zdwvm6lgkove1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1107">
+      <c r="A1107" t="inlineStr">
+        <is>
+          <t>1k2ishw</t>
+        </is>
+      </c>
+      <c r="B1107" t="inlineStr">
+        <is>
+          <t>First time press ons!</t>
+        </is>
+      </c>
+      <c r="C1107" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k2ishw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1108">
+      <c r="A1108" t="inlineStr">
+        <is>
+          <t>1k2isfl</t>
+        </is>
+      </c>
+      <c r="B1108" t="inlineStr">
+        <is>
+          <t>🖤🖤💅🏽</t>
+        </is>
+      </c>
+      <c r="C1108" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k2isfl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1109">
+      <c r="A1109" t="inlineStr">
+        <is>
+          <t>1k2is49</t>
+        </is>
+      </c>
+      <c r="B1109" t="inlineStr">
+        <is>
+          <t>all hand painted nail art</t>
+        </is>
+      </c>
+      <c r="C1109" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k2is49</t>
+        </is>
+      </c>
+    </row>
+    <row r="1110">
+      <c r="A1110" t="inlineStr">
+        <is>
+          <t>1k2irb3</t>
+        </is>
+      </c>
+      <c r="B1110" t="inlineStr">
+        <is>
+          <t>Got these done today, not sure how I feel about them.</t>
+        </is>
+      </c>
+      <c r="C1110" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k2irb3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1111">
+      <c r="A1111" t="inlineStr">
+        <is>
+          <t>1k2ioss</t>
+        </is>
+      </c>
+      <c r="B1111" t="inlineStr">
+        <is>
+          <t>My new fave colour.</t>
+        </is>
+      </c>
+      <c r="C1111" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8s907epygove1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1112">
+      <c r="A1112" t="inlineStr">
+        <is>
+          <t>1k2h0me</t>
+        </is>
+      </c>
+      <c r="B1112" t="inlineStr">
+        <is>
+          <t>💜💚 Easter skittle inspired by tulips 🌷</t>
+        </is>
+      </c>
+      <c r="C1112" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k2h0me</t>
+        </is>
+      </c>
+    </row>
+    <row r="1113">
+      <c r="A1113" t="inlineStr">
+        <is>
+          <t>1k2gini</t>
+        </is>
+      </c>
+      <c r="B1113" t="inlineStr">
+        <is>
+          <t>Self training on my nails</t>
+        </is>
+      </c>
+      <c r="C1113" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k2gini</t>
+        </is>
+      </c>
+    </row>
+    <row r="1114">
+      <c r="A1114" t="inlineStr">
+        <is>
+          <t>1k2i959</t>
+        </is>
+      </c>
+      <c r="B1114" t="inlineStr">
+        <is>
+          <t>Novice to DIY nails and looking for advice and product recommendations pls!</t>
+        </is>
+      </c>
+      <c r="C1114" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k2i959/novice_to_diy_nails_and_looking_for_advice_and/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1115">
+      <c r="A1115" t="inlineStr">
+        <is>
+          <t>1k2ibr7</t>
+        </is>
+      </c>
+      <c r="B1115" t="inlineStr">
+        <is>
+          <t>which one’s your favorite? 💞</t>
+        </is>
+      </c>
+      <c r="C1115" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k2ibr7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1116">
+      <c r="A1116" t="inlineStr">
+        <is>
+          <t>1k2imn7</t>
+        </is>
+      </c>
+      <c r="B1116" t="inlineStr">
+        <is>
+          <t>Love a simple cat eye polish💓</t>
+        </is>
+      </c>
+      <c r="C1116" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ayruihnfgove1.gif</t>
+        </is>
+      </c>
+    </row>
+    <row r="1117">
+      <c r="A1117" t="inlineStr">
+        <is>
+          <t>1k2i9ly</t>
+        </is>
+      </c>
+      <c r="B1117" t="inlineStr">
+        <is>
+          <t>I got this adorable strawberry manicure! I went to Lina’s Nails in Port Orange FL. So if ur ever there give them a try! The lady who did them was so sweet. I can’t get over how good of a job she did!</t>
+        </is>
+      </c>
+      <c r="C1117" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k2i9ly</t>
+        </is>
+      </c>
+    </row>
+    <row r="1118">
+      <c r="A1118" t="inlineStr">
+        <is>
+          <t>1k2i8vt</t>
+        </is>
+      </c>
+      <c r="B1118" t="inlineStr">
+        <is>
+          <t>So at first i was not sure, but i love the final job, simple.</t>
+        </is>
+      </c>
+      <c r="C1118" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/no11zxg3dove1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1119">
+      <c r="A1119" t="inlineStr">
+        <is>
+          <t>1k2i5t6</t>
+        </is>
+      </c>
+      <c r="B1119" t="inlineStr">
+        <is>
+          <t>Birthday nails</t>
+        </is>
+      </c>
+      <c r="C1119" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tqs6mx5dcove1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1120">
+      <c r="A1120" t="inlineStr">
+        <is>
+          <t>1k2hf5i</t>
+        </is>
+      </c>
+      <c r="B1120" t="inlineStr">
+        <is>
+          <t>2nd Time in my life trying to paint black nails (dark colors)</t>
+        </is>
+      </c>
+      <c r="C1120" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k2hf5i</t>
+        </is>
+      </c>
+    </row>
+    <row r="1121">
+      <c r="A1121" t="inlineStr">
+        <is>
+          <t>1k2h8zd</t>
+        </is>
+      </c>
+      <c r="B1121" t="inlineStr">
+        <is>
+          <t>First time doing my own nails! I love them but can't wait to get more practice!</t>
+        </is>
+      </c>
+      <c r="C1121" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/unyfm2am4ove1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1122">
+      <c r="A1122" t="inlineStr">
+        <is>
+          <t>1k2fuw7</t>
+        </is>
+      </c>
+      <c r="B1122" t="inlineStr">
+        <is>
+          <t>Never been so obsessed</t>
+        </is>
+      </c>
+      <c r="C1122" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/m07hhugbtnve1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1123">
+      <c r="A1123" t="inlineStr">
+        <is>
+          <t>1k2ewcm</t>
+        </is>
+      </c>
+      <c r="B1123" t="inlineStr">
+        <is>
+          <t>What I wanted vs what I got from @topcoatnails</t>
+        </is>
+      </c>
+      <c r="C1123" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k2ewcm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1124">
+      <c r="A1124" t="inlineStr">
+        <is>
+          <t>1k2febw</t>
+        </is>
+      </c>
+      <c r="B1124" t="inlineStr">
+        <is>
+          <t>Did my friend’s and I’s nails💕</t>
+        </is>
+      </c>
+      <c r="C1124" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oukpq4frpnve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1125">
+      <c r="A1125" t="inlineStr">
+        <is>
+          <t>1k2famq</t>
+        </is>
+      </c>
+      <c r="B1125" t="inlineStr">
+        <is>
+          <t>Estoy muy contenta con este resultado</t>
+        </is>
+      </c>
+      <c r="C1125" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/34f5okayonve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1126">
+      <c r="A1126" t="inlineStr">
+        <is>
+          <t>1k2f5ya</t>
+        </is>
+      </c>
+      <c r="B1126" t="inlineStr">
+        <is>
+          <t>how are they?</t>
+        </is>
+      </c>
+      <c r="C1126" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5toa8bjynnve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1127">
+      <c r="A1127" t="inlineStr">
+        <is>
+          <t>1k2f23j</t>
+        </is>
+      </c>
+      <c r="B1127" t="inlineStr">
+        <is>
+          <t>Roast my Easter Egg Nails</t>
+        </is>
+      </c>
+      <c r="C1127" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k2f23j</t>
+        </is>
+      </c>
+    </row>
+    <row r="1128">
+      <c r="A1128" t="inlineStr">
+        <is>
+          <t>1k2eo81</t>
+        </is>
+      </c>
+      <c r="B1128" t="inlineStr">
+        <is>
+          <t>Classic.</t>
+        </is>
+      </c>
+      <c r="C1128" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rna5jtj5knve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1129">
+      <c r="A1129" t="inlineStr">
+        <is>
+          <t>1k2el1f</t>
+        </is>
+      </c>
+      <c r="B1129" t="inlineStr">
+        <is>
+          <t>Wedding nails + a few faves!</t>
+        </is>
+      </c>
+      <c r="C1129" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k2el1f</t>
+        </is>
+      </c>
+    </row>
+    <row r="1130">
+      <c r="A1130" t="inlineStr">
+        <is>
+          <t>1k2eho4</t>
+        </is>
+      </c>
+      <c r="B1130" t="inlineStr">
+        <is>
+          <t>What type of nails do I have and what would look good?</t>
+        </is>
+      </c>
+      <c r="C1130" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k2eho4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1131">
+      <c r="A1131" t="inlineStr">
+        <is>
+          <t>1k2eh4t</t>
+        </is>
+      </c>
+      <c r="B1131" t="inlineStr">
+        <is>
+          <t>Spring Flower Nail Set 🌺</t>
+        </is>
+      </c>
+      <c r="C1131" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k2eh4t</t>
+        </is>
+      </c>
+    </row>
+    <row r="1132">
+      <c r="A1132" t="inlineStr">
+        <is>
+          <t>1k2dmbn</t>
+        </is>
+      </c>
+      <c r="B1132" t="inlineStr">
+        <is>
+          <t>DIY gel nail "extensions" attempt #2</t>
+        </is>
+      </c>
+      <c r="C1132" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k2dmbn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1133">
+      <c r="A1133" t="inlineStr">
+        <is>
+          <t>1k2dsfl</t>
+        </is>
+      </c>
+      <c r="B1133" t="inlineStr">
+        <is>
+          <t>gel x or hard/builder gel? which is better for your nails?</t>
+        </is>
+      </c>
+      <c r="C1133" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k2dsfl/gel_x_or_hardbuilder_gel_which_is_better_for_your/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1134">
+      <c r="A1134" t="inlineStr">
+        <is>
+          <t>1k2dri0</t>
+        </is>
+      </c>
+      <c r="B1134" t="inlineStr">
+        <is>
+          <t>Saying "florals for spring? Groundbreaking" when wearing florals in spring? Groundbreaking</t>
+        </is>
+      </c>
+      <c r="C1134" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cw4hwsn5dnve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1135">
+      <c r="A1135" t="inlineStr">
+        <is>
+          <t>1k2dipt</t>
+        </is>
+      </c>
+      <c r="B1135" t="inlineStr">
+        <is>
+          <t>Didn’t expect to fall in love with white nails, but here we are 🤍💖</t>
+        </is>
+      </c>
+      <c r="C1135" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k2dipt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1136">
+      <c r="A1136" t="inlineStr">
+        <is>
+          <t>1k2dh84</t>
+        </is>
+      </c>
+      <c r="B1136" t="inlineStr">
+        <is>
+          <t>First time getting my nails done professionally and probably the last :(</t>
+        </is>
+      </c>
+      <c r="C1136" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k2dh84</t>
+        </is>
+      </c>
+    </row>
+    <row r="1137">
+      <c r="A1137" t="inlineStr">
+        <is>
+          <t>1k2depj</t>
+        </is>
+      </c>
+      <c r="B1137" t="inlineStr">
+        <is>
+          <t>Doggie approved</t>
+        </is>
+      </c>
+      <c r="C1137" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k2depj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1138">
+      <c r="A1138" t="inlineStr">
+        <is>
+          <t>1k2cyvm</t>
+        </is>
+      </c>
+      <c r="B1138" t="inlineStr">
+        <is>
+          <t>Fresh set</t>
+        </is>
+      </c>
+      <c r="C1138" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k2cyvm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1139">
+      <c r="A1139" t="inlineStr">
+        <is>
+          <t>1k2clfn</t>
+        </is>
+      </c>
+      <c r="B1139" t="inlineStr">
+        <is>
+          <t>Too soon for new set?</t>
+        </is>
+      </c>
+      <c r="C1139" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k2clfn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1140">
+      <c r="A1140" t="inlineStr">
+        <is>
+          <t>1k2c5tc</t>
+        </is>
+      </c>
+      <c r="B1140" t="inlineStr">
+        <is>
+          <t>New fresh fill. Some bright purple &amp; unicorn chrome. I’m in 💜💜💜💜💜.</t>
+        </is>
+      </c>
+      <c r="C1140" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a1iayfhv0nve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1141">
+      <c r="A1141" t="inlineStr">
+        <is>
+          <t>1k2bfun</t>
+        </is>
+      </c>
+      <c r="B1141" t="inlineStr">
+        <is>
+          <t>Some more of my nail art..</t>
+        </is>
+      </c>
+      <c r="C1141" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k2bfun</t>
+        </is>
+      </c>
+    </row>
+    <row r="1142">
+      <c r="A1142" t="inlineStr">
+        <is>
+          <t>1k2b7e5</t>
+        </is>
+      </c>
+      <c r="B1142" t="inlineStr">
+        <is>
+          <t>Went to a new place/nail tech. Too thick or not?</t>
+        </is>
+      </c>
+      <c r="C1142" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k2b7e5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1143">
+      <c r="A1143" t="inlineStr">
+        <is>
+          <t>1k2b5w4</t>
+        </is>
+      </c>
+      <c r="B1143" t="inlineStr">
+        <is>
+          <t>Western Dreams</t>
+        </is>
+      </c>
+      <c r="C1143" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k2b5w4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1144">
+      <c r="A1144" t="inlineStr">
+        <is>
+          <t>1k2b4qr</t>
+        </is>
+      </c>
+      <c r="B1144" t="inlineStr">
+        <is>
+          <t>Can you tell these are gel wraps? And does it look okay?</t>
+        </is>
+      </c>
+      <c r="C1144" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/16mmjiy7tmve1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1145">
+      <c r="A1145" t="inlineStr">
+        <is>
+          <t>1k2b1u7</t>
+        </is>
+      </c>
+      <c r="B1145" t="inlineStr">
+        <is>
+          <t>First time going to an independent nail tech, loved this set ♥️</t>
+        </is>
+      </c>
+      <c r="C1145" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rge88vomsmve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1146">
+      <c r="A1146" t="inlineStr">
+        <is>
+          <t>1k2az86</t>
+        </is>
+      </c>
+      <c r="B1146" t="inlineStr">
+        <is>
+          <t>Spring! 🐝🌼</t>
+        </is>
+      </c>
+      <c r="C1146" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k2az86</t>
+        </is>
+      </c>
+    </row>
+    <row r="1147">
+      <c r="A1147" t="inlineStr">
+        <is>
+          <t>1k2al0q</t>
+        </is>
+      </c>
+      <c r="B1147" t="inlineStr">
+        <is>
+          <t>Pink with gold chrome</t>
+        </is>
+      </c>
+      <c r="C1147" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c8lu6u14pmve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1148">
+      <c r="A1148" t="inlineStr">
+        <is>
+          <t>1k2ahls</t>
+        </is>
+      </c>
+      <c r="B1148" t="inlineStr">
+        <is>
+          <t>Help on cleaning up nails?</t>
+        </is>
+      </c>
+      <c r="C1148" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hd8bwhddomve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1149">
+      <c r="A1149" t="inlineStr">
+        <is>
+          <t>1k2ag6q</t>
+        </is>
+      </c>
+      <c r="B1149" t="inlineStr">
+        <is>
+          <t>I love them sm 🥺</t>
+        </is>
+      </c>
+      <c r="C1149" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k2ag6q</t>
+        </is>
+      </c>
+    </row>
+    <row r="1150">
+      <c r="A1150" t="inlineStr">
+        <is>
+          <t>1k29uhd</t>
+        </is>
+      </c>
+      <c r="B1150" t="inlineStr">
+        <is>
+          <t>Am I about to make my wallet cry?</t>
+        </is>
+      </c>
+      <c r="C1150" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k29uhd/am_i_about_to_make_my_wallet_cry/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1151">
+      <c r="A1151" t="inlineStr">
+        <is>
+          <t>1k29jqg</t>
+        </is>
+      </c>
+      <c r="B1151" t="inlineStr">
+        <is>
+          <t>i love these nails</t>
+        </is>
+      </c>
+      <c r="C1151" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/60xj19vghmve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1152">
+      <c r="A1152" t="inlineStr">
+        <is>
+          <t>1k21xnu</t>
+        </is>
+      </c>
+      <c r="B1152" t="inlineStr">
+        <is>
+          <t>Easter egg inspired</t>
+        </is>
+      </c>
+      <c r="C1152" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k21xnu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1153">
+      <c r="A1153" t="inlineStr">
+        <is>
+          <t>1k1xona</t>
+        </is>
+      </c>
+      <c r="B1153" t="inlineStr">
+        <is>
+          <t>i’m scared my nail tech did something to my nails</t>
+        </is>
+      </c>
+      <c r="C1153" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k1xona/im_scared_my_nail_tech_did_something_to_my_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1154">
+      <c r="A1154" t="inlineStr">
+        <is>
+          <t>1k1zj1i</t>
+        </is>
+      </c>
+      <c r="B1154" t="inlineStr">
+        <is>
+          <t>My Easter set- pastel sprinkles! 💅</t>
+        </is>
+      </c>
+      <c r="C1154" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k1zj1i</t>
+        </is>
+      </c>
+    </row>
+    <row r="1155">
+      <c r="A1155" t="inlineStr">
+        <is>
+          <t>1k2048t</t>
+        </is>
+      </c>
+      <c r="B1155" t="inlineStr">
+        <is>
+          <t>tips on how to make nails sturdy??</t>
+        </is>
+      </c>
+      <c r="C1155" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wt88uxei2kve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1156">
+      <c r="A1156" t="inlineStr">
+        <is>
+          <t>1k24eo9</t>
+        </is>
+      </c>
+      <c r="B1156" t="inlineStr">
+        <is>
+          <t>My nails and the inspo pic</t>
+        </is>
+      </c>
+      <c r="C1156" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k24eo9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1157">
+      <c r="A1157" t="inlineStr">
+        <is>
+          <t>1k275kn</t>
+        </is>
+      </c>
+      <c r="B1157" t="inlineStr">
+        <is>
+          <t>10 Years of Damage</t>
+        </is>
+      </c>
+      <c r="C1157" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fasvpmvizlve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1158">
+      <c r="A1158" t="inlineStr">
+        <is>
+          <t>1k29b57</t>
+        </is>
+      </c>
+      <c r="B1158" t="inlineStr">
+        <is>
+          <t>2013 called… they want their nail art back🧁🎀🤍</t>
+        </is>
+      </c>
+      <c r="C1158" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k29b57</t>
+        </is>
+      </c>
+    </row>
+    <row r="1159">
+      <c r="A1159" t="inlineStr">
+        <is>
+          <t>1k29b44</t>
+        </is>
+      </c>
+      <c r="B1159" t="inlineStr">
+        <is>
+          <t>Best At/Home Gel Polish Brand?</t>
+        </is>
+      </c>
+      <c r="C1159" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k29b44/best_athome_gel_polish_brand/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1160">
+      <c r="A1160" t="inlineStr">
+        <is>
+          <t>1k2938s</t>
+        </is>
+      </c>
+      <c r="B1160" t="inlineStr">
+        <is>
+          <t>Star Wars:May the Fourth</t>
+        </is>
+      </c>
+      <c r="C1160" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/43ld6000emve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1161">
+      <c r="A1161" t="inlineStr">
+        <is>
+          <t>1k28yhx</t>
+        </is>
+      </c>
+      <c r="B1161" t="inlineStr">
+        <is>
+          <t>Learning to make my own press ons!</t>
+        </is>
+      </c>
+      <c r="C1161" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bjwap9k0dmve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1162">
+      <c r="A1162" t="inlineStr">
+        <is>
+          <t>1k28xq0</t>
+        </is>
+      </c>
+      <c r="B1162" t="inlineStr">
+        <is>
+          <t>My first ever at-home French! For a first attempt I’m pretty happy!</t>
+        </is>
+      </c>
+      <c r="C1162" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k28xq0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1163">
+      <c r="A1163" t="inlineStr">
+        <is>
+          <t>1k28wbz</t>
+        </is>
+      </c>
+      <c r="B1163" t="inlineStr">
+        <is>
+          <t>RIP nail</t>
+        </is>
+      </c>
+      <c r="C1163" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2n73rjxjcmve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1164">
+      <c r="A1164" t="inlineStr">
+        <is>
+          <t>1k28r7v</t>
+        </is>
+      </c>
+      <c r="B1164" t="inlineStr">
+        <is>
+          <t>Kokoist wide nail brush</t>
+        </is>
+      </c>
+      <c r="C1164" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k28r7v/kokoist_wide_nail_brush/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1165">
+      <c r="A1165" t="inlineStr">
+        <is>
+          <t>1k28qqk</t>
+        </is>
+      </c>
+      <c r="B1165" t="inlineStr">
+        <is>
+          <t>Love my nail tech!</t>
+        </is>
+      </c>
+      <c r="C1165" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/i5wdo94dbmve1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1166">
+      <c r="A1166" t="inlineStr">
+        <is>
+          <t>1k28c9l</t>
+        </is>
+      </c>
+      <c r="B1166" t="inlineStr">
+        <is>
+          <t>Animal Crossing Nails!</t>
+        </is>
+      </c>
+      <c r="C1166" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/61flhxpd8mve1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1167">
+      <c r="A1167" t="inlineStr">
+        <is>
+          <t>1k27ye1</t>
+        </is>
+      </c>
+      <c r="B1167" t="inlineStr">
+        <is>
+          <t>How did my nail tech do? 🌈🤌🏻</t>
+        </is>
+      </c>
+      <c r="C1167" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k27ye1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1168">
+      <c r="A1168" t="inlineStr">
+        <is>
+          <t>1k2qwoo</t>
+        </is>
+      </c>
+      <c r="B1168" t="inlineStr">
+        <is>
+          <t>help pls</t>
+        </is>
+      </c>
+      <c r="C1168" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k2qwoo/help_pls/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1169">
+      <c r="A1169" t="inlineStr">
+        <is>
+          <t>1k2qcqa</t>
+        </is>
+      </c>
+      <c r="B1169" t="inlineStr">
+        <is>
+          <t>Has anyone tried these?</t>
+        </is>
+      </c>
+      <c r="C1169" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5rqot9n0pqve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1170">
+      <c r="A1170" t="inlineStr">
+        <is>
+          <t>1k2nvvf</t>
+        </is>
+      </c>
+      <c r="B1170" t="inlineStr">
+        <is>
+          <t>Sally Hansen Marine Scene</t>
+        </is>
+      </c>
+      <c r="C1170" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/urcmw72wvpve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1171">
+      <c r="A1171" t="inlineStr">
+        <is>
+          <t>1k2nvhf</t>
+        </is>
+      </c>
+      <c r="B1171" t="inlineStr">
+        <is>
+          <t>This is the way a pearl is supposed to be 🥓</t>
+        </is>
+      </c>
+      <c r="C1171" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tuoba1grvpve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1172">
+      <c r="A1172" t="inlineStr">
+        <is>
+          <t>1k2nunk</t>
+        </is>
+      </c>
+      <c r="B1172" t="inlineStr">
+        <is>
+          <t>Completely forgot to post these, so I figured spring is the perfect time 🌿</t>
+        </is>
+      </c>
+      <c r="C1172" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k2nunk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1173">
+      <c r="A1173" t="inlineStr">
+        <is>
+          <t>1k2kjfc</t>
+        </is>
+      </c>
+      <c r="B1173" t="inlineStr">
+        <is>
+          <t>Recommendations for Clionadh polishes</t>
+        </is>
+      </c>
+      <c r="C1173" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k2kjfc/recommendations_for_clionadh_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1174">
+      <c r="A1174" t="inlineStr">
+        <is>
+          <t>1k2jo33</t>
+        </is>
+      </c>
+      <c r="B1174" t="inlineStr">
+        <is>
+          <t>Would you consider this a dupe?</t>
+        </is>
+      </c>
+      <c r="C1174" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/83txp0gupove1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1175">
+      <c r="A1175" t="inlineStr">
+        <is>
+          <t>1k2niqe</t>
+        </is>
+      </c>
+      <c r="B1175" t="inlineStr">
+        <is>
+          <t>Three times three (bee's knees)</t>
+        </is>
+      </c>
+      <c r="C1175" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k2niqe</t>
+        </is>
+      </c>
+    </row>
+    <row r="1176">
+      <c r="A1176" t="inlineStr">
+        <is>
+          <t>1k2najv</t>
+        </is>
+      </c>
+      <c r="B1176" t="inlineStr">
+        <is>
+          <t>Mooncat’s Estimated Taxes?</t>
+        </is>
+      </c>
+      <c r="C1176" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k2najv/mooncats_estimated_taxes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1177">
+      <c r="A1177" t="inlineStr">
+        <is>
+          <t>1k2mdpd</t>
+        </is>
+      </c>
+      <c r="B1177" t="inlineStr">
+        <is>
+          <t>Where can I find this color?</t>
+        </is>
+      </c>
+      <c r="C1177" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k2mdpd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1178">
+      <c r="A1178" t="inlineStr">
+        <is>
+          <t>1k2m77p</t>
+        </is>
+      </c>
+      <c r="B1178" t="inlineStr">
+        <is>
+          <t>BKL “Get Lobstered” Dupe?</t>
+        </is>
+      </c>
+      <c r="C1178" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k2m77p/bkl_get_lobstered_dupe/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1179">
+      <c r="A1179" t="inlineStr">
+        <is>
+          <t>1k2l33v</t>
+        </is>
+      </c>
+      <c r="B1179" t="inlineStr">
+        <is>
+          <t>My first time trying KBShimmer, and wowow 🤩</t>
+        </is>
+      </c>
+      <c r="C1179" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/qz84zi6e3pve1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1180">
+      <c r="A1180" t="inlineStr">
+        <is>
+          <t>1k2kzbs</t>
+        </is>
+      </c>
+      <c r="B1180" t="inlineStr">
+        <is>
+          <t>$15 haul from fb marketplace!! Total jackpot 🎰😭</t>
+        </is>
+      </c>
+      <c r="C1180" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k2kzbs</t>
+        </is>
+      </c>
+    </row>
+    <row r="1181">
+      <c r="A1181" t="inlineStr">
+        <is>
+          <t>1k2kvar</t>
+        </is>
+      </c>
+      <c r="B1181" t="inlineStr">
+        <is>
+          <t>Lurid Lacquer</t>
+        </is>
+      </c>
+      <c r="C1181" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/htmh40ab1pve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1182">
+      <c r="A1182" t="inlineStr">
+        <is>
+          <t>1k2kuu4</t>
+        </is>
+      </c>
+      <c r="B1182" t="inlineStr">
+        <is>
+          <t>Wedding Nails</t>
+        </is>
+      </c>
+      <c r="C1182" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k2kuu4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1183">
+      <c r="A1183" t="inlineStr">
+        <is>
+          <t>1k2kt59</t>
+        </is>
+      </c>
+      <c r="B1183" t="inlineStr">
+        <is>
+          <t>ILNP - Poison (velvetized) 🌹</t>
+        </is>
+      </c>
+      <c r="C1183" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k2kt59</t>
+        </is>
+      </c>
+    </row>
+    <row r="1184">
+      <c r="A1184" t="inlineStr">
+        <is>
+          <t>1k2k7jg</t>
+        </is>
+      </c>
+      <c r="B1184" t="inlineStr">
+        <is>
+          <t>Can’t get over how sparkly this combo is in the light</t>
+        </is>
+      </c>
+      <c r="C1184" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/r9bhq3c1vove1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1185">
+      <c r="A1185" t="inlineStr">
+        <is>
+          <t>1k2jzs0</t>
+        </is>
+      </c>
+      <c r="B1185" t="inlineStr">
+        <is>
+          <t>Spring Mani!</t>
+        </is>
+      </c>
+      <c r="C1185" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zrjhnggysove1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1186">
+      <c r="A1186" t="inlineStr">
+        <is>
+          <t>1k2joac</t>
+        </is>
+      </c>
+      <c r="B1186" t="inlineStr">
+        <is>
+          <t>Looking for a rainbow set of creme polishes - what do you suggest?</t>
+        </is>
+      </c>
+      <c r="C1186" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k2joac/looking_for_a_rainbow_set_of_creme_polishes_what/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1187">
+      <c r="A1187" t="inlineStr">
+        <is>
+          <t>1k2j4oa</t>
+        </is>
+      </c>
+      <c r="B1187" t="inlineStr">
+        <is>
+          <t>Peace, Love &amp; Pineapples💖🍍</t>
+        </is>
+      </c>
+      <c r="C1187" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k2j4oa</t>
+        </is>
+      </c>
+    </row>
+    <row r="1188">
+      <c r="A1188" t="inlineStr">
+        <is>
+          <t>1k2ivyf</t>
+        </is>
+      </c>
+      <c r="B1188" t="inlineStr">
+        <is>
+          <t>First lurid order!</t>
+        </is>
+      </c>
+      <c r="C1188" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ceofx1kpiove1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1189">
+      <c r="A1189" t="inlineStr">
+        <is>
+          <t>1k2isrf</t>
+        </is>
+      </c>
+      <c r="B1189" t="inlineStr">
+        <is>
+          <t>First time using stickers and gems!</t>
+        </is>
+      </c>
+      <c r="C1189" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k2isrf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1190">
+      <c r="A1190" t="inlineStr">
+        <is>
+          <t>1k2isaf</t>
+        </is>
+      </c>
+      <c r="B1190" t="inlineStr">
+        <is>
+          <t>First lurid order, can’t wait!!!</t>
+        </is>
+      </c>
+      <c r="C1190" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pk309o5thove1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1191">
+      <c r="A1191" t="inlineStr">
+        <is>
+          <t>1k2ipc1</t>
+        </is>
+      </c>
+      <c r="B1191" t="inlineStr">
+        <is>
+          <t>OPI - I Can Never Hut Up- 2017 Spring Fiji Collection</t>
+        </is>
+      </c>
+      <c r="C1191" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k2ipc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1192">
+      <c r="A1192" t="inlineStr">
+        <is>
+          <t>1k2iidd</t>
+        </is>
+      </c>
+      <c r="B1192" t="inlineStr">
+        <is>
+          <t>First attempt at nail art for the cherry blossom festival 🌸</t>
+        </is>
+      </c>
+      <c r="C1192" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k2iidd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1193">
+      <c r="A1193" t="inlineStr">
+        <is>
+          <t>1k2ibxx</t>
+        </is>
+      </c>
+      <c r="B1193" t="inlineStr">
+        <is>
+          <t>Where are my fellow goths/emo/vampire types?</t>
+        </is>
+      </c>
+      <c r="C1193" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k2ibxx/where_are_my_fellow_gothsemovampire_types/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1194">
+      <c r="A1194" t="inlineStr">
+        <is>
+          <t>1k2i4z7</t>
+        </is>
+      </c>
+      <c r="B1194" t="inlineStr">
+        <is>
+          <t>Baby’s first thermal!!!</t>
+        </is>
+      </c>
+      <c r="C1194" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k2i4z7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1195">
+      <c r="A1195" t="inlineStr">
+        <is>
+          <t>1k2hyll</t>
+        </is>
+      </c>
+      <c r="B1195" t="inlineStr">
+        <is>
+          <t>Ever thought “Is this my signature nail color?”</t>
+        </is>
+      </c>
+      <c r="C1195" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o6fh5rnnaove1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1196">
+      <c r="A1196" t="inlineStr">
+        <is>
+          <t>1k2hr9s</t>
+        </is>
+      </c>
+      <c r="B1196" t="inlineStr">
+        <is>
+          <t>New colour drop??? Bringing the tea for teal!! 🦚</t>
+        </is>
+      </c>
+      <c r="C1196" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/boo8xt6u7ove1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1197">
+      <c r="A1197" t="inlineStr">
+        <is>
+          <t>1k2hk9w</t>
+        </is>
+      </c>
+      <c r="B1197" t="inlineStr">
+        <is>
+          <t>am i crazy for feeling like this is dark neutral ?</t>
+        </is>
+      </c>
+      <c r="C1197" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k2hk9w</t>
+        </is>
+      </c>
+    </row>
+    <row r="1198">
+      <c r="A1198" t="inlineStr">
+        <is>
+          <t>1k2hexo</t>
+        </is>
+      </c>
+      <c r="B1198" t="inlineStr">
+        <is>
+          <t>It’s that time of year</t>
+        </is>
+      </c>
+      <c r="C1198" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k2hexo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1199">
+      <c r="A1199" t="inlineStr">
+        <is>
+          <t>1k2h9sv</t>
+        </is>
+      </c>
+      <c r="B1199" t="inlineStr">
+        <is>
+          <t>Holo Taco smoothing base odor</t>
+        </is>
+      </c>
+      <c r="C1199" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k2h9sv/holo_taco_smoothing_base_odor/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1200">
+      <c r="A1200" t="inlineStr">
+        <is>
+          <t>1k2h1yo</t>
+        </is>
+      </c>
+      <c r="B1200" t="inlineStr">
+        <is>
+          <t>how do i recreate this?</t>
+        </is>
+      </c>
+      <c r="C1200" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fr5952iy2ove1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1201">
+      <c r="A1201" t="inlineStr">
+        <is>
+          <t>1k2gzos</t>
+        </is>
+      </c>
+      <c r="B1201" t="inlineStr">
+        <is>
+          <t>Help me find a nail polish</t>
+        </is>
+      </c>
+      <c r="C1201" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k2gzos</t>
+        </is>
+      </c>
+    </row>
+    <row r="1202">
+      <c r="A1202" t="inlineStr">
+        <is>
+          <t>1k2gy10</t>
+        </is>
+      </c>
+      <c r="B1202" t="inlineStr">
+        <is>
+          <t>💜💚 Easter skittle inspired by tulips 🌷</t>
+        </is>
+      </c>
+      <c r="C1202" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k2gy10</t>
+        </is>
+      </c>
+    </row>
+    <row r="1203">
+      <c r="A1203" t="inlineStr">
+        <is>
+          <t>1k2gko8</t>
+        </is>
+      </c>
+      <c r="B1203" t="inlineStr">
+        <is>
+          <t>Is this a streaky looking formula? Maybe I’m overthinking it? Maybe I’m high?</t>
+        </is>
+      </c>
+      <c r="C1203" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wtvkv632znve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1204">
+      <c r="A1204" t="inlineStr">
+        <is>
+          <t>1k2gezn</t>
+        </is>
+      </c>
+      <c r="B1204" t="inlineStr">
+        <is>
+          <t>pastel purple for spring? 💟 ✨</t>
+        </is>
+      </c>
+      <c r="C1204" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k2gezn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1205">
+      <c r="A1205" t="inlineStr">
+        <is>
+          <t>1k2ebtc</t>
+        </is>
+      </c>
+      <c r="B1205" t="inlineStr">
+        <is>
+          <t>Different types of French Tips</t>
+        </is>
+      </c>
+      <c r="C1205" t="inlineStr">
+        <is>
+          <t>https://www.tiktok.com/t/ZTjFmKhkv/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1206">
+      <c r="A1206" t="inlineStr">
+        <is>
+          <t>1k2drlu</t>
+        </is>
+      </c>
+      <c r="B1206" t="inlineStr">
+        <is>
+          <t>I always miss the Zoya sales..</t>
+        </is>
+      </c>
+      <c r="C1206" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k2drlu/i_always_miss_the_zoya_sales/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1207">
+      <c r="A1207" t="inlineStr">
+        <is>
+          <t>1k2db5r</t>
+        </is>
+      </c>
+      <c r="B1207" t="inlineStr">
+        <is>
+          <t>Pahlish- Olivine</t>
+        </is>
+      </c>
+      <c r="C1207" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k2db5r</t>
+        </is>
+      </c>
+    </row>
+    <row r="1208">
+      <c r="A1208" t="inlineStr">
+        <is>
+          <t>1k2d7al</t>
+        </is>
+      </c>
+      <c r="B1208" t="inlineStr">
+        <is>
+          <t>Getting Ready for BKL Bees Knees Lacquer sale!</t>
+        </is>
+      </c>
+      <c r="C1208" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k2d7al/getting_ready_for_bkl_bees_knees_lacquer_sale/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1209">
+      <c r="A1209" t="inlineStr">
+        <is>
+          <t>1k2d2au</t>
+        </is>
+      </c>
+      <c r="B1209" t="inlineStr">
+        <is>
+          <t>Plant Aunt💚</t>
+        </is>
+      </c>
+      <c r="C1209" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k2d2au</t>
+        </is>
+      </c>
+    </row>
+    <row r="1210">
+      <c r="A1210" t="inlineStr">
+        <is>
+          <t>1k2d120</t>
+        </is>
+      </c>
+      <c r="B1210" t="inlineStr">
+        <is>
+          <t>Mango 🥭</t>
+        </is>
+      </c>
+      <c r="C1210" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k2d120/mango/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1211">
+      <c r="A1211" t="inlineStr">
+        <is>
+          <t>1k2czlg</t>
+        </is>
+      </c>
+      <c r="B1211" t="inlineStr">
+        <is>
+          <t>BKL- I Choose the Bear 🐻</t>
+        </is>
+      </c>
+      <c r="C1211" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/nq9k3na57nve1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1212">
+      <c r="A1212" t="inlineStr">
+        <is>
+          <t>1k2cxju</t>
+        </is>
+      </c>
+      <c r="B1212" t="inlineStr">
+        <is>
+          <t>Mooncat, Tariffs, &amp; Sales</t>
+        </is>
+      </c>
+      <c r="C1212" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k2cxju/mooncat_tariffs_sales/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1213">
+      <c r="A1213" t="inlineStr">
+        <is>
+          <t>1k2cg9g</t>
+        </is>
+      </c>
+      <c r="B1213" t="inlineStr">
+        <is>
+          <t>Nail art is not my strong suit, but dammit I will give it my best shot for Easter!</t>
+        </is>
+      </c>
+      <c r="C1213" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k2cg9g</t>
+        </is>
+      </c>
+    </row>
+    <row r="1214">
+      <c r="A1214" t="inlineStr">
+        <is>
+          <t>1k2cf2s</t>
+        </is>
+      </c>
+      <c r="B1214" t="inlineStr">
+        <is>
+          <t>Recs for a non-UV base for structure.</t>
+        </is>
+      </c>
+      <c r="C1214" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k2cf2s/recs_for_a_nonuv_base_for_structure/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1215">
+      <c r="A1215" t="inlineStr">
+        <is>
+          <t>1k2bwx0</t>
+        </is>
+      </c>
+      <c r="B1215" t="inlineStr">
+        <is>
+          <t>I went yesterday to have for the first time proper manicure done and it started chipping and cracking already.</t>
+        </is>
+      </c>
+      <c r="C1215" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k2bwx0/i_went_yesterday_to_have_for_the_first_time/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1216">
+      <c r="A1216" t="inlineStr">
+        <is>
+          <t>1k2bnr5</t>
+        </is>
+      </c>
+      <c r="B1216" t="inlineStr">
+        <is>
+          <t>Speed demon top coat bubbles??</t>
+        </is>
+      </c>
+      <c r="C1216" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k2bnr5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1217">
+      <c r="A1217" t="inlineStr">
+        <is>
+          <t>1k2bf99</t>
+        </is>
+      </c>
+      <c r="B1217" t="inlineStr">
+        <is>
+          <t>Spring flowers</t>
+        </is>
+      </c>
+      <c r="C1217" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k2bf99</t>
+        </is>
+      </c>
+    </row>
+    <row r="1218">
+      <c r="A1218" t="inlineStr">
+        <is>
+          <t>1k2anvb</t>
+        </is>
+      </c>
+      <c r="B1218" t="inlineStr">
+        <is>
+          <t>It's almost Easter and these are eggs 🍳🐣</t>
+        </is>
+      </c>
+      <c r="C1218" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/45fysczopmve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1219">
+      <c r="A1219" t="inlineStr">
+        <is>
+          <t>1k2a2xo</t>
+        </is>
+      </c>
+      <c r="B1219" t="inlineStr">
+        <is>
+          <t>Say My Name 3 Times!</t>
+        </is>
+      </c>
+      <c r="C1219" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k2a2xo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1220">
+      <c r="A1220" t="inlineStr">
+        <is>
+          <t>1k2a131</t>
+        </is>
+      </c>
+      <c r="B1220" t="inlineStr">
+        <is>
+          <t>Reflective glitters make me so happy</t>
+        </is>
+      </c>
+      <c r="C1220" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k2a131</t>
+        </is>
+      </c>
+    </row>
+    <row r="1221">
+      <c r="A1221" t="inlineStr">
+        <is>
+          <t>1k2a0j3</t>
+        </is>
+      </c>
+      <c r="B1221" t="inlineStr">
+        <is>
+          <t>OPI Do You Sea What I Sea</t>
+        </is>
+      </c>
+      <c r="C1221" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mpdxjedvkmve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1222">
+      <c r="A1222" t="inlineStr">
+        <is>
+          <t>1k29y2f</t>
+        </is>
+      </c>
+      <c r="B1222" t="inlineStr">
+        <is>
+          <t>Easter egg nails</t>
+        </is>
+      </c>
+      <c r="C1222" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ly3ldymdkmve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1223">
+      <c r="A1223" t="inlineStr">
+        <is>
+          <t>1k29wa4</t>
+        </is>
+      </c>
+      <c r="B1223" t="inlineStr">
+        <is>
+          <t>Pink shimmer for this rainy day!</t>
+        </is>
+      </c>
+      <c r="C1223" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k29wa4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1224">
+      <c r="A1224" t="inlineStr">
+        <is>
+          <t>1k29qfn</t>
+        </is>
+      </c>
+      <c r="B1224" t="inlineStr">
+        <is>
+          <t>KBShimmer order was just delivered, say goodbye to my 2-day old mani</t>
+        </is>
+      </c>
+      <c r="C1224" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k29qfn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1225">
+      <c r="A1225" t="inlineStr">
+        <is>
+          <t>1k29kl8</t>
+        </is>
+      </c>
+      <c r="B1225" t="inlineStr">
+        <is>
+          <t>Bought this today for my son, can any men show off their manis please? I know he’s going to love it.</t>
+        </is>
+      </c>
+      <c r="C1225" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wpt15ecnhmve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1226">
+      <c r="A1226" t="inlineStr">
+        <is>
+          <t>1k29fua</t>
+        </is>
+      </c>
+      <c r="B1226" t="inlineStr">
+        <is>
+          <t>Anything super sparkly, similar to Mooncat’s Star Destroyer?</t>
+        </is>
+      </c>
+      <c r="C1226" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k29fua/anything_super_sparkly_similar_to_mooncats_star/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1227">
+      <c r="A1227" t="inlineStr">
+        <is>
+          <t>1k28x07</t>
+        </is>
+      </c>
+      <c r="B1227" t="inlineStr">
+        <is>
+          <t>Garden Party</t>
+        </is>
+      </c>
+      <c r="C1227" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k28x07</t>
+        </is>
+      </c>
+    </row>
+    <row r="1228">
+      <c r="A1228" t="inlineStr">
+        <is>
+          <t>1k28vd8</t>
+        </is>
+      </c>
+      <c r="B1228" t="inlineStr">
+        <is>
+          <t>I blame all of you for helping me justify this</t>
+        </is>
+      </c>
+      <c r="C1228" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k28vd8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1229">
+      <c r="A1229" t="inlineStr">
+        <is>
+          <t>1k28ss9</t>
+        </is>
+      </c>
+      <c r="B1229" t="inlineStr">
+        <is>
+          <t>Rescue Beauty Lounge ‘No More War’</t>
+        </is>
+      </c>
+      <c r="C1229" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1y7fphqsbmve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1230">
+      <c r="A1230" t="inlineStr">
+        <is>
+          <t>1k28csg</t>
+        </is>
+      </c>
+      <c r="B1230" t="inlineStr">
+        <is>
+          <t>What do you do when you have more colors you want to use than fingers?</t>
+        </is>
+      </c>
+      <c r="C1230" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k289td</t>
+        </is>
+      </c>
+    </row>
+    <row r="1231">
+      <c r="A1231" t="inlineStr">
+        <is>
+          <t>1k283a5</t>
+        </is>
+      </c>
+      <c r="B1231" t="inlineStr">
+        <is>
+          <t>Pink holo with extra holo, I'm feeling loud</t>
+        </is>
+      </c>
+      <c r="C1231" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k283a5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1232">
+      <c r="A1232" t="inlineStr">
+        <is>
+          <t>1k27on6</t>
+        </is>
+      </c>
+      <c r="B1232" t="inlineStr">
+        <is>
+          <t>Easter Nails</t>
+        </is>
+      </c>
+      <c r="C1232" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k27on6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1233">
+      <c r="A1233" t="inlineStr">
+        <is>
+          <t>1k26rsx</t>
+        </is>
+      </c>
+      <c r="B1233" t="inlineStr">
+        <is>
+          <t>🍪C is for Cookie🍪</t>
+        </is>
+      </c>
+      <c r="C1233" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k26rsx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1234">
+      <c r="A1234" t="inlineStr">
+        <is>
+          <t>1k2605l</t>
+        </is>
+      </c>
+      <c r="B1234" t="inlineStr">
+        <is>
+          <t>The high of taking a decent photo for once led me down a silly (&amp; cursed) path…</t>
+        </is>
+      </c>
+      <c r="C1234" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k2605l</t>
+        </is>
+      </c>
+    </row>
+    <row r="1235">
+      <c r="A1235" t="inlineStr">
+        <is>
+          <t>1k25ysu</t>
+        </is>
+      </c>
+      <c r="B1235" t="inlineStr">
+        <is>
+          <t>How would you make this more visually interesting?</t>
+        </is>
+      </c>
+      <c r="C1235" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ui9jkbjcqlve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1236">
+      <c r="A1236" t="inlineStr">
+        <is>
+          <t>1k25o1q</t>
+        </is>
+      </c>
+      <c r="B1236" t="inlineStr">
+        <is>
+          <t>Hand-painted Ellie (Bella Ramsey) from The Last of Us</t>
+        </is>
+      </c>
+      <c r="C1236" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/8zi18iiunlve1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1237">
+      <c r="A1237" t="inlineStr">
+        <is>
+          <t>1k25bud</t>
+        </is>
+      </c>
+      <c r="B1237" t="inlineStr">
+        <is>
+          <t>Abe &amp; Aesop</t>
+        </is>
+      </c>
+      <c r="C1237" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k25bud</t>
+        </is>
+      </c>
+    </row>
+    <row r="1238">
+      <c r="A1238" t="inlineStr">
+        <is>
+          <t>1k256ce</t>
+        </is>
+      </c>
+      <c r="B1238" t="inlineStr">
+        <is>
+          <t>Managed to fix this damage and not have to redo my nails!</t>
+        </is>
+      </c>
+      <c r="C1238" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/chhjwge1klve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1239">
+      <c r="A1239" t="inlineStr">
+        <is>
+          <t>1k2500c</t>
+        </is>
+      </c>
+      <c r="B1239" t="inlineStr">
+        <is>
+          <t>They absolutely nailed the inspiration for this one!</t>
+        </is>
+      </c>
+      <c r="C1239" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k2500c</t>
+        </is>
+      </c>
+    </row>
+    <row r="1240">
+      <c r="A1240" t="inlineStr">
+        <is>
+          <t>1k24phk</t>
+        </is>
+      </c>
+      <c r="B1240" t="inlineStr">
+        <is>
+          <t>had a cart filled with mooncat for their sale. slowly dwindled it down to 4 from 7, hit check out, then closed out after realizing they’re still $12/bottle and it’s not a great deal 🤷🏼‍♀️</t>
+        </is>
+      </c>
+      <c r="C1240" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k24phk/had_a_cart_filled_with_mooncat_for_their_sale/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1241">
+      <c r="A1241" t="inlineStr">
+        <is>
+          <t>1k24lrg</t>
+        </is>
+      </c>
+      <c r="B1241" t="inlineStr">
+        <is>
+          <t>blue &amp; glittery</t>
+        </is>
+      </c>
+      <c r="C1241" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k24lrg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1242">
+      <c r="A1242" t="inlineStr">
+        <is>
+          <t>1k24fjd</t>
+        </is>
+      </c>
+      <c r="B1242" t="inlineStr">
+        <is>
+          <t>Helping people out with the Clionadh sale - here is Palace in various lightings!</t>
+        </is>
+      </c>
+      <c r="C1242" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/zwfp59tndlve1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1243">
+      <c r="A1243" t="inlineStr">
+        <is>
+          <t>1k23smu</t>
+        </is>
+      </c>
+      <c r="B1243" t="inlineStr">
+        <is>
+          <t>first time doing press ons!</t>
+        </is>
+      </c>
+      <c r="C1243" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ufxkvz3z7lve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1244">
+      <c r="A1244" t="inlineStr">
+        <is>
+          <t>1k238m7</t>
+        </is>
+      </c>
+      <c r="B1244" t="inlineStr">
+        <is>
+          <t>Easter Eggs</t>
+        </is>
+      </c>
+      <c r="C1244" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bhmu5eio2lve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1245">
+      <c r="A1245" t="inlineStr">
+        <is>
+          <t>1k22c9m</t>
+        </is>
+      </c>
+      <c r="B1245" t="inlineStr">
+        <is>
+          <t>Happy (early) Earth Day!</t>
+        </is>
+      </c>
+      <c r="C1245" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k22c9m</t>
+        </is>
+      </c>
+    </row>
+    <row r="1246">
+      <c r="A1246" t="inlineStr">
+        <is>
+          <t>1k217ri</t>
+        </is>
+      </c>
+      <c r="B1246" t="inlineStr">
+        <is>
+          <t>When you manicure just lasts uncommonly long... (9 days in)</t>
+        </is>
+      </c>
+      <c r="C1246" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k217ri</t>
+        </is>
+      </c>
+    </row>
+    <row r="1247">
+      <c r="A1247" t="inlineStr">
+        <is>
+          <t>1k1zspy</t>
+        </is>
+      </c>
+      <c r="B1247" t="inlineStr">
+        <is>
+          <t>Suspension bases recommendations</t>
+        </is>
+      </c>
+      <c r="C1247" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k1zspy/suspension_bases_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1248">
+      <c r="A1248" t="inlineStr">
+        <is>
+          <t>1k2qh0h</t>
+        </is>
+      </c>
+      <c r="B1248" t="inlineStr">
+        <is>
+          <t>Beginner nail set ⭐️ Vegas themed 😍🎲 How’d I do??</t>
+        </is>
+      </c>
+      <c r="C1248" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k2qh0h</t>
+        </is>
+      </c>
+    </row>
+    <row r="1249">
+      <c r="A1249" t="inlineStr">
+        <is>
+          <t>1k2qfue</t>
+        </is>
+      </c>
+      <c r="B1249" t="inlineStr">
+        <is>
+          <t>Im seeing progress 🙌🏼</t>
+        </is>
+      </c>
+      <c r="C1249" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k2qfue</t>
+        </is>
+      </c>
+    </row>
+    <row r="1250">
+      <c r="A1250" t="inlineStr">
+        <is>
+          <t>1k2qftv</t>
+        </is>
+      </c>
+      <c r="B1250" t="inlineStr">
+        <is>
+          <t>Finally figured out how to do chrome without gel polish ✨</t>
+        </is>
+      </c>
+      <c r="C1250" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/364qom01qqve1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1251">
+      <c r="A1251" t="inlineStr">
+        <is>
+          <t>1k2qecj</t>
+        </is>
+      </c>
+      <c r="B1251" t="inlineStr">
+        <is>
+          <t>Finally figured out how to do chrome without gel polish ✨</t>
+        </is>
+      </c>
+      <c r="C1251" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4qr7mjvkpqve1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1252">
+      <c r="A1252" t="inlineStr">
+        <is>
+          <t>1k2jfvx</t>
+        </is>
+      </c>
+      <c r="B1252" t="inlineStr">
+        <is>
+          <t>Gel polish/structured gel</t>
+        </is>
+      </c>
+      <c r="C1252" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1k2jfvx/gel_polishstructured_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1253">
+      <c r="A1253" t="inlineStr">
+        <is>
+          <t>1k2nk75</t>
+        </is>
+      </c>
+      <c r="B1253" t="inlineStr">
+        <is>
+          <t>My handpainted SpongeBob GelX</t>
+        </is>
+      </c>
+      <c r="C1253" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k2nk75</t>
+        </is>
+      </c>
+    </row>
+    <row r="1254">
+      <c r="A1254" t="inlineStr">
+        <is>
+          <t>1k2lcm1</t>
+        </is>
+      </c>
+      <c r="B1254" t="inlineStr">
+        <is>
+          <t>Mexico vacation nails</t>
+        </is>
+      </c>
+      <c r="C1254" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k2lcm1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1255">
+      <c r="A1255" t="inlineStr">
+        <is>
+          <t>1k2kheo</t>
+        </is>
+      </c>
+      <c r="B1255" t="inlineStr">
+        <is>
+          <t>Vegas Press On Set I Made</t>
+        </is>
+      </c>
+      <c r="C1255" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rteq5lunxove1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1256">
+      <c r="A1256" t="inlineStr">
+        <is>
+          <t>1k2jtow</t>
+        </is>
+      </c>
+      <c r="B1256" t="inlineStr">
+        <is>
+          <t>Inspired</t>
+        </is>
+      </c>
+      <c r="C1256" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f4nf9mpbrove1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1257">
+      <c r="A1257" t="inlineStr">
+        <is>
+          <t>1k2iq2h</t>
+        </is>
+      </c>
+      <c r="B1257" t="inlineStr">
+        <is>
+          <t>all hand painted nail art by me</t>
+        </is>
+      </c>
+      <c r="C1257" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k2iq2h</t>
+        </is>
+      </c>
+    </row>
+    <row r="1258">
+      <c r="A1258" t="inlineStr">
+        <is>
+          <t>1k2i02r</t>
+        </is>
+      </c>
+      <c r="B1258" t="inlineStr">
+        <is>
+          <t>3D Glob Practice &amp; New Chrome</t>
+        </is>
+      </c>
+      <c r="C1258" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k2i02r</t>
+        </is>
+      </c>
+    </row>
+    <row r="1259">
+      <c r="A1259" t="inlineStr">
+        <is>
+          <t>1k2ho0k</t>
+        </is>
+      </c>
+      <c r="B1259" t="inlineStr">
+        <is>
+          <t>My 2nd set ever. I think it came out pretty good.</t>
+        </is>
+      </c>
+      <c r="C1259" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k2ho0k</t>
+        </is>
+      </c>
+    </row>
+    <row r="1260">
+      <c r="A1260" t="inlineStr">
+        <is>
+          <t>1k2f5ek</t>
+        </is>
+      </c>
+      <c r="B1260" t="inlineStr">
+        <is>
+          <t>How do I do this design?</t>
+        </is>
+      </c>
+      <c r="C1260" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oo1lurbunnve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1261">
+      <c r="A1261" t="inlineStr">
+        <is>
+          <t>1k2e7ul</t>
+        </is>
+      </c>
+      <c r="B1261" t="inlineStr">
+        <is>
+          <t>My very first attempt at an acrylic set</t>
+        </is>
+      </c>
+      <c r="C1261" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wqe1tiolgnve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1262">
+      <c r="A1262" t="inlineStr">
+        <is>
+          <t>1k2e6wj</t>
+        </is>
+      </c>
+      <c r="B1262" t="inlineStr">
+        <is>
+          <t>Spring Flower Nail Set 🌺</t>
+        </is>
+      </c>
+      <c r="C1262" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k2e6wj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1263">
+      <c r="A1263" t="inlineStr">
+        <is>
+          <t>1k2dqwm</t>
+        </is>
+      </c>
+      <c r="B1263" t="inlineStr">
+        <is>
+          <t>Saying "florals for spring? Groundbreaking" when wearing florals in spring? Groundbreaking</t>
+        </is>
+      </c>
+      <c r="C1263" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kuzjii31dnve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1264">
+      <c r="A1264" t="inlineStr">
+        <is>
+          <t>1k2dpjz</t>
+        </is>
+      </c>
+      <c r="B1264" t="inlineStr">
+        <is>
+          <t>Feeling these nails but I’m curious—what do you all think of this look?</t>
+        </is>
+      </c>
+      <c r="C1264" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k2dpjz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1265">
+      <c r="A1265" t="inlineStr">
+        <is>
+          <t>1k2cxrt</t>
+        </is>
+      </c>
+      <c r="B1265" t="inlineStr">
+        <is>
+          <t>Toro cat press-ons</t>
+        </is>
+      </c>
+      <c r="C1265" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k2cxrt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1266">
+      <c r="A1266" t="inlineStr">
+        <is>
+          <t>1k2bsth</t>
+        </is>
+      </c>
+      <c r="B1266" t="inlineStr">
+        <is>
+          <t>Cheetah Nails !!!</t>
+        </is>
+      </c>
+      <c r="C1266" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1k2bsth/cheetah_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1267">
+      <c r="A1267" t="inlineStr">
+        <is>
+          <t>1k2b7zm</t>
+        </is>
+      </c>
+      <c r="B1267" t="inlineStr">
+        <is>
+          <t>Picnic inspired nails for Spring. They're messy but I still like them. 🍒🍋</t>
+        </is>
+      </c>
+      <c r="C1267" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/24nc5edxtmve1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1268">
+      <c r="A1268" t="inlineStr">
+        <is>
+          <t>1k2b4ui</t>
+        </is>
+      </c>
+      <c r="B1268" t="inlineStr">
+        <is>
+          <t>Western Dreams</t>
+        </is>
+      </c>
+      <c r="C1268" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k2b4ui</t>
+        </is>
+      </c>
+    </row>
+    <row r="1269">
+      <c r="A1269" t="inlineStr">
+        <is>
+          <t>1k28100</t>
+        </is>
+      </c>
+      <c r="B1269" t="inlineStr">
+        <is>
+          <t>Our client requested 3D Cherries to match her cup ✨🍒Swipe ➡️ for the inspo 💅🏽</t>
+        </is>
+      </c>
+      <c r="C1269" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k28100</t>
+        </is>
+      </c>
+    </row>
+    <row r="1270">
+      <c r="A1270" t="inlineStr">
+        <is>
+          <t>1k280je</t>
+        </is>
+      </c>
+      <c r="B1270" t="inlineStr">
+        <is>
+          <t>How did my nail tech do? 🌈🤌🏻</t>
+        </is>
+      </c>
+      <c r="C1270" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k280je</t>
+        </is>
+      </c>
+    </row>
+    <row r="1271">
+      <c r="A1271" t="inlineStr">
+        <is>
+          <t>1k27vzm</t>
+        </is>
+      </c>
+      <c r="B1271" t="inlineStr">
+        <is>
+          <t>Coraline inspired 🌀</t>
+        </is>
+      </c>
+      <c r="C1271" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k27vzm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1272">
+      <c r="A1272" t="inlineStr">
+        <is>
+          <t>1k27u9s</t>
+        </is>
+      </c>
+      <c r="B1272" t="inlineStr">
+        <is>
+          <t>All the nails I’ve done this month! (So far)</t>
+        </is>
+      </c>
+      <c r="C1272" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k27u9s</t>
+        </is>
+      </c>
+    </row>
+    <row r="1273">
+      <c r="A1273" t="inlineStr">
+        <is>
+          <t>1k26t0k</t>
+        </is>
+      </c>
+      <c r="B1273" t="inlineStr">
+        <is>
+          <t>Press On Spring Sunset Frenchies</t>
+        </is>
+      </c>
+      <c r="C1273" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/0oaq02ltwlve1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1274">
+      <c r="A1274" t="inlineStr">
+        <is>
+          <t>1k25v22</t>
+        </is>
+      </c>
+      <c r="B1274" t="inlineStr">
+        <is>
+          <t>How I painted Ellie (Bella Ramsey) from The Last of Us on a nail</t>
+        </is>
+      </c>
+      <c r="C1274" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/9oco30ifplve1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1275">
+      <c r="A1275" t="inlineStr">
+        <is>
+          <t>1k20rpz</t>
+        </is>
+      </c>
+      <c r="B1275" t="inlineStr">
+        <is>
+          <t>Purple and pink cheetah print nails 💅💕</t>
+        </is>
+      </c>
+      <c r="C1275" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7te0j6xxakve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1276">
+      <c r="A1276" t="inlineStr">
+        <is>
+          <t>1k20igo</t>
+        </is>
+      </c>
+      <c r="B1276" t="inlineStr">
+        <is>
+          <t>Getting better every day!</t>
+        </is>
+      </c>
+      <c r="C1276" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6qudm4wl7kve1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sun Apr 20 08:10:12 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_04_20.xlsx
+++ b/data/collected_data/2025_04_20.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1276"/>
+  <dimension ref="A1:C1473"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -22125,6 +22125,3355 @@
         </is>
       </c>
     </row>
+    <row r="1277">
+      <c r="A1277" t="inlineStr">
+        <is>
+          <t>1k3h53j</t>
+        </is>
+      </c>
+      <c r="B1277" t="inlineStr">
+        <is>
+          <t>are those classy or looking cheap</t>
+        </is>
+      </c>
+      <c r="C1277" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d0ld2r0myxve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1278">
+      <c r="A1278" t="inlineStr">
+        <is>
+          <t>1k3h50w</t>
+        </is>
+      </c>
+      <c r="B1278" t="inlineStr">
+        <is>
+          <t>Simple Nails</t>
+        </is>
+      </c>
+      <c r="C1278" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nlh5clipyxve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1279">
+      <c r="A1279" t="inlineStr">
+        <is>
+          <t>1k3e2dt</t>
+        </is>
+      </c>
+      <c r="B1279" t="inlineStr">
+        <is>
+          <t>Should I be concerned?</t>
+        </is>
+      </c>
+      <c r="C1279" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k91de92kywve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1280">
+      <c r="A1280" t="inlineStr">
+        <is>
+          <t>1k3f5t1</t>
+        </is>
+      </c>
+      <c r="B1280" t="inlineStr">
+        <is>
+          <t>New press ons!!!</t>
+        </is>
+      </c>
+      <c r="C1280" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k3f5t1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1281">
+      <c r="A1281" t="inlineStr">
+        <is>
+          <t>1k3g5yz</t>
+        </is>
+      </c>
+      <c r="B1281" t="inlineStr">
+        <is>
+          <t>did cat eye polish for the first time and i’m obsessed</t>
+        </is>
+      </c>
+      <c r="C1281" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/uv0jop8qmxve1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1282">
+      <c r="A1282" t="inlineStr">
+        <is>
+          <t>1k3fo2f</t>
+        </is>
+      </c>
+      <c r="B1282" t="inlineStr">
+        <is>
+          <t>have yall ever forgot to put base coat on a full set you worked on for hours?</t>
+        </is>
+      </c>
+      <c r="C1282" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k3fo2f/have_yall_ever_forgot_to_put_base_coat_on_a_full/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1283">
+      <c r="A1283" t="inlineStr">
+        <is>
+          <t>1k3fjba</t>
+        </is>
+      </c>
+      <c r="B1283" t="inlineStr">
+        <is>
+          <t>im inlove!!</t>
+        </is>
+      </c>
+      <c r="C1283" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e0p6d1y9fxve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1284">
+      <c r="A1284" t="inlineStr">
+        <is>
+          <t>1k3fegj</t>
+        </is>
+      </c>
+      <c r="B1284" t="inlineStr">
+        <is>
+          <t>Loving my Hello Kitty Dolphine Nails</t>
+        </is>
+      </c>
+      <c r="C1284" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k3fegj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1285">
+      <c r="A1285" t="inlineStr">
+        <is>
+          <t>1k3fdgq</t>
+        </is>
+      </c>
+      <c r="B1285" t="inlineStr">
+        <is>
+          <t>Easter Egg Nails</t>
+        </is>
+      </c>
+      <c r="C1285" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8oi1sjgddxve1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1286">
+      <c r="A1286" t="inlineStr">
+        <is>
+          <t>1k3esqm</t>
+        </is>
+      </c>
+      <c r="B1286" t="inlineStr">
+        <is>
+          <t>Spring is here :)</t>
+        </is>
+      </c>
+      <c r="C1286" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gfzaytrn6xve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1287">
+      <c r="A1287" t="inlineStr">
+        <is>
+          <t>1k3ep0k</t>
+        </is>
+      </c>
+      <c r="B1287" t="inlineStr">
+        <is>
+          <t>Feeling springy! My most recent gel attempts</t>
+        </is>
+      </c>
+      <c r="C1287" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k3ep0k</t>
+        </is>
+      </c>
+    </row>
+    <row r="1288">
+      <c r="A1288" t="inlineStr">
+        <is>
+          <t>1k3elpd</t>
+        </is>
+      </c>
+      <c r="B1288" t="inlineStr">
+        <is>
+          <t>Trying *really* hard to grow my natural nails</t>
+        </is>
+      </c>
+      <c r="C1288" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q8jph2xe4xve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1289">
+      <c r="A1289" t="inlineStr">
+        <is>
+          <t>1k3e30a</t>
+        </is>
+      </c>
+      <c r="B1289" t="inlineStr">
+        <is>
+          <t>Some of my recent sets, all done by me.</t>
+        </is>
+      </c>
+      <c r="C1289" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k3e30a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1290">
+      <c r="A1290" t="inlineStr">
+        <is>
+          <t>1k3dzbs</t>
+        </is>
+      </c>
+      <c r="B1290" t="inlineStr">
+        <is>
+          <t>new nailss!!! &lt;3</t>
+        </is>
+      </c>
+      <c r="C1290" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k3dzbs</t>
+        </is>
+      </c>
+    </row>
+    <row r="1291">
+      <c r="A1291" t="inlineStr">
+        <is>
+          <t>1k3dx8o</t>
+        </is>
+      </c>
+      <c r="B1291" t="inlineStr">
+        <is>
+          <t>Hard Gel Overlay</t>
+        </is>
+      </c>
+      <c r="C1291" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k3dx8o</t>
+        </is>
+      </c>
+    </row>
+    <row r="1292">
+      <c r="A1292" t="inlineStr">
+        <is>
+          <t>1k3dwy7</t>
+        </is>
+      </c>
+      <c r="B1292" t="inlineStr">
+        <is>
+          <t>My favorite nail set of all time</t>
+        </is>
+      </c>
+      <c r="C1292" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aluxa9exwwve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1293">
+      <c r="A1293" t="inlineStr">
+        <is>
+          <t>1k39npc</t>
+        </is>
+      </c>
+      <c r="B1293" t="inlineStr">
+        <is>
+          <t>update gel allergy</t>
+        </is>
+      </c>
+      <c r="C1293" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vy6vcz9ppvve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1294">
+      <c r="A1294" t="inlineStr">
+        <is>
+          <t>1k3cm86</t>
+        </is>
+      </c>
+      <c r="B1294" t="inlineStr">
+        <is>
+          <t>Clown nails</t>
+        </is>
+      </c>
+      <c r="C1294" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k3cm86</t>
+        </is>
+      </c>
+    </row>
+    <row r="1295">
+      <c r="A1295" t="inlineStr">
+        <is>
+          <t>1k3cybr</t>
+        </is>
+      </c>
+      <c r="B1295" t="inlineStr">
+        <is>
+          <t>Just in time for Easter/Spring</t>
+        </is>
+      </c>
+      <c r="C1295" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/655jbsynmwve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1296">
+      <c r="A1296" t="inlineStr">
+        <is>
+          <t>1k3cr56</t>
+        </is>
+      </c>
+      <c r="B1296" t="inlineStr">
+        <is>
+          <t>New nail gal, I think she killed it!</t>
+        </is>
+      </c>
+      <c r="C1296" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8hl7ds7hkwve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1297">
+      <c r="A1297" t="inlineStr">
+        <is>
+          <t>1k3cgb1</t>
+        </is>
+      </c>
+      <c r="B1297" t="inlineStr">
+        <is>
+          <t>Influencer Nails</t>
+        </is>
+      </c>
+      <c r="C1297" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k3cgb1/influencer_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1298">
+      <c r="A1298" t="inlineStr">
+        <is>
+          <t>1k3by2m</t>
+        </is>
+      </c>
+      <c r="B1298" t="inlineStr">
+        <is>
+          <t>handpainted suns on some shorties ☀️</t>
+        </is>
+      </c>
+      <c r="C1298" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pz93hq52cwve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1299">
+      <c r="A1299" t="inlineStr">
+        <is>
+          <t>1k3btmy</t>
+        </is>
+      </c>
+      <c r="B1299" t="inlineStr">
+        <is>
+          <t>Is this grown out enough for a fill?</t>
+        </is>
+      </c>
+      <c r="C1299" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/myvt0u2sawve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1300">
+      <c r="A1300" t="inlineStr">
+        <is>
+          <t>1k3bg4s</t>
+        </is>
+      </c>
+      <c r="B1300" t="inlineStr">
+        <is>
+          <t>Nude pink 💗</t>
+        </is>
+      </c>
+      <c r="C1300" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k3bg4s</t>
+        </is>
+      </c>
+    </row>
+    <row r="1301">
+      <c r="A1301" t="inlineStr">
+        <is>
+          <t>1k3bfh7</t>
+        </is>
+      </c>
+      <c r="B1301" t="inlineStr">
+        <is>
+          <t>Strawberry nails</t>
+        </is>
+      </c>
+      <c r="C1301" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2h0arbbr6wve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1302">
+      <c r="A1302" t="inlineStr">
+        <is>
+          <t>1k3aygt</t>
+        </is>
+      </c>
+      <c r="B1302" t="inlineStr">
+        <is>
+          <t>I did my first vendor event!</t>
+        </is>
+      </c>
+      <c r="C1302" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k3aygt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1303">
+      <c r="A1303" t="inlineStr">
+        <is>
+          <t>1k3apt2</t>
+        </is>
+      </c>
+      <c r="B1303" t="inlineStr">
+        <is>
+          <t>Nails</t>
+        </is>
+      </c>
+      <c r="C1303" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3sahre4tzvve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1304">
+      <c r="A1304" t="inlineStr">
+        <is>
+          <t>1k3aphf</t>
+        </is>
+      </c>
+      <c r="B1304" t="inlineStr">
+        <is>
+          <t>baby pink nails ready for Easter and my niece's bday</t>
+        </is>
+      </c>
+      <c r="C1304" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k3aphf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1305">
+      <c r="A1305" t="inlineStr">
+        <is>
+          <t>1k3aiga</t>
+        </is>
+      </c>
+      <c r="B1305" t="inlineStr">
+        <is>
+          <t>Bees n honey 🥰</t>
+        </is>
+      </c>
+      <c r="C1305" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/2cmqromtxvve1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1306">
+      <c r="A1306" t="inlineStr">
+        <is>
+          <t>1k3a0ot</t>
+        </is>
+      </c>
+      <c r="B1306" t="inlineStr">
+        <is>
+          <t>Is it possible to color switch on Gel X at home without an efile?</t>
+        </is>
+      </c>
+      <c r="C1306" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k3a0ot/is_it_possible_to_color_switch_on_gel_x_at_home/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1307">
+      <c r="A1307" t="inlineStr">
+        <is>
+          <t>1k39kr6</t>
+        </is>
+      </c>
+      <c r="B1307" t="inlineStr">
+        <is>
+          <t>I was going for rain drop vibes, it’s giving mermaid instead but I’m here for it</t>
+        </is>
+      </c>
+      <c r="C1307" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6buy2lyxovve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1308">
+      <c r="A1308" t="inlineStr">
+        <is>
+          <t>1k38su5</t>
+        </is>
+      </c>
+      <c r="B1308" t="inlineStr">
+        <is>
+          <t>First few nail sets</t>
+        </is>
+      </c>
+      <c r="C1308" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k38su5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1309">
+      <c r="A1309" t="inlineStr">
+        <is>
+          <t>1k3953m</t>
+        </is>
+      </c>
+      <c r="B1309" t="inlineStr">
+        <is>
+          <t>Mini Egg nails for Easter!</t>
+        </is>
+      </c>
+      <c r="C1309" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j7g5fvbzkvve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1310">
+      <c r="A1310" t="inlineStr">
+        <is>
+          <t>1k394b6</t>
+        </is>
+      </c>
+      <c r="B1310" t="inlineStr">
+        <is>
+          <t>Love a little witchy moment on my nails. All handpainted by my tech (Naturally Nails in Clayton, BC)</t>
+        </is>
+      </c>
+      <c r="C1310" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a640pbknkvve1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1311">
+      <c r="A1311" t="inlineStr">
+        <is>
+          <t>1k3907j</t>
+        </is>
+      </c>
+      <c r="B1311" t="inlineStr">
+        <is>
+          <t>Nails!</t>
+        </is>
+      </c>
+      <c r="C1311" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3flpmcbsjvve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1312">
+      <c r="A1312" t="inlineStr">
+        <is>
+          <t>1k38r8r</t>
+        </is>
+      </c>
+      <c r="B1312" t="inlineStr">
+        <is>
+          <t>Gel X Press-Ons or Acrylics?</t>
+        </is>
+      </c>
+      <c r="C1312" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k38r8r/gel_x_pressons_or_acrylics/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1313">
+      <c r="A1313" t="inlineStr">
+        <is>
+          <t>1k38npq</t>
+        </is>
+      </c>
+      <c r="B1313" t="inlineStr">
+        <is>
+          <t>I accidentally used a matte top coat instead of regular glossy. These were supposed to have a jelly more translucent look to them. Can I apply the regular top coat to bring back some gloss at least?</t>
+        </is>
+      </c>
+      <c r="C1313" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c4df7dxpgvve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1314">
+      <c r="A1314" t="inlineStr">
+        <is>
+          <t>1k38l04</t>
+        </is>
+      </c>
+      <c r="B1314" t="inlineStr">
+        <is>
+          <t>A doozy of a 24 hours</t>
+        </is>
+      </c>
+      <c r="C1314" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k38l04</t>
+        </is>
+      </c>
+    </row>
+    <row r="1315">
+      <c r="A1315" t="inlineStr">
+        <is>
+          <t>1k38d2t</t>
+        </is>
+      </c>
+      <c r="B1315" t="inlineStr">
+        <is>
+          <t>I like long nails better, but they still look pretty.</t>
+        </is>
+      </c>
+      <c r="C1315" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sehyicr1evve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1316">
+      <c r="A1316" t="inlineStr">
+        <is>
+          <t>1k38aqa</t>
+        </is>
+      </c>
+      <c r="B1316" t="inlineStr">
+        <is>
+          <t>My most popular nail design to date.</t>
+        </is>
+      </c>
+      <c r="C1316" t="inlineStr">
+        <is>
+          <t>https://v.lemon8-app.com/al/OgZembcpkp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1317">
+      <c r="A1317" t="inlineStr">
+        <is>
+          <t>1k38332</t>
+        </is>
+      </c>
+      <c r="B1317" t="inlineStr">
+        <is>
+          <t>French at home natural nails</t>
+        </is>
+      </c>
+      <c r="C1317" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k38332/french_at_home_natural_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1318">
+      <c r="A1318" t="inlineStr">
+        <is>
+          <t>1k380fv</t>
+        </is>
+      </c>
+      <c r="B1318" t="inlineStr">
+        <is>
+          <t>Happy Easter! 🩷✨</t>
+        </is>
+      </c>
+      <c r="C1318" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hnmde1tyavve1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1319">
+      <c r="A1319" t="inlineStr">
+        <is>
+          <t>1k37x9x</t>
+        </is>
+      </c>
+      <c r="B1319" t="inlineStr">
+        <is>
+          <t>Nail file for oily, hard-to-file nails?</t>
+        </is>
+      </c>
+      <c r="C1319" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k37x9x/nail_file_for_oily_hardtofile_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1320">
+      <c r="A1320" t="inlineStr">
+        <is>
+          <t>1k360uh</t>
+        </is>
+      </c>
+      <c r="B1320" t="inlineStr">
+        <is>
+          <t>Blue and gold</t>
+        </is>
+      </c>
+      <c r="C1320" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k360uh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1321">
+      <c r="A1321" t="inlineStr">
+        <is>
+          <t>1k37lct</t>
+        </is>
+      </c>
+      <c r="B1321" t="inlineStr">
+        <is>
+          <t>French Nails</t>
+        </is>
+      </c>
+      <c r="C1321" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vljoy9u87vve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1322">
+      <c r="A1322" t="inlineStr">
+        <is>
+          <t>1k37k5o</t>
+        </is>
+      </c>
+      <c r="B1322" t="inlineStr">
+        <is>
+          <t>Can’t go wrong with purple nails ✨</t>
+        </is>
+      </c>
+      <c r="C1322" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/plrta5dy6vve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1323">
+      <c r="A1323" t="inlineStr">
+        <is>
+          <t>1k378ko</t>
+        </is>
+      </c>
+      <c r="B1323" t="inlineStr">
+        <is>
+          <t>vacation nails:)</t>
+        </is>
+      </c>
+      <c r="C1323" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tioxhga74vve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1324">
+      <c r="A1324" t="inlineStr">
+        <is>
+          <t>1k372xg</t>
+        </is>
+      </c>
+      <c r="B1324" t="inlineStr">
+        <is>
+          <t>There’s just something about matte and neon colours that gets me every time 🤤💅</t>
+        </is>
+      </c>
+      <c r="C1324" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dvxm8ygu2vve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1325">
+      <c r="A1325" t="inlineStr">
+        <is>
+          <t>1k371kx</t>
+        </is>
+      </c>
+      <c r="B1325" t="inlineStr">
+        <is>
+          <t>What do we think of this color? ( thanks to my senior cat for acting as a backdrop)</t>
+        </is>
+      </c>
+      <c r="C1325" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/khknnn9j2vve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1326">
+      <c r="A1326" t="inlineStr">
+        <is>
+          <t>1k36i8m</t>
+        </is>
+      </c>
+      <c r="B1326" t="inlineStr">
+        <is>
+          <t>first time getting my nails done✨</t>
+        </is>
+      </c>
+      <c r="C1326" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6071wayyxuve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1327">
+      <c r="A1327" t="inlineStr">
+        <is>
+          <t>1k3680h</t>
+        </is>
+      </c>
+      <c r="B1327" t="inlineStr">
+        <is>
+          <t>What’s your favorite sheer nail polish?</t>
+        </is>
+      </c>
+      <c r="C1327" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k3680h/whats_your_favorite_sheer_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1328">
+      <c r="A1328" t="inlineStr">
+        <is>
+          <t>1k366bv</t>
+        </is>
+      </c>
+      <c r="B1328" t="inlineStr">
+        <is>
+          <t>🍯 🐝</t>
+        </is>
+      </c>
+      <c r="C1328" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0c6lggg7vuve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1329">
+      <c r="A1329" t="inlineStr">
+        <is>
+          <t>1k35wlh</t>
+        </is>
+      </c>
+      <c r="B1329" t="inlineStr">
+        <is>
+          <t>Eat your fruit</t>
+        </is>
+      </c>
+      <c r="C1329" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k35wlh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1330">
+      <c r="A1330" t="inlineStr">
+        <is>
+          <t>1k35umn</t>
+        </is>
+      </c>
+      <c r="B1330" t="inlineStr">
+        <is>
+          <t>simple pink with accent nails for spring 💖</t>
+        </is>
+      </c>
+      <c r="C1330" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k35umn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1331">
+      <c r="A1331" t="inlineStr">
+        <is>
+          <t>1k35u2h</t>
+        </is>
+      </c>
+      <c r="B1331" t="inlineStr">
+        <is>
+          <t>I regret the colour combination</t>
+        </is>
+      </c>
+      <c r="C1331" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k35u2h</t>
+        </is>
+      </c>
+    </row>
+    <row r="1332">
+      <c r="A1332" t="inlineStr">
+        <is>
+          <t>1k35t78</t>
+        </is>
+      </c>
+      <c r="B1332" t="inlineStr">
+        <is>
+          <t>Investing in DND gel</t>
+        </is>
+      </c>
+      <c r="C1332" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k35t78/investing_in_dnd_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1333">
+      <c r="A1333" t="inlineStr">
+        <is>
+          <t>1k35hj0</t>
+        </is>
+      </c>
+      <c r="B1333" t="inlineStr">
+        <is>
+          <t>Got my nails did</t>
+        </is>
+      </c>
+      <c r="C1333" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/085dltkgpuve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1334">
+      <c r="A1334" t="inlineStr">
+        <is>
+          <t>1k35egt</t>
+        </is>
+      </c>
+      <c r="B1334" t="inlineStr">
+        <is>
+          <t>Nail shape question</t>
+        </is>
+      </c>
+      <c r="C1334" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ophvx9jrouve1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1335">
+      <c r="A1335" t="inlineStr">
+        <is>
+          <t>1k35dki</t>
+        </is>
+      </c>
+      <c r="B1335" t="inlineStr">
+        <is>
+          <t>Tips?</t>
+        </is>
+      </c>
+      <c r="C1335" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k35dki</t>
+        </is>
+      </c>
+    </row>
+    <row r="1336">
+      <c r="A1336" t="inlineStr">
+        <is>
+          <t>1k35c93</t>
+        </is>
+      </c>
+      <c r="B1336" t="inlineStr">
+        <is>
+          <t>new spot what do we think?</t>
+        </is>
+      </c>
+      <c r="C1336" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2arq80z8ouve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1337">
+      <c r="A1337" t="inlineStr">
+        <is>
+          <t>1k355hz</t>
+        </is>
+      </c>
+      <c r="B1337" t="inlineStr">
+        <is>
+          <t>Shall I make these more almond?</t>
+        </is>
+      </c>
+      <c r="C1337" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4ba2o65pmuve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1338">
+      <c r="A1338" t="inlineStr">
+        <is>
+          <t>1k34v7j</t>
+        </is>
+      </c>
+      <c r="B1338" t="inlineStr">
+        <is>
+          <t>Do you like this manicure I got?</t>
+        </is>
+      </c>
+      <c r="C1338" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wlnjwhxdkuve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1339">
+      <c r="A1339" t="inlineStr">
+        <is>
+          <t>1k34ujj</t>
+        </is>
+      </c>
+      <c r="B1339" t="inlineStr">
+        <is>
+          <t>I use some colors that reminded me of Easter.</t>
+        </is>
+      </c>
+      <c r="C1339" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k34ujj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1340">
+      <c r="A1340" t="inlineStr">
+        <is>
+          <t>1k33xsz</t>
+        </is>
+      </c>
+      <c r="B1340" t="inlineStr">
+        <is>
+          <t>nail detached and fell off</t>
+        </is>
+      </c>
+      <c r="C1340" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lz59p4vrcuve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1341">
+      <c r="A1341" t="inlineStr">
+        <is>
+          <t>1k33l9l</t>
+        </is>
+      </c>
+      <c r="B1341" t="inlineStr">
+        <is>
+          <t>Does anyone know the tool she uses? Pic from Insta creator karenbella.unhas</t>
+        </is>
+      </c>
+      <c r="C1341" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9sp49tw1auve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1342">
+      <c r="A1342" t="inlineStr">
+        <is>
+          <t>1k342r6</t>
+        </is>
+      </c>
+      <c r="B1342" t="inlineStr">
+        <is>
+          <t>🦋</t>
+        </is>
+      </c>
+      <c r="C1342" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xrckqp6wduve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1343">
+      <c r="A1343" t="inlineStr">
+        <is>
+          <t>1k33jts</t>
+        </is>
+      </c>
+      <c r="B1343" t="inlineStr">
+        <is>
+          <t>Probando algo diferente</t>
+        </is>
+      </c>
+      <c r="C1343" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1gqzqb1q9uve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1344">
+      <c r="A1344" t="inlineStr">
+        <is>
+          <t>1k32vq3</t>
+        </is>
+      </c>
+      <c r="B1344" t="inlineStr">
+        <is>
+          <t>I want to DIY cat eye as a novice. Should I purchase things accordingly or will it be averagish?</t>
+        </is>
+      </c>
+      <c r="C1344" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k32vq3/i_want_to_diy_cat_eye_as_a_novice_should_i/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1345">
+      <c r="A1345" t="inlineStr">
+        <is>
+          <t>1k32sqq</t>
+        </is>
+      </c>
+      <c r="B1345" t="inlineStr">
+        <is>
+          <t>studio ghibli nails</t>
+        </is>
+      </c>
+      <c r="C1345" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/64zh3wtm3uve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1346">
+      <c r="A1346" t="inlineStr">
+        <is>
+          <t>1k33hpo</t>
+        </is>
+      </c>
+      <c r="B1346" t="inlineStr">
+        <is>
+          <t>What do we think??</t>
+        </is>
+      </c>
+      <c r="C1346" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k33hpo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1347">
+      <c r="A1347" t="inlineStr">
+        <is>
+          <t>1k33fge</t>
+        </is>
+      </c>
+      <c r="B1347" t="inlineStr">
+        <is>
+          <t>How did she do</t>
+        </is>
+      </c>
+      <c r="C1347" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k33fge</t>
+        </is>
+      </c>
+    </row>
+    <row r="1348">
+      <c r="A1348" t="inlineStr">
+        <is>
+          <t>1k33ase</t>
+        </is>
+      </c>
+      <c r="B1348" t="inlineStr">
+        <is>
+          <t>Red for spring🥀</t>
+        </is>
+      </c>
+      <c r="C1348" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5urchhxn7uve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1349">
+      <c r="A1349" t="inlineStr">
+        <is>
+          <t>1k338qd</t>
+        </is>
+      </c>
+      <c r="B1349" t="inlineStr">
+        <is>
+          <t>Sea Glass with Cat Eye</t>
+        </is>
+      </c>
+      <c r="C1349" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g25fvhy67uve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1350">
+      <c r="A1350" t="inlineStr">
+        <is>
+          <t>1k330ve</t>
+        </is>
+      </c>
+      <c r="B1350" t="inlineStr">
+        <is>
+          <t>4:20 Nails 💚</t>
+        </is>
+      </c>
+      <c r="C1350" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k330ve</t>
+        </is>
+      </c>
+    </row>
+    <row r="1351">
+      <c r="A1351" t="inlineStr">
+        <is>
+          <t>1k32rod</t>
+        </is>
+      </c>
+      <c r="B1351" t="inlineStr">
+        <is>
+          <t>dreamy nails🫧</t>
+        </is>
+      </c>
+      <c r="C1351" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k32rod</t>
+        </is>
+      </c>
+    </row>
+    <row r="1352">
+      <c r="A1352" t="inlineStr">
+        <is>
+          <t>1k32e9i</t>
+        </is>
+      </c>
+      <c r="B1352" t="inlineStr">
+        <is>
+          <t>Owwwww</t>
+        </is>
+      </c>
+      <c r="C1352" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uwxdrkgh0uve1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1353">
+      <c r="A1353" t="inlineStr">
+        <is>
+          <t>1k328bc</t>
+        </is>
+      </c>
+      <c r="B1353" t="inlineStr">
+        <is>
+          <t>Finally Got Them Done</t>
+        </is>
+      </c>
+      <c r="C1353" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k328bc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1354">
+      <c r="A1354" t="inlineStr">
+        <is>
+          <t>1k31yyg</t>
+        </is>
+      </c>
+      <c r="B1354" t="inlineStr">
+        <is>
+          <t>Interview nails</t>
+        </is>
+      </c>
+      <c r="C1354" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hmj3g605xtve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1355">
+      <c r="A1355" t="inlineStr">
+        <is>
+          <t>1k31vrw</t>
+        </is>
+      </c>
+      <c r="B1355" t="inlineStr">
+        <is>
+          <t>Help; nail chipped and I’m not sure what to do</t>
+        </is>
+      </c>
+      <c r="C1355" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/poqc8rkfwtve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1356">
+      <c r="A1356" t="inlineStr">
+        <is>
+          <t>1k31v73</t>
+        </is>
+      </c>
+      <c r="B1356" t="inlineStr">
+        <is>
+          <t>another *better* picture of my natural nails! :)</t>
+        </is>
+      </c>
+      <c r="C1356" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1nonga7bwtve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1357">
+      <c r="A1357" t="inlineStr">
+        <is>
+          <t>1k31thm</t>
+        </is>
+      </c>
+      <c r="B1357" t="inlineStr">
+        <is>
+          <t>Cat eye beginner</t>
+        </is>
+      </c>
+      <c r="C1357" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k31thm/cat_eye_beginner/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1358">
+      <c r="A1358" t="inlineStr">
+        <is>
+          <t>1k31sw0</t>
+        </is>
+      </c>
+      <c r="B1358" t="inlineStr">
+        <is>
+          <t>1000% natural long nails</t>
+        </is>
+      </c>
+      <c r="C1358" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0jdamussvtve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1359">
+      <c r="A1359" t="inlineStr">
+        <is>
+          <t>1k31h56</t>
+        </is>
+      </c>
+      <c r="B1359" t="inlineStr">
+        <is>
+          <t>My nail tech ate with these</t>
+        </is>
+      </c>
+      <c r="C1359" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fmaqlrs5ttve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1360">
+      <c r="A1360" t="inlineStr">
+        <is>
+          <t>1k31dcj</t>
+        </is>
+      </c>
+      <c r="B1360" t="inlineStr">
+        <is>
+          <t>Everyday is Valentines Day when you’re a lover girl 💕</t>
+        </is>
+      </c>
+      <c r="C1360" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vy6axf7dstve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1361">
+      <c r="A1361" t="inlineStr">
+        <is>
+          <t>1k317gm</t>
+        </is>
+      </c>
+      <c r="B1361" t="inlineStr">
+        <is>
+          <t>Something subtle</t>
+        </is>
+      </c>
+      <c r="C1361" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aywxpfn3rtve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1362">
+      <c r="A1362" t="inlineStr">
+        <is>
+          <t>1k30fgv</t>
+        </is>
+      </c>
+      <c r="B1362" t="inlineStr">
+        <is>
+          <t>Can someone help me with nails for a vacation for flat beds?</t>
+        </is>
+      </c>
+      <c r="C1362" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k30fgv/can_someone_help_me_with_nails_for_a_vacation_for/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1363">
+      <c r="A1363" t="inlineStr">
+        <is>
+          <t>1k313xw</t>
+        </is>
+      </c>
+      <c r="B1363" t="inlineStr">
+        <is>
+          <t>Cadillacquer - In Disguise</t>
+        </is>
+      </c>
+      <c r="C1363" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k313xw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1364">
+      <c r="A1364" t="inlineStr">
+        <is>
+          <t>1k30rzv</t>
+        </is>
+      </c>
+      <c r="B1364" t="inlineStr">
+        <is>
+          <t>Just sharing my nails</t>
+        </is>
+      </c>
+      <c r="C1364" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/guufjopsntve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1365">
+      <c r="A1365" t="inlineStr">
+        <is>
+          <t>1k30qwd</t>
+        </is>
+      </c>
+      <c r="B1365" t="inlineStr">
+        <is>
+          <t>French❤️</t>
+        </is>
+      </c>
+      <c r="C1365" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g75hg6vjntve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1366">
+      <c r="A1366" t="inlineStr">
+        <is>
+          <t>1k30hbl</t>
+        </is>
+      </c>
+      <c r="B1366" t="inlineStr">
+        <is>
+          <t>Diva tipz</t>
+        </is>
+      </c>
+      <c r="C1366" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k30hbl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1367">
+      <c r="A1367" t="inlineStr">
+        <is>
+          <t>1k30fwr</t>
+        </is>
+      </c>
+      <c r="B1367" t="inlineStr">
+        <is>
+          <t>Nails for 2 weeks in Europe</t>
+        </is>
+      </c>
+      <c r="C1367" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1k30fwr/nails_for_2_weeks_in_europe/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1368">
+      <c r="A1368" t="inlineStr">
+        <is>
+          <t>1k30f5p</t>
+        </is>
+      </c>
+      <c r="B1368" t="inlineStr">
+        <is>
+          <t>What do you think of my new set?!</t>
+        </is>
+      </c>
+      <c r="C1368" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/3h8bbusvktve1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1369">
+      <c r="A1369" t="inlineStr">
+        <is>
+          <t>1k30a0o</t>
+        </is>
+      </c>
+      <c r="B1369" t="inlineStr">
+        <is>
+          <t>Freestyle</t>
+        </is>
+      </c>
+      <c r="C1369" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k30a0o</t>
+        </is>
+      </c>
+    </row>
+    <row r="1370">
+      <c r="A1370" t="inlineStr">
+        <is>
+          <t>1k2zwju</t>
+        </is>
+      </c>
+      <c r="B1370" t="inlineStr">
+        <is>
+          <t>I love my nail tech</t>
+        </is>
+      </c>
+      <c r="C1370" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bg2qb1orgtve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1371">
+      <c r="A1371" t="inlineStr">
+        <is>
+          <t>1k2zoi2</t>
+        </is>
+      </c>
+      <c r="B1371" t="inlineStr">
+        <is>
+          <t>My first French design</t>
+        </is>
+      </c>
+      <c r="C1371" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w0fcldqzetve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1372">
+      <c r="A1372" t="inlineStr">
+        <is>
+          <t>1k2zmzi</t>
+        </is>
+      </c>
+      <c r="B1372" t="inlineStr">
+        <is>
+          <t>🖤First ombre attempt💚</t>
+        </is>
+      </c>
+      <c r="C1372" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k2zmzi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1373">
+      <c r="A1373" t="inlineStr">
+        <is>
+          <t>1k2zhnp</t>
+        </is>
+      </c>
+      <c r="B1373" t="inlineStr">
+        <is>
+          <t>Favorite sets so far this year!</t>
+        </is>
+      </c>
+      <c r="C1373" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k2zhnp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1374">
+      <c r="A1374" t="inlineStr">
+        <is>
+          <t>1k2zfjk</t>
+        </is>
+      </c>
+      <c r="B1374" t="inlineStr">
+        <is>
+          <t>Natural nails with clear hard gel looking stripey</t>
+        </is>
+      </c>
+      <c r="C1374" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k2zfjk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1375">
+      <c r="A1375" t="inlineStr">
+        <is>
+          <t>1k2ywcr</t>
+        </is>
+      </c>
+      <c r="B1375" t="inlineStr">
+        <is>
+          <t>New week, new nails.. ! I love them!</t>
+        </is>
+      </c>
+      <c r="C1375" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t13w5hau8tve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1376">
+      <c r="A1376" t="inlineStr">
+        <is>
+          <t>1k2yiga</t>
+        </is>
+      </c>
+      <c r="B1376" t="inlineStr">
+        <is>
+          <t>Cruise nails I did</t>
+        </is>
+      </c>
+      <c r="C1376" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k2yiga</t>
+        </is>
+      </c>
+    </row>
+    <row r="1377">
+      <c r="A1377" t="inlineStr">
+        <is>
+          <t>1k3dowr</t>
+        </is>
+      </c>
+      <c r="B1377" t="inlineStr">
+        <is>
+          <t>Glowy Shimmer</t>
+        </is>
+      </c>
+      <c r="C1377" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k3dowr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1378">
+      <c r="A1378" t="inlineStr">
+        <is>
+          <t>1k3d2f8</t>
+        </is>
+      </c>
+      <c r="B1378" t="inlineStr">
+        <is>
+          <t>Affordable dupe for Dazzle Dry in Stardust/Cupids Bow?</t>
+        </is>
+      </c>
+      <c r="C1378" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k3d2f8/affordable_dupe_for_dazzle_dry_in_stardustcupids/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1379">
+      <c r="A1379" t="inlineStr">
+        <is>
+          <t>1k3crpg</t>
+        </is>
+      </c>
+      <c r="B1379" t="inlineStr">
+        <is>
+          <t>Do you swatch your destash pile over black?</t>
+        </is>
+      </c>
+      <c r="C1379" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v4mwqfgnkwve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1380">
+      <c r="A1380" t="inlineStr">
+        <is>
+          <t>1k3cew4</t>
+        </is>
+      </c>
+      <c r="B1380" t="inlineStr">
+        <is>
+          <t>Lottie London GO OFF with La Colors Candy Sprinkles on top</t>
+        </is>
+      </c>
+      <c r="C1380" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l2f7o6zbgwve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1381">
+      <c r="A1381" t="inlineStr">
+        <is>
+          <t>1k3c6ei</t>
+        </is>
+      </c>
+      <c r="B1381" t="inlineStr">
+        <is>
+          <t>Oh she definitely glows</t>
+        </is>
+      </c>
+      <c r="C1381" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k3c6ei</t>
+        </is>
+      </c>
+    </row>
+    <row r="1382">
+      <c r="A1382" t="inlineStr">
+        <is>
+          <t>1k3bzvm</t>
+        </is>
+      </c>
+      <c r="B1382" t="inlineStr">
+        <is>
+          <t>Has anyone heard of the brand Conatsu?</t>
+        </is>
+      </c>
+      <c r="C1382" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1902u1nlcwve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1383">
+      <c r="A1383" t="inlineStr">
+        <is>
+          <t>1k3bhce</t>
+        </is>
+      </c>
+      <c r="B1383" t="inlineStr">
+        <is>
+          <t>regular polish + gel polish</t>
+        </is>
+      </c>
+      <c r="C1383" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k3bhce/regular_polish_gel_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1384">
+      <c r="A1384" t="inlineStr">
+        <is>
+          <t>1k3ay27</t>
+        </is>
+      </c>
+      <c r="B1384" t="inlineStr">
+        <is>
+          <t>Lurid - light breaks on the horizon</t>
+        </is>
+      </c>
+      <c r="C1384" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k3ay27/lurid_light_breaks_on_the_horizon/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1385">
+      <c r="A1385" t="inlineStr">
+        <is>
+          <t>1k3aova</t>
+        </is>
+      </c>
+      <c r="B1385" t="inlineStr">
+        <is>
+          <t>Any ways to dye nails at home?</t>
+        </is>
+      </c>
+      <c r="C1385" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k3aova/any_ways_to_dye_nails_at_home/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1386">
+      <c r="A1386" t="inlineStr">
+        <is>
+          <t>1k3airx</t>
+        </is>
+      </c>
+      <c r="B1386" t="inlineStr">
+        <is>
+          <t>Help find this color in gel</t>
+        </is>
+      </c>
+      <c r="C1386" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i5w28tdyxvve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1387">
+      <c r="A1387" t="inlineStr">
+        <is>
+          <t>1k3ahgx</t>
+        </is>
+      </c>
+      <c r="B1387" t="inlineStr">
+        <is>
+          <t>Can you make indentations in your gel polish?</t>
+        </is>
+      </c>
+      <c r="C1387" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k3ahgx/can_you_make_indentations_in_your_gel_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1388">
+      <c r="A1388" t="inlineStr">
+        <is>
+          <t>1k3a2ov</t>
+        </is>
+      </c>
+      <c r="B1388" t="inlineStr">
+        <is>
+          <t>Easter Egg Chaos Skittle</t>
+        </is>
+      </c>
+      <c r="C1388" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k3a2ov</t>
+        </is>
+      </c>
+    </row>
+    <row r="1389">
+      <c r="A1389" t="inlineStr">
+        <is>
+          <t>1k39zyj</t>
+        </is>
+      </c>
+      <c r="B1389" t="inlineStr">
+        <is>
+          <t>First Lurid order. So excited</t>
+        </is>
+      </c>
+      <c r="C1389" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sl7nh8lusvve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1390">
+      <c r="A1390" t="inlineStr">
+        <is>
+          <t>1k39yim</t>
+        </is>
+      </c>
+      <c r="B1390" t="inlineStr">
+        <is>
+          <t>Hard to photograph but I'm loving this subtle yet flashy flake for Easter</t>
+        </is>
+      </c>
+      <c r="C1390" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k39yim</t>
+        </is>
+      </c>
+    </row>
+    <row r="1391">
+      <c r="A1391" t="inlineStr">
+        <is>
+          <t>1k39v15</t>
+        </is>
+      </c>
+      <c r="B1391" t="inlineStr">
+        <is>
+          <t>I’m beautiful. I’m mad. It’s showtime.</t>
+        </is>
+      </c>
+      <c r="C1391" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k39v15</t>
+        </is>
+      </c>
+    </row>
+    <row r="1392">
+      <c r="A1392" t="inlineStr">
+        <is>
+          <t>1k39up9</t>
+        </is>
+      </c>
+      <c r="B1392" t="inlineStr">
+        <is>
+          <t>LA Colors:  Spirit of the Sea ($1.25)</t>
+        </is>
+      </c>
+      <c r="C1392" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6f443ugarvve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1393">
+      <c r="A1393" t="inlineStr">
+        <is>
+          <t>1k39gda</t>
+        </is>
+      </c>
+      <c r="B1393" t="inlineStr">
+        <is>
+          <t>She’s Everything♥️💖💙</t>
+        </is>
+      </c>
+      <c r="C1393" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k39gda</t>
+        </is>
+      </c>
+    </row>
+    <row r="1394">
+      <c r="A1394" t="inlineStr">
+        <is>
+          <t>1k39bqz</t>
+        </is>
+      </c>
+      <c r="B1394" t="inlineStr">
+        <is>
+          <t>Matching with nature</t>
+        </is>
+      </c>
+      <c r="C1394" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zisf3q3omvve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1395">
+      <c r="A1395" t="inlineStr">
+        <is>
+          <t>1k3971j</t>
+        </is>
+      </c>
+      <c r="B1395" t="inlineStr">
+        <is>
+          <t>i’ve wanted tibberz!!! for a while but i can’t justify the cost after shipping etc for just one polish. are there any similar dupes that aren’t $14? 😭</t>
+        </is>
+      </c>
+      <c r="C1395" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6locxyrhlvve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1396">
+      <c r="A1396" t="inlineStr">
+        <is>
+          <t>1k392az</t>
+        </is>
+      </c>
+      <c r="B1396" t="inlineStr">
+        <is>
+          <t>I'm a hobbyist, so they are never perfect but I was proud of this set for Easter ☺️</t>
+        </is>
+      </c>
+      <c r="C1396" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k392az</t>
+        </is>
+      </c>
+    </row>
+    <row r="1397">
+      <c r="A1397" t="inlineStr">
+        <is>
+          <t>1k38i3f</t>
+        </is>
+      </c>
+      <c r="B1397" t="inlineStr">
+        <is>
+          <t>Barely-there nude recommendations</t>
+        </is>
+      </c>
+      <c r="C1397" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zoctmshbfvve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1398">
+      <c r="A1398" t="inlineStr">
+        <is>
+          <t>1k38ggb</t>
+        </is>
+      </c>
+      <c r="B1398" t="inlineStr">
+        <is>
+          <t>The cool tone red of my dreams 🍎</t>
+        </is>
+      </c>
+      <c r="C1398" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k38ggb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1399">
+      <c r="A1399" t="inlineStr">
+        <is>
+          <t>1k38fsv</t>
+        </is>
+      </c>
+      <c r="B1399" t="inlineStr">
+        <is>
+          <t>Shrink days later</t>
+        </is>
+      </c>
+      <c r="C1399" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/axpfn2gqevve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1400">
+      <c r="A1400" t="inlineStr">
+        <is>
+          <t>1k3807z</t>
+        </is>
+      </c>
+      <c r="B1400" t="inlineStr">
+        <is>
+          <t>Not my usual color preference. A friend suggested I try brighter colors for Spring.</t>
+        </is>
+      </c>
+      <c r="C1400" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3b38u1zwavve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1401">
+      <c r="A1401" t="inlineStr">
+        <is>
+          <t>1k37zzf</t>
+        </is>
+      </c>
+      <c r="B1401" t="inlineStr">
+        <is>
+          <t>TONITE: A Goofy Movie</t>
+        </is>
+      </c>
+      <c r="C1401" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ucn6vy59avve1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1402">
+      <c r="A1402" t="inlineStr">
+        <is>
+          <t>1k36hq4</t>
+        </is>
+      </c>
+      <c r="B1402" t="inlineStr">
+        <is>
+          <t>Mouse Ballerina 🐭</t>
+        </is>
+      </c>
+      <c r="C1402" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k36hq4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1403">
+      <c r="A1403" t="inlineStr">
+        <is>
+          <t>1k36zgw</t>
+        </is>
+      </c>
+      <c r="B1403" t="inlineStr">
+        <is>
+          <t>Dream lacquer</t>
+        </is>
+      </c>
+      <c r="C1403" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k36zgw/dream_lacquer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1404">
+      <c r="A1404" t="inlineStr">
+        <is>
+          <t>1k37od0</t>
+        </is>
+      </c>
+      <c r="B1404" t="inlineStr">
+        <is>
+          <t>Touch Grass, yo!</t>
+        </is>
+      </c>
+      <c r="C1404" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g39n5qwz7vve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1405">
+      <c r="A1405" t="inlineStr">
+        <is>
+          <t>1k378nv</t>
+        </is>
+      </c>
+      <c r="B1405" t="inlineStr">
+        <is>
+          <t>Are any of these old polishes worth keeping?</t>
+        </is>
+      </c>
+      <c r="C1405" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/74bro2x74vve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1406">
+      <c r="A1406" t="inlineStr">
+        <is>
+          <t>1k377u7</t>
+        </is>
+      </c>
+      <c r="B1406" t="inlineStr">
+        <is>
+          <t>My roommate said it looked like I fisted shrek and it was “giving kidney failure”</t>
+        </is>
+      </c>
+      <c r="C1406" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qi9eorm04vve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1407">
+      <c r="A1407" t="inlineStr">
+        <is>
+          <t>1k3771t</t>
+        </is>
+      </c>
+      <c r="B1407" t="inlineStr">
+        <is>
+          <t>Memories unlocked</t>
+        </is>
+      </c>
+      <c r="C1407" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l2009iiq3vve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1408">
+      <c r="A1408" t="inlineStr">
+        <is>
+          <t>1k372jj</t>
+        </is>
+      </c>
+      <c r="B1408" t="inlineStr">
+        <is>
+          <t>Need help choosing a nice shimmery in-your-face red</t>
+        </is>
+      </c>
+      <c r="C1408" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k372jj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1409">
+      <c r="A1409" t="inlineStr">
+        <is>
+          <t>1k36yh6</t>
+        </is>
+      </c>
+      <c r="B1409" t="inlineStr">
+        <is>
+          <t>Help comparing a few polishes</t>
+        </is>
+      </c>
+      <c r="C1409" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k36yh6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1410">
+      <c r="A1410" t="inlineStr">
+        <is>
+          <t>1k36tb3</t>
+        </is>
+      </c>
+      <c r="B1410" t="inlineStr">
+        <is>
+          <t>emotional support polish!</t>
+        </is>
+      </c>
+      <c r="C1410" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k36tb3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1411">
+      <c r="A1411" t="inlineStr">
+        <is>
+          <t>1k36q1z</t>
+        </is>
+      </c>
+      <c r="B1411" t="inlineStr">
+        <is>
+          <t>Pure platinum ✨</t>
+        </is>
+      </c>
+      <c r="C1411" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k36q1z</t>
+        </is>
+      </c>
+    </row>
+    <row r="1412">
+      <c r="A1412" t="inlineStr">
+        <is>
+          <t>1k36k93</t>
+        </is>
+      </c>
+      <c r="B1412" t="inlineStr">
+        <is>
+          <t>I've reached the Zenith!</t>
+        </is>
+      </c>
+      <c r="C1412" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/md4zu4ufyuve1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1413">
+      <c r="A1413" t="inlineStr">
+        <is>
+          <t>1k36fb8</t>
+        </is>
+      </c>
+      <c r="B1413" t="inlineStr">
+        <is>
+          <t>Max 2 day mani Lacqueristas, I think I've solved it!</t>
+        </is>
+      </c>
+      <c r="C1413" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k36fb8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1414">
+      <c r="A1414" t="inlineStr">
+        <is>
+          <t>1k368wl</t>
+        </is>
+      </c>
+      <c r="B1414" t="inlineStr">
+        <is>
+          <t>Trying to convince myself to like pastels + a Mooncat polish I don't like</t>
+        </is>
+      </c>
+      <c r="C1414" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k368wl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1415">
+      <c r="A1415" t="inlineStr">
+        <is>
+          <t>1k367ux</t>
+        </is>
+      </c>
+      <c r="B1415" t="inlineStr">
+        <is>
+          <t>Jewel of the Ball is impossible to photograph</t>
+        </is>
+      </c>
+      <c r="C1415" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k367ux</t>
+        </is>
+      </c>
+    </row>
+    <row r="1416">
+      <c r="A1416" t="inlineStr">
+        <is>
+          <t>1k367r4</t>
+        </is>
+      </c>
+      <c r="B1416" t="inlineStr">
+        <is>
+          <t>Tips</t>
+        </is>
+      </c>
+      <c r="C1416" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k367r4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1417">
+      <c r="A1417" t="inlineStr">
+        <is>
+          <t>1k35siz</t>
+        </is>
+      </c>
+      <c r="B1417" t="inlineStr">
+        <is>
+          <t>Marshmallow Lake yumminess</t>
+        </is>
+      </c>
+      <c r="C1417" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8c658jqzruve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1418">
+      <c r="A1418" t="inlineStr">
+        <is>
+          <t>1k34ufs</t>
+        </is>
+      </c>
+      <c r="B1418" t="inlineStr">
+        <is>
+          <t>Posting for the topcoat</t>
+        </is>
+      </c>
+      <c r="C1418" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k34ufs</t>
+        </is>
+      </c>
+    </row>
+    <row r="1419">
+      <c r="A1419" t="inlineStr">
+        <is>
+          <t>1k34si8</t>
+        </is>
+      </c>
+      <c r="B1419" t="inlineStr">
+        <is>
+          <t>Let's talk polish descriptions.</t>
+        </is>
+      </c>
+      <c r="C1419" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k34si8/lets_talk_polish_descriptions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1420">
+      <c r="A1420" t="inlineStr">
+        <is>
+          <t>1k34jql</t>
+        </is>
+      </c>
+      <c r="B1420" t="inlineStr">
+        <is>
+          <t>Water based plus durable topcoat cheat?</t>
+        </is>
+      </c>
+      <c r="C1420" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/df0ld3tjhuve1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1421">
+      <c r="A1421" t="inlineStr">
+        <is>
+          <t>1k34h2d</t>
+        </is>
+      </c>
+      <c r="B1421" t="inlineStr">
+        <is>
+          <t>Looking for polish shade similar to Tyla’s Coachella nails</t>
+        </is>
+      </c>
+      <c r="C1421" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k34h2d</t>
+        </is>
+      </c>
+    </row>
+    <row r="1422">
+      <c r="A1422" t="inlineStr">
+        <is>
+          <t>1k34gc3</t>
+        </is>
+      </c>
+      <c r="B1422" t="inlineStr">
+        <is>
+          <t>Name a more perfect Easter polish</t>
+        </is>
+      </c>
+      <c r="C1422" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/mgb2fp8lguve1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1423">
+      <c r="A1423" t="inlineStr">
+        <is>
+          <t>1k349dw</t>
+        </is>
+      </c>
+      <c r="B1423" t="inlineStr">
+        <is>
+          <t>Clionadh and Dogs</t>
+        </is>
+      </c>
+      <c r="C1423" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k349dw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1424">
+      <c r="A1424" t="inlineStr">
+        <is>
+          <t>1k32y3l</t>
+        </is>
+      </c>
+      <c r="B1424" t="inlineStr">
+        <is>
+          <t>Hoppy Easter</t>
+        </is>
+      </c>
+      <c r="C1424" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k32y3l</t>
+        </is>
+      </c>
+    </row>
+    <row r="1425">
+      <c r="A1425" t="inlineStr">
+        <is>
+          <t>1k32mla</t>
+        </is>
+      </c>
+      <c r="B1425" t="inlineStr">
+        <is>
+          <t>These are my “I wish that I could be on vacation at the beach right now” nails 🏝️</t>
+        </is>
+      </c>
+      <c r="C1425" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f76lylra2uve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1426">
+      <c r="A1426" t="inlineStr">
+        <is>
+          <t>1k32a5a</t>
+        </is>
+      </c>
+      <c r="B1426" t="inlineStr">
+        <is>
+          <t>Who doesn’t love a good accidental color match?</t>
+        </is>
+      </c>
+      <c r="C1426" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bdf0bt1mztve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1427">
+      <c r="A1427" t="inlineStr">
+        <is>
+          <t>1k3244d</t>
+        </is>
+      </c>
+      <c r="B1427" t="inlineStr">
+        <is>
+          <t>At this point, my friend is curating my collection.</t>
+        </is>
+      </c>
+      <c r="C1427" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3i1t93ebytve1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1428">
+      <c r="A1428" t="inlineStr">
+        <is>
+          <t>1k31zeg</t>
+        </is>
+      </c>
+      <c r="B1428" t="inlineStr">
+        <is>
+          <t>In my 🌟glowy🌟 era pt 2</t>
+        </is>
+      </c>
+      <c r="C1428" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k31zeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1429">
+      <c r="A1429" t="inlineStr">
+        <is>
+          <t>1k31u99</t>
+        </is>
+      </c>
+      <c r="B1429" t="inlineStr">
+        <is>
+          <t>dreamy combo 🌸🦋</t>
+        </is>
+      </c>
+      <c r="C1429" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k31u99</t>
+        </is>
+      </c>
+    </row>
+    <row r="1430">
+      <c r="A1430" t="inlineStr">
+        <is>
+          <t>1k31dms</t>
+        </is>
+      </c>
+      <c r="B1430" t="inlineStr">
+        <is>
+          <t>What is wrong with my polish? Not enough thinner? Too little? Does my application just suck?</t>
+        </is>
+      </c>
+      <c r="C1430" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k31dms</t>
+        </is>
+      </c>
+    </row>
+    <row r="1431">
+      <c r="A1431" t="inlineStr">
+        <is>
+          <t>1k3144s</t>
+        </is>
+      </c>
+      <c r="B1431" t="inlineStr">
+        <is>
+          <t>Cadillacquer - In Disguise</t>
+        </is>
+      </c>
+      <c r="C1431" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k3144s</t>
+        </is>
+      </c>
+    </row>
+    <row r="1432">
+      <c r="A1432" t="inlineStr">
+        <is>
+          <t>1k30ycj</t>
+        </is>
+      </c>
+      <c r="B1432" t="inlineStr">
+        <is>
+          <t>Cut or Patch 😰</t>
+        </is>
+      </c>
+      <c r="C1432" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k30ycj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1433">
+      <c r="A1433" t="inlineStr">
+        <is>
+          <t>1k30f65</t>
+        </is>
+      </c>
+      <c r="B1433" t="inlineStr">
+        <is>
+          <t>Where can I buy UNT Ready for Take Off?</t>
+        </is>
+      </c>
+      <c r="C1433" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k30f65/where_can_i_buy_unt_ready_for_take_off/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1434">
+      <c r="A1434" t="inlineStr">
+        <is>
+          <t>1k2zzcb</t>
+        </is>
+      </c>
+      <c r="B1434" t="inlineStr">
+        <is>
+          <t>ILNP Glowstick (unmagnetized)</t>
+        </is>
+      </c>
+      <c r="C1434" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pytouxidhtve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1435">
+      <c r="A1435" t="inlineStr">
+        <is>
+          <t>1k2ztm2</t>
+        </is>
+      </c>
+      <c r="B1435" t="inlineStr">
+        <is>
+          <t>🖤First ombre attempt💚</t>
+        </is>
+      </c>
+      <c r="C1435" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k2ztm2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1436">
+      <c r="A1436" t="inlineStr">
+        <is>
+          <t>1k2ztfp</t>
+        </is>
+      </c>
+      <c r="B1436" t="inlineStr">
+        <is>
+          <t>Two weeks of wear with Phoenix Rainbow Fluorite 🤯</t>
+        </is>
+      </c>
+      <c r="C1436" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mkchjmy2gtve1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1437">
+      <c r="A1437" t="inlineStr">
+        <is>
+          <t>1k2z4ml</t>
+        </is>
+      </c>
+      <c r="B1437" t="inlineStr">
+        <is>
+          <t>California Raisins</t>
+        </is>
+      </c>
+      <c r="C1437" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k2z4ml</t>
+        </is>
+      </c>
+    </row>
+    <row r="1438">
+      <c r="A1438" t="inlineStr">
+        <is>
+          <t>1k2ymxm</t>
+        </is>
+      </c>
+      <c r="B1438" t="inlineStr">
+        <is>
+          <t>Impulse buy win</t>
+        </is>
+      </c>
+      <c r="C1438" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/le69xews6tve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1439">
+      <c r="A1439" t="inlineStr">
+        <is>
+          <t>1k2ye8i</t>
+        </is>
+      </c>
+      <c r="B1439" t="inlineStr">
+        <is>
+          <t>A fall look in spring</t>
+        </is>
+      </c>
+      <c r="C1439" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k2ye8i</t>
+        </is>
+      </c>
+    </row>
+    <row r="1440">
+      <c r="A1440" t="inlineStr">
+        <is>
+          <t>1k2y9ez</t>
+        </is>
+      </c>
+      <c r="B1440" t="inlineStr">
+        <is>
+          <t>Poems for a Harvest Moon dupe?</t>
+        </is>
+      </c>
+      <c r="C1440" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tkiykmdw3tve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1441">
+      <c r="A1441" t="inlineStr">
+        <is>
+          <t>1k2x4l7</t>
+        </is>
+      </c>
+      <c r="B1441" t="inlineStr">
+        <is>
+          <t>Y'all ARE the problem!</t>
+        </is>
+      </c>
+      <c r="C1441" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2z52dqwiusve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1442">
+      <c r="A1442" t="inlineStr">
+        <is>
+          <t>1k2x21s</t>
+        </is>
+      </c>
+      <c r="B1442" t="inlineStr">
+        <is>
+          <t>So perfect for spring</t>
+        </is>
+      </c>
+      <c r="C1442" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pjsr3joftsve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1443">
+      <c r="A1443" t="inlineStr">
+        <is>
+          <t>1k2wb47</t>
+        </is>
+      </c>
+      <c r="B1443" t="inlineStr">
+        <is>
+          <t>Just for fun flowers</t>
+        </is>
+      </c>
+      <c r="C1443" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k2wb47</t>
+        </is>
+      </c>
+    </row>
+    <row r="1444">
+      <c r="A1444" t="inlineStr">
+        <is>
+          <t>1k2vot9</t>
+        </is>
+      </c>
+      <c r="B1444" t="inlineStr">
+        <is>
+          <t>🩷💛Easter Stripes💚💙</t>
+        </is>
+      </c>
+      <c r="C1444" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k2vot9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1445">
+      <c r="A1445" t="inlineStr">
+        <is>
+          <t>1k2vm5f</t>
+        </is>
+      </c>
+      <c r="B1445" t="inlineStr">
+        <is>
+          <t>Gingham Bows</t>
+        </is>
+      </c>
+      <c r="C1445" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k2vm5f</t>
+        </is>
+      </c>
+    </row>
+    <row r="1446">
+      <c r="A1446" t="inlineStr">
+        <is>
+          <t>1k2veti</t>
+        </is>
+      </c>
+      <c r="B1446" t="inlineStr">
+        <is>
+          <t>Recently used a maniology stamping kit. Why did certain polishes fail epically?</t>
+        </is>
+      </c>
+      <c r="C1446" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dfgxmo0wesve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1447">
+      <c r="A1447" t="inlineStr">
+        <is>
+          <t>1k2vcc2</t>
+        </is>
+      </c>
+      <c r="B1447" t="inlineStr">
+        <is>
+          <t>Magnetic polish application tips?</t>
+        </is>
+      </c>
+      <c r="C1447" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k2vcc2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1448">
+      <c r="A1448" t="inlineStr">
+        <is>
+          <t>1k2vayb</t>
+        </is>
+      </c>
+      <c r="B1448" t="inlineStr">
+        <is>
+          <t>Socialite, how much do I love thee? Let me count the ways...</t>
+        </is>
+      </c>
+      <c r="C1448" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9d1oefbudsve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1449">
+      <c r="A1449" t="inlineStr">
+        <is>
+          <t>1k2v20t</t>
+        </is>
+      </c>
+      <c r="B1449" t="inlineStr">
+        <is>
+          <t>Death Valley Nails new “Kerosene” show off</t>
+        </is>
+      </c>
+      <c r="C1449" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/qx4saywcbsve1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1450">
+      <c r="A1450" t="inlineStr">
+        <is>
+          <t>1k2uq81</t>
+        </is>
+      </c>
+      <c r="B1450" t="inlineStr">
+        <is>
+          <t>Cuticula subscription</t>
+        </is>
+      </c>
+      <c r="C1450" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1k2uq81/cuticula_subscription/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1451">
+      <c r="A1451" t="inlineStr">
+        <is>
+          <t>1k2tg9p</t>
+        </is>
+      </c>
+      <c r="B1451" t="inlineStr">
+        <is>
+          <t>Ultrahot💖💛</t>
+        </is>
+      </c>
+      <c r="C1451" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k2tg9p</t>
+        </is>
+      </c>
+    </row>
+    <row r="1452">
+      <c r="A1452" t="inlineStr">
+        <is>
+          <t>1k2sx9x</t>
+        </is>
+      </c>
+      <c r="B1452" t="inlineStr">
+        <is>
+          <t>ILNP - Deep Space</t>
+        </is>
+      </c>
+      <c r="C1452" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k2sx9x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1453">
+      <c r="A1453" t="inlineStr">
+        <is>
+          <t>1k3g7pv</t>
+        </is>
+      </c>
+      <c r="B1453" t="inlineStr">
+        <is>
+          <t>Cruella Deville vibes</t>
+        </is>
+      </c>
+      <c r="C1453" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r1q4hwncnxve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1454">
+      <c r="A1454" t="inlineStr">
+        <is>
+          <t>1k3fulw</t>
+        </is>
+      </c>
+      <c r="B1454" t="inlineStr">
+        <is>
+          <t>My first ombré (with chrome)... I welcome any and all criticism! :)</t>
+        </is>
+      </c>
+      <c r="C1454" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k3fulw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1455">
+      <c r="A1455" t="inlineStr">
+        <is>
+          <t>1k36v7n</t>
+        </is>
+      </c>
+      <c r="B1455" t="inlineStr">
+        <is>
+          <t>What colour would have been better?</t>
+        </is>
+      </c>
+      <c r="C1455" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n97oyc501vve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1456">
+      <c r="A1456" t="inlineStr">
+        <is>
+          <t>1k37lkk</t>
+        </is>
+      </c>
+      <c r="B1456" t="inlineStr">
+        <is>
+          <t>last summer nails, is this still a thing?</t>
+        </is>
+      </c>
+      <c r="C1456" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e2wk0eja7vve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1457">
+      <c r="A1457" t="inlineStr">
+        <is>
+          <t>1k37imk</t>
+        </is>
+      </c>
+      <c r="B1457" t="inlineStr">
+        <is>
+          <t>use this image to design nails?</t>
+        </is>
+      </c>
+      <c r="C1457" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k4x6e4ik6vve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1458">
+      <c r="A1458" t="inlineStr">
+        <is>
+          <t>1k36zh0</t>
+        </is>
+      </c>
+      <c r="B1458" t="inlineStr">
+        <is>
+          <t>Nail art for first time</t>
+        </is>
+      </c>
+      <c r="C1458" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k36zh0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1459">
+      <c r="A1459" t="inlineStr">
+        <is>
+          <t>1k36vix</t>
+        </is>
+      </c>
+      <c r="B1459" t="inlineStr">
+        <is>
+          <t>Formula 1 set ✨🏁</t>
+        </is>
+      </c>
+      <c r="C1459" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a9xo43q21vve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1460">
+      <c r="A1460" t="inlineStr">
+        <is>
+          <t>1k364jp</t>
+        </is>
+      </c>
+      <c r="B1460" t="inlineStr">
+        <is>
+          <t>Blue and gold</t>
+        </is>
+      </c>
+      <c r="C1460" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k364jp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1461">
+      <c r="A1461" t="inlineStr">
+        <is>
+          <t>1k35xow</t>
+        </is>
+      </c>
+      <c r="B1461" t="inlineStr">
+        <is>
+          <t>Magical fairy pond, made this for fun!</t>
+        </is>
+      </c>
+      <c r="C1461" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pt9vsf46tuve1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1462">
+      <c r="A1462" t="inlineStr">
+        <is>
+          <t>1k33gz1</t>
+        </is>
+      </c>
+      <c r="B1462" t="inlineStr">
+        <is>
+          <t>Easter nails for my teen</t>
+        </is>
+      </c>
+      <c r="C1462" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k33gz1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1463">
+      <c r="A1463" t="inlineStr">
+        <is>
+          <t>1k337ec</t>
+        </is>
+      </c>
+      <c r="B1463" t="inlineStr">
+        <is>
+          <t>For my customers, I made this nail design.</t>
+        </is>
+      </c>
+      <c r="C1463" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k337ec</t>
+        </is>
+      </c>
+    </row>
+    <row r="1464">
+      <c r="A1464" t="inlineStr">
+        <is>
+          <t>1k32xyj</t>
+        </is>
+      </c>
+      <c r="B1464" t="inlineStr">
+        <is>
+          <t>4:20 Nails 💚</t>
+        </is>
+      </c>
+      <c r="C1464" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k32xyj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1465">
+      <c r="A1465" t="inlineStr">
+        <is>
+          <t>1k32wur</t>
+        </is>
+      </c>
+      <c r="B1465" t="inlineStr">
+        <is>
+          <t>Hoppy Easter!</t>
+        </is>
+      </c>
+      <c r="C1465" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k32wur</t>
+        </is>
+      </c>
+    </row>
+    <row r="1466">
+      <c r="A1466" t="inlineStr">
+        <is>
+          <t>1k32ege</t>
+        </is>
+      </c>
+      <c r="B1466" t="inlineStr">
+        <is>
+          <t>Feeling Funny Bunnies. Hand painting is not my strength but I couldn’t find high bunny decals/stickers.</t>
+        </is>
+      </c>
+      <c r="C1466" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/49mwxpwi0uve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1467">
+      <c r="A1467" t="inlineStr">
+        <is>
+          <t>1k31xll</t>
+        </is>
+      </c>
+      <c r="B1467" t="inlineStr">
+        <is>
+          <t>So tomorrow is 420 and I made NAIIIIILS!!!!</t>
+        </is>
+      </c>
+      <c r="C1467" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k31xll</t>
+        </is>
+      </c>
+    </row>
+    <row r="1468">
+      <c r="A1468" t="inlineStr">
+        <is>
+          <t>1k30na0</t>
+        </is>
+      </c>
+      <c r="B1468" t="inlineStr">
+        <is>
+          <t>Chinese inspired</t>
+        </is>
+      </c>
+      <c r="C1468" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jfgm7phqmtve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1469">
+      <c r="A1469" t="inlineStr">
+        <is>
+          <t>1k30fnf</t>
+        </is>
+      </c>
+      <c r="B1469" t="inlineStr">
+        <is>
+          <t>Happy Easter</t>
+        </is>
+      </c>
+      <c r="C1469" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k30fnf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1470">
+      <c r="A1470" t="inlineStr">
+        <is>
+          <t>1k2zhdm</t>
+        </is>
+      </c>
+      <c r="B1470" t="inlineStr">
+        <is>
+          <t>Easter nails 😊</t>
+        </is>
+      </c>
+      <c r="C1470" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d3xnod0hdtve1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1471">
+      <c r="A1471" t="inlineStr">
+        <is>
+          <t>1k2yl12</t>
+        </is>
+      </c>
+      <c r="B1471" t="inlineStr">
+        <is>
+          <t>Nails I did for my first ever cruise 🌊🌊🌊🐙</t>
+        </is>
+      </c>
+      <c r="C1471" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k2yl12</t>
+        </is>
+      </c>
+    </row>
+    <row r="1472">
+      <c r="A1472" t="inlineStr">
+        <is>
+          <t>1k2w6db</t>
+        </is>
+      </c>
+      <c r="B1472" t="inlineStr">
+        <is>
+          <t>Sunflowers &amp; Ladybugs</t>
+        </is>
+      </c>
+      <c r="C1472" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6b3ictg5msve1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1473">
+      <c r="A1473" t="inlineStr">
+        <is>
+          <t>1k2v1g2</t>
+        </is>
+      </c>
+      <c r="B1473" t="inlineStr">
+        <is>
+          <t>Nail sets</t>
+        </is>
+      </c>
+      <c r="C1473" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1k2v1g2</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>